<commit_message>
Bookmarking mostly works in image module, DT language selection sorted.
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2D8A3C8-DA6B-4EAE-860D-0B2A5636A27C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D6B42A-5058-4124-B5D5-E791E687F2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12195" yWindow="2100" windowWidth="17250" windowHeight="9945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="169">
   <si>
     <t>id</t>
   </si>
@@ -452,6 +452,81 @@
   </si>
   <si>
     <t>Date/temps</t>
+  </si>
+  <si>
+    <t>DT internationalization</t>
+  </si>
+  <si>
+    <t>tbl_info</t>
+  </si>
+  <si>
+    <t>tbl_prev</t>
+  </si>
+  <si>
+    <t>Previous</t>
+  </si>
+  <si>
+    <t>tbl_search</t>
+  </si>
+  <si>
+    <t>Search:</t>
+  </si>
+  <si>
+    <t>Recherche</t>
+  </si>
+  <si>
+    <t>tbl_next</t>
+  </si>
+  <si>
+    <t>Next</t>
+  </si>
+  <si>
+    <t>Prochain</t>
+  </si>
+  <si>
+    <t>Précédent</t>
+  </si>
+  <si>
+    <t>tbl_length</t>
+  </si>
+  <si>
+    <t>Montrer _MENU_ éléments</t>
+  </si>
+  <si>
+    <t>tbl_filtered</t>
+  </si>
+  <si>
+    <t>(filtrées de _MAX_ éléments)</t>
+  </si>
+  <si>
+    <t>tbl_zero</t>
+  </si>
+  <si>
+    <t>No matching records found</t>
+  </si>
+  <si>
+    <t>Aucunes données existantes</t>
+  </si>
+  <si>
+    <t>tbl_info_empty</t>
+  </si>
+  <si>
+    <t>_TOTAL_ éléments au total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> _TOTAL_ records total</t>
+  </si>
+  <si>
+    <t>No records to show!</t>
+  </si>
+  <si>
+    <t>(filtered from _MAX_ records)</t>
+  </si>
+  <si>
+    <t>Show _MENU_ records</t>
+  </si>
+  <si>
+    <t>Rien à voir ici!</t>
   </si>
 </sst>
 </file>
@@ -1368,10 +1443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D48" sqref="D48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1964,52 +2039,164 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="A47" t="s">
+        <v>145</v>
+      </c>
+      <c r="B47" t="s">
+        <v>144</v>
+      </c>
+      <c r="C47" t="s">
+        <v>164</v>
+      </c>
+      <c r="D47" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="B48" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="C48" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="D48" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="B49" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="C49" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="D49" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>151</v>
+      </c>
+      <c r="B50" t="s">
+        <v>144</v>
+      </c>
+      <c r="C50" t="s">
+        <v>152</v>
+      </c>
+      <c r="D50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>148</v>
+      </c>
+      <c r="B51" t="s">
+        <v>144</v>
+      </c>
+      <c r="C51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>155</v>
+      </c>
+      <c r="B52" t="s">
+        <v>144</v>
+      </c>
+      <c r="C52" t="s">
+        <v>167</v>
+      </c>
+      <c r="D52" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" t="s">
+        <v>144</v>
+      </c>
+      <c r="C53" t="s">
+        <v>166</v>
+      </c>
+      <c r="D53" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>159</v>
+      </c>
+      <c r="B54" t="s">
+        <v>144</v>
+      </c>
+      <c r="C54" t="s">
+        <v>160</v>
+      </c>
+      <c r="D54" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" t="s">
+        <v>90</v>
+      </c>
+      <c r="C56" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+      <c r="C57" t="s">
+        <v>71</v>
+      </c>
+      <c r="D57" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>95</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B58" t="s">
         <v>90</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C58" t="s">
         <v>96</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D58" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Addition of "about" tab to the app with content.
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D6B42A-5058-4124-B5D5-E791E687F2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C7C8A5-311E-4590-AD72-EC402D20EABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12195" yWindow="2100" windowWidth="17250" windowHeight="9945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="193">
   <si>
     <t>id</t>
   </si>
@@ -527,13 +527,85 @@
   </si>
   <si>
     <t>Rien à voir ici!</t>
+  </si>
+  <si>
+    <t>About view module</t>
+  </si>
+  <si>
+    <t>about_view_title</t>
+  </si>
+  <si>
+    <t>About</t>
+  </si>
+  <si>
+    <t>À propos</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>About us</t>
+  </si>
+  <si>
+    <t>À propos de nous</t>
+  </si>
+  <si>
+    <t>about_title1</t>
+  </si>
+  <si>
+    <t>About this web site</t>
+  </si>
+  <si>
+    <t>À propos de ce site web</t>
+  </si>
+  <si>
+    <t>about_content1</t>
+  </si>
+  <si>
+    <t>content</t>
+  </si>
+  <si>
+    <t>about_content2</t>
+  </si>
+  <si>
+    <t>about_url</t>
+  </si>
+  <si>
+    <t>about_content3</t>
+  </si>
+  <si>
+    <t>url</t>
+  </si>
+  <si>
+    <t xml:space="preserve">. </t>
+  </si>
+  <si>
+    <t>https://github.com/YukonWRB/YGwater</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>about_title2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ce site web a été conçu en utilisant R Shiny, ce qui nous permet de tirer parti de l'aptitude inhérente du langage de programmation R pour la manipulation de données et la création de graphiques. Le code de l'application est contenu dans un package R qui comprend de nombreuses fonctions utiles et intéressantes en plus de celles présentées dans cette application, et est publiquement consultable à </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This web site was created using R Shiny, which allows us to leverage the R programming language's inherent suitability for data wrangling and plotting. The application code is contained within an R package which which holds many useful and interesting functions besides those showcased in this application, and is publicly viewable at </t>
+  </si>
+  <si>
+    <t>Content to be developed!</t>
+  </si>
+  <si>
+    <t>À développer!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -668,6 +740,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="41">
     <fill>
@@ -1014,7 +1094,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1057,8 +1137,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1068,8 +1149,9 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1103,6 +1185,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -1443,10 +1526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1840,363 +1923,477 @@
         <v>124</v>
       </c>
     </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+    </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>49</v>
+      </c>
+      <c r="C32" t="s">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="A33" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>170</v>
+      </c>
+      <c r="B34" t="s">
         <v>49</v>
       </c>
-      <c r="C33" t="s">
-        <v>60</v>
-      </c>
-      <c r="D33" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="C34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D34" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>62</v>
+        <v>176</v>
       </c>
       <c r="B35" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="C35" t="s">
-        <v>63</v>
+        <v>174</v>
       </c>
       <c r="D35" t="s">
-        <v>64</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>125</v>
+        <v>179</v>
       </c>
       <c r="B36" t="s">
-        <v>9</v>
+        <v>180</v>
       </c>
       <c r="C36" t="s">
-        <v>126</v>
+        <v>191</v>
       </c>
       <c r="D36" t="s">
-        <v>127</v>
+        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>65</v>
+        <v>188</v>
       </c>
       <c r="B37" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="C37" t="s">
-        <v>66</v>
+        <v>177</v>
       </c>
       <c r="D37" t="s">
-        <v>67</v>
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>181</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>180</v>
       </c>
       <c r="C38" t="s">
-        <v>69</v>
+        <v>190</v>
       </c>
       <c r="D38" t="s">
-        <v>70</v>
+        <v>189</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>182</v>
       </c>
       <c r="B39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" t="s">
-        <v>73</v>
+        <v>184</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>186</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>74</v>
+        <v>183</v>
       </c>
       <c r="B40" t="s">
-        <v>9</v>
+        <v>180</v>
       </c>
       <c r="C40" t="s">
-        <v>75</v>
+        <v>185</v>
       </c>
       <c r="D40" t="s">
-        <v>76</v>
+        <v>187</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>77</v>
-      </c>
-      <c r="B41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" t="s">
-        <v>78</v>
-      </c>
-      <c r="D41" t="s">
-        <v>79</v>
-      </c>
+      <c r="A41" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="D43" t="s">
-        <v>88</v>
+        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="D44" t="s">
-        <v>11</v>
+        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>141</v>
+        <v>68</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>142</v>
+        <v>69</v>
       </c>
       <c r="D45" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>15</v>
+        <v>71</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>16</v>
+        <v>72</v>
       </c>
       <c r="D46" t="s">
-        <v>17</v>
+        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>145</v>
+        <v>74</v>
       </c>
       <c r="B47" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>164</v>
+        <v>75</v>
       </c>
       <c r="D47" t="s">
-        <v>163</v>
+        <v>76</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>162</v>
+        <v>77</v>
       </c>
       <c r="B48" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>165</v>
+        <v>78</v>
       </c>
       <c r="D48" t="s">
-        <v>168</v>
+        <v>79</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="B49" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
       <c r="D49" t="s">
-        <v>154</v>
+        <v>82</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>151</v>
+        <v>86</v>
       </c>
       <c r="B50" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>152</v>
+        <v>87</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>88</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>148</v>
+        <v>8</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>149</v>
+        <v>10</v>
       </c>
       <c r="D51" t="s">
-        <v>150</v>
+        <v>11</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B52" t="s">
-        <v>144</v>
+        <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>167</v>
+        <v>142</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>157</v>
+        <v>15</v>
       </c>
       <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>16</v>
+      </c>
+      <c r="D53" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C53" t="s">
-        <v>166</v>
-      </c>
-      <c r="D53" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>159</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>145</v>
+      </c>
+      <c r="B55" t="s">
         <v>144</v>
       </c>
-      <c r="C54" t="s">
-        <v>160</v>
-      </c>
-      <c r="D54" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
+      <c r="C55" t="s">
+        <v>164</v>
+      </c>
+      <c r="D55" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>89</v>
+        <v>162</v>
       </c>
       <c r="B56" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="C56" t="s">
-        <v>91</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
-        <v>92</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>93</v>
+        <v>146</v>
       </c>
       <c r="B57" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
       <c r="C57" t="s">
-        <v>71</v>
+        <v>147</v>
       </c>
       <c r="D57" t="s">
-        <v>94</v>
+        <v>154</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
+        <v>151</v>
+      </c>
+      <c r="B58" t="s">
+        <v>144</v>
+      </c>
+      <c r="C58" t="s">
+        <v>152</v>
+      </c>
+      <c r="D58" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>148</v>
+      </c>
+      <c r="B59" t="s">
+        <v>144</v>
+      </c>
+      <c r="C59" t="s">
+        <v>149</v>
+      </c>
+      <c r="D59" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>155</v>
+      </c>
+      <c r="B60" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" t="s">
+        <v>167</v>
+      </c>
+      <c r="D60" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>157</v>
+      </c>
+      <c r="B61" t="s">
+        <v>144</v>
+      </c>
+      <c r="C61" t="s">
+        <v>166</v>
+      </c>
+      <c r="D61" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>159</v>
+      </c>
+      <c r="B62" t="s">
+        <v>144</v>
+      </c>
+      <c r="C62" t="s">
+        <v>160</v>
+      </c>
+      <c r="D62" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B63" s="4"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>89</v>
+      </c>
+      <c r="B64" t="s">
+        <v>90</v>
+      </c>
+      <c r="C64" t="s">
+        <v>91</v>
+      </c>
+      <c r="D64" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>93</v>
+      </c>
+      <c r="B65" t="s">
+        <v>90</v>
+      </c>
+      <c r="C65" t="s">
+        <v>71</v>
+      </c>
+      <c r="D65" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>95</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B66" t="s">
         <v>90</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C66" t="s">
         <v>96</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D66" t="s">
         <v>97</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Row selection no longer re-renders the table, keyboard arrows can navigate images.
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5C7C8A5-311E-4590-AD72-EC402D20EABF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7494A5A-FDA7-437D-BD32-CDC069F119E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="199">
   <si>
     <t>id</t>
   </si>
@@ -148,9 +148,6 @@
     <t>pop-up error message title</t>
   </si>
   <si>
-    <t>Our appologies!</t>
-  </si>
-  <si>
     <t>Désolé!</t>
   </si>
   <si>
@@ -599,6 +596,27 @@
   </si>
   <si>
     <t>À développer!</t>
+  </si>
+  <si>
+    <t>Our apologies!</t>
+  </si>
+  <si>
+    <t>param_group_col</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>group_fr</t>
+  </si>
+  <si>
+    <t>param_group</t>
+  </si>
+  <si>
+    <t>Parameter Group</t>
+  </si>
+  <si>
+    <t>Groupe de paramètre</t>
   </si>
 </sst>
 </file>
@@ -1526,10 +1544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1569,21 +1587,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s">
         <v>102</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>103</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>104</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1689,7 +1707,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1703,29 +1721,29 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
+        <v>192</v>
+      </c>
+      <c r="D13" t="s">
         <v>42</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>45</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>46</v>
-      </c>
-      <c r="D14" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1733,49 +1751,49 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" t="s">
         <v>48</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>49</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
         <v>84</v>
-      </c>
-      <c r="D17" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B18" t="s">
         <v>106</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>107</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>108</v>
-      </c>
-      <c r="D18" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1783,49 +1801,49 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>51</v>
+      </c>
+      <c r="B20" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" t="s">
         <v>52</v>
       </c>
-      <c r="B20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>53</v>
-      </c>
-      <c r="D20" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" t="s">
         <v>98</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>99</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>100</v>
-      </c>
-      <c r="D21" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" t="s">
         <v>137</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>138</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>139</v>
-      </c>
-      <c r="D22" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
@@ -1833,21 +1851,21 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" t="s">
         <v>55</v>
       </c>
-      <c r="B24" t="s">
-        <v>49</v>
-      </c>
-      <c r="C24" t="s">
-        <v>56</v>
-      </c>
       <c r="D24" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B25" s="6"/>
       <c r="C25" s="6"/>
@@ -1855,77 +1873,77 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" t="s">
         <v>57</v>
       </c>
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" t="s">
-        <v>58</v>
-      </c>
       <c r="D26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>109</v>
+      </c>
+      <c r="B27" t="s">
         <v>110</v>
       </c>
-      <c r="B27" t="s">
-        <v>111</v>
-      </c>
       <c r="C27" t="s">
+        <v>118</v>
+      </c>
+      <c r="D27" t="s">
         <v>119</v>
-      </c>
-      <c r="D27" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>111</v>
+      </c>
+      <c r="B28" t="s">
         <v>112</v>
       </c>
-      <c r="B28" t="s">
-        <v>113</v>
-      </c>
       <c r="C28" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D28" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C29" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D29" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>120</v>
+      </c>
+      <c r="B30" t="s">
         <v>121</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>122</v>
       </c>
-      <c r="C30" t="s">
+      <c r="D30" t="s">
         <v>123</v>
-      </c>
-      <c r="D30" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B31" s="7"/>
       <c r="C31" s="7"/>
@@ -1933,21 +1951,21 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
         <v>59</v>
       </c>
-      <c r="B32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>60</v>
-      </c>
-      <c r="D32" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1955,105 +1973,105 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>169</v>
+      </c>
+      <c r="B34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" t="s">
         <v>170</v>
       </c>
-      <c r="B34" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="D34" t="s">
         <v>171</v>
-      </c>
-      <c r="D34" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B35" t="s">
+        <v>172</v>
+      </c>
+      <c r="C35" t="s">
         <v>173</v>
       </c>
-      <c r="C35" t="s">
+      <c r="D35" t="s">
         <v>174</v>
-      </c>
-      <c r="D35" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>178</v>
+      </c>
+      <c r="B36" t="s">
         <v>179</v>
       </c>
-      <c r="B36" t="s">
-        <v>180</v>
-      </c>
       <c r="C36" t="s">
+        <v>190</v>
+      </c>
+      <c r="D36" t="s">
         <v>191</v>
-      </c>
-      <c r="D36" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C37" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37" t="s">
         <v>177</v>
-      </c>
-      <c r="D37" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B38" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C38" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D38" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B39" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B40" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C40" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D40" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
@@ -2061,231 +2079,231 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B42" t="s">
         <v>9</v>
       </c>
       <c r="C42" t="s">
+        <v>62</v>
+      </c>
+      <c r="D42" t="s">
         <v>63</v>
-      </c>
-      <c r="D42" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B43" t="s">
         <v>9</v>
       </c>
       <c r="C43" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" t="s">
         <v>126</v>
-      </c>
-      <c r="D43" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
+        <v>65</v>
+      </c>
+      <c r="D44" t="s">
         <v>66</v>
-      </c>
-      <c r="D44" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" t="s">
         <v>69</v>
-      </c>
-      <c r="D45" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
+        <v>71</v>
+      </c>
+      <c r="D46" t="s">
         <v>72</v>
-      </c>
-      <c r="D46" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>74</v>
+        <v>196</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>197</v>
       </c>
       <c r="D47" t="s">
-        <v>76</v>
+        <v>198</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D48" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D49" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="D50" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>10</v>
+        <v>86</v>
       </c>
       <c r="D51" t="s">
-        <v>11</v>
+        <v>87</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>141</v>
+        <v>8</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>142</v>
+        <v>10</v>
       </c>
       <c r="D52" t="s">
-        <v>143</v>
+        <v>11</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
       </c>
       <c r="C53" t="s">
+        <v>141</v>
+      </c>
+      <c r="D53" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
         <v>16</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2"/>
-    </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>145</v>
-      </c>
-      <c r="B55" t="s">
-        <v>144</v>
-      </c>
-      <c r="C55" t="s">
-        <v>164</v>
-      </c>
-      <c r="D55" t="s">
-        <v>163</v>
-      </c>
+      <c r="A55" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="B55" s="2"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>144</v>
+      </c>
+      <c r="B56" t="s">
+        <v>143</v>
+      </c>
+      <c r="C56" t="s">
+        <v>163</v>
+      </c>
+      <c r="D56" t="s">
         <v>162</v>
-      </c>
-      <c r="B56" t="s">
-        <v>144</v>
-      </c>
-      <c r="C56" t="s">
-        <v>165</v>
-      </c>
-      <c r="D56" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="B57" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C57" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="D57" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B58" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C58" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D58" t="s">
         <v>153</v>
@@ -2293,108 +2311,136 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B59" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C59" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="D59" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B60" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C60" t="s">
-        <v>167</v>
+        <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B61" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C61" t="s">
         <v>166</v>
       </c>
       <c r="D61" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>156</v>
+      </c>
+      <c r="B62" t="s">
+        <v>143</v>
+      </c>
+      <c r="C62" t="s">
+        <v>165</v>
+      </c>
+      <c r="D62" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>158</v>
+      </c>
+      <c r="B63" t="s">
+        <v>143</v>
+      </c>
+      <c r="C63" t="s">
         <v>159</v>
       </c>
-      <c r="B62" t="s">
-        <v>144</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="D63" t="s">
         <v>160</v>
       </c>
-      <c r="D62" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>89</v>
-      </c>
-      <c r="B64" t="s">
-        <v>90</v>
-      </c>
-      <c r="C64" t="s">
-        <v>91</v>
-      </c>
-      <c r="D64" t="s">
-        <v>92</v>
-      </c>
+      <c r="A64" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64" s="4"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B65" t="s">
+        <v>89</v>
+      </c>
+      <c r="C65" t="s">
         <v>90</v>
       </c>
-      <c r="C65" t="s">
-        <v>71</v>
-      </c>
       <c r="D65" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
+        <v>92</v>
+      </c>
+      <c r="B66" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>193</v>
+      </c>
+      <c r="B67" t="s">
+        <v>89</v>
+      </c>
+      <c r="C67" t="s">
+        <v>194</v>
+      </c>
+      <c r="D67" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>94</v>
+      </c>
+      <c r="B68" t="s">
+        <v>89</v>
+      </c>
+      <c r="C68" t="s">
         <v>95</v>
       </c>
-      <c r="B66" t="s">
-        <v>90</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="D68" t="s">
         <v>96</v>
-      </c>
-      <c r="D66" t="s">
-        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Create login button and modal, improve map popups.
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7494A5A-FDA7-437D-BD32-CDC069F119E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FF119C-269B-44FE-A08E-27C60842920E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="228">
   <si>
     <t>id</t>
   </si>
@@ -617,6 +617,93 @@
   </si>
   <si>
     <t>Groupe de paramètre</t>
+  </si>
+  <si>
+    <t>Parameters</t>
+  </si>
+  <si>
+    <t>Networks</t>
+  </si>
+  <si>
+    <t>Réseaux</t>
+  </si>
+  <si>
+    <t>networks</t>
+  </si>
+  <si>
+    <t>projects</t>
+  </si>
+  <si>
+    <t>parameters</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
+  <si>
+    <t>Projets</t>
+  </si>
+  <si>
+    <t>param_groups</t>
+  </si>
+  <si>
+    <t>Parameter Groups</t>
+  </si>
+  <si>
+    <t>Groupes de paramètres</t>
+  </si>
+  <si>
+    <t>param_types</t>
+  </si>
+  <si>
+    <t>Parameter Types</t>
+  </si>
+  <si>
+    <t>Types de paramètres</t>
+  </si>
+  <si>
+    <t>Parameter Type(s)</t>
+  </si>
+  <si>
+    <t>Type(s) de paramètre(s)</t>
+  </si>
+  <si>
+    <t>param_type(s)</t>
+  </si>
+  <si>
+    <t>parameter(s)</t>
+  </si>
+  <si>
+    <t>Parameter(s)</t>
+  </si>
+  <si>
+    <t>Paramètre(s)</t>
+  </si>
+  <si>
+    <t>project(s)</t>
+  </si>
+  <si>
+    <t>Project(s)</t>
+  </si>
+  <si>
+    <t>Projet(s)</t>
+  </si>
+  <si>
+    <t>param_group(s)</t>
+  </si>
+  <si>
+    <t>Parameter Group(s)</t>
+  </si>
+  <si>
+    <t>Groupe(s) de paramètre(s)</t>
+  </si>
+  <si>
+    <t>network(s)</t>
+  </si>
+  <si>
+    <t>Network(s)</t>
+  </si>
+  <si>
+    <t>Réseau(x)</t>
   </si>
 </sst>
 </file>
@@ -1544,10 +1631,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2149,297 +2236,437 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>196</v>
+        <v>210</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="D47" t="s">
-        <v>198</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>215</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>213</v>
       </c>
       <c r="D48" t="s">
-        <v>75</v>
+        <v>214</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>76</v>
+        <v>196</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>77</v>
+        <v>197</v>
       </c>
       <c r="D49" t="s">
-        <v>78</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>207</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>80</v>
+        <v>208</v>
       </c>
       <c r="D50" t="s">
-        <v>81</v>
+        <v>209</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
+        <v>222</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>86</v>
+        <v>223</v>
       </c>
       <c r="D51" t="s">
-        <v>87</v>
+        <v>224</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="D52" t="s">
-        <v>11</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>140</v>
+        <v>204</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>141</v>
+        <v>199</v>
       </c>
       <c r="D53" t="s">
-        <v>142</v>
+        <v>17</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>15</v>
+        <v>216</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>16</v>
+        <v>217</v>
       </c>
       <c r="D54" t="s">
-        <v>17</v>
+        <v>218</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
+      <c r="A55" t="s">
+        <v>76</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="B56" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>163</v>
+        <v>205</v>
       </c>
       <c r="D56" t="s">
-        <v>162</v>
+        <v>206</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>161</v>
+        <v>219</v>
       </c>
       <c r="B57" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="D57" t="s">
-        <v>167</v>
+        <v>221</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="B58" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
       <c r="D58" t="s">
-        <v>153</v>
+        <v>81</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>150</v>
+        <v>202</v>
       </c>
       <c r="B59" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>151</v>
+        <v>200</v>
       </c>
       <c r="D59" t="s">
-        <v>152</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>147</v>
+        <v>225</v>
       </c>
       <c r="B60" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>148</v>
+        <v>226</v>
       </c>
       <c r="D60" t="s">
-        <v>149</v>
+        <v>227</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>154</v>
+        <v>85</v>
       </c>
       <c r="B61" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>166</v>
+        <v>86</v>
       </c>
       <c r="D61" t="s">
-        <v>155</v>
+        <v>87</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>156</v>
+        <v>8</v>
       </c>
       <c r="B62" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>165</v>
+        <v>10</v>
       </c>
       <c r="D62" t="s">
-        <v>157</v>
+        <v>11</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>141</v>
+      </c>
+      <c r="D63" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>15</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>16</v>
+      </c>
+      <c r="D64" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="C63" t="s">
-        <v>159</v>
-      </c>
-      <c r="D63" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>88</v>
-      </c>
-      <c r="B65" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" t="s">
-        <v>90</v>
-      </c>
-      <c r="D65" t="s">
-        <v>91</v>
-      </c>
+      <c r="B65" s="2"/>
+      <c r="C65" s="2"/>
+      <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>92</v>
+        <v>144</v>
       </c>
       <c r="B66" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="C66" t="s">
-        <v>70</v>
+        <v>163</v>
       </c>
       <c r="D66" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>193</v>
+        <v>161</v>
       </c>
       <c r="B67" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>194</v>
+        <v>164</v>
       </c>
       <c r="D67" t="s">
-        <v>195</v>
+        <v>167</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
+        <v>145</v>
+      </c>
+      <c r="B68" t="s">
+        <v>143</v>
+      </c>
+      <c r="C68" t="s">
+        <v>146</v>
+      </c>
+      <c r="D68" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>150</v>
+      </c>
+      <c r="B69" t="s">
+        <v>143</v>
+      </c>
+      <c r="C69" t="s">
+        <v>151</v>
+      </c>
+      <c r="D69" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>147</v>
+      </c>
+      <c r="B70" t="s">
+        <v>143</v>
+      </c>
+      <c r="C70" t="s">
+        <v>148</v>
+      </c>
+      <c r="D70" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>154</v>
+      </c>
+      <c r="B71" t="s">
+        <v>143</v>
+      </c>
+      <c r="C71" t="s">
+        <v>166</v>
+      </c>
+      <c r="D71" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>156</v>
+      </c>
+      <c r="B72" t="s">
+        <v>143</v>
+      </c>
+      <c r="C72" t="s">
+        <v>165</v>
+      </c>
+      <c r="D72" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>158</v>
+      </c>
+      <c r="B73" t="s">
+        <v>143</v>
+      </c>
+      <c r="C73" t="s">
+        <v>159</v>
+      </c>
+      <c r="D73" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>88</v>
+      </c>
+      <c r="B75" t="s">
+        <v>89</v>
+      </c>
+      <c r="C75" t="s">
+        <v>90</v>
+      </c>
+      <c r="D75" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>92</v>
+      </c>
+      <c r="B76" t="s">
+        <v>89</v>
+      </c>
+      <c r="C76" t="s">
+        <v>70</v>
+      </c>
+      <c r="D76" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>193</v>
+      </c>
+      <c r="B77" t="s">
+        <v>89</v>
+      </c>
+      <c r="C77" t="s">
+        <v>194</v>
+      </c>
+      <c r="D77" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>94</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B78" t="s">
         <v>89</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C78" t="s">
         <v>95</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D78" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Applied data.table to the map module, sorted out how to pass values from module to main server.
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FF119C-269B-44FE-A08E-27C60842920E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006FDBAB-48D9-46A6-B7EA-E7D3F2A117AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="231">
   <si>
     <t>id</t>
   </si>
@@ -704,6 +704,15 @@
   </si>
   <si>
     <t>Réseau(x)</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>direct translations</t>
+  </si>
+  <si>
+    <t>à</t>
   </si>
 </sst>
 </file>
@@ -1631,10 +1640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2460,213 +2469,227 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>140</v>
+        <v>228</v>
       </c>
       <c r="B63" t="s">
-        <v>9</v>
+        <v>229</v>
       </c>
       <c r="C63" t="s">
-        <v>141</v>
+        <v>228</v>
       </c>
       <c r="D63" t="s">
-        <v>142</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>15</v>
+        <v>140</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" t="s">
+        <v>141</v>
+      </c>
+      <c r="D64" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>15</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
         <v>16</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D65" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="2" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="B65" s="2"/>
-      <c r="C65" s="2"/>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>144</v>
-      </c>
-      <c r="B66" t="s">
-        <v>143</v>
-      </c>
-      <c r="C66" t="s">
-        <v>163</v>
-      </c>
-      <c r="D66" t="s">
-        <v>162</v>
-      </c>
+      <c r="B66" s="2"/>
+      <c r="C66" s="2"/>
+      <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="B67" t="s">
         <v>143</v>
       </c>
       <c r="C67" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D67" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>145</v>
+        <v>161</v>
       </c>
       <c r="B68" t="s">
         <v>143</v>
       </c>
       <c r="C68" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="D68" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B69" t="s">
         <v>143</v>
       </c>
       <c r="C69" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="D69" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B70" t="s">
         <v>143</v>
       </c>
       <c r="C70" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D70" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B71" t="s">
         <v>143</v>
       </c>
       <c r="C71" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="D71" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B72" t="s">
         <v>143</v>
       </c>
       <c r="C72" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D72" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B73" t="s">
         <v>143</v>
       </c>
       <c r="C73" t="s">
+        <v>165</v>
+      </c>
+      <c r="D73" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>158</v>
+      </c>
+      <c r="B74" t="s">
+        <v>143</v>
+      </c>
+      <c r="C74" t="s">
         <v>159</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D74" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>88</v>
-      </c>
-      <c r="B75" t="s">
-        <v>89</v>
-      </c>
-      <c r="C75" t="s">
-        <v>90</v>
-      </c>
-      <c r="D75" t="s">
-        <v>91</v>
-      </c>
+      <c r="B75" s="4"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B76" t="s">
         <v>89</v>
       </c>
       <c r="C76" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="D76" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>193</v>
+        <v>92</v>
       </c>
       <c r="B77" t="s">
         <v>89</v>
       </c>
       <c r="C77" t="s">
-        <v>194</v>
+        <v>70</v>
       </c>
       <c r="D77" t="s">
-        <v>195</v>
+        <v>93</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>94</v>
+        <v>193</v>
       </c>
       <c r="B78" t="s">
         <v>89</v>
       </c>
       <c r="C78" t="s">
+        <v>194</v>
+      </c>
+      <c r="D78" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>94</v>
+      </c>
+      <c r="B79" t="s">
+        <v>89</v>
+      </c>
+      <c r="C79" t="s">
         <v>95</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D79" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DB pulls happen in main server, change data.frame syntax to pure data.table, map popups trigger events.
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006FDBAB-48D9-46A6-B7EA-E7D3F2A117AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F4B54-2488-4EDE-97B7-CB4B9275ECBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="247">
   <si>
     <t>id</t>
   </si>
@@ -316,9 +316,6 @@
     <t>dl_data</t>
   </si>
   <si>
-    <t>direct translation for tab panel title</t>
-  </si>
-  <si>
     <t>Download Data</t>
   </si>
   <si>
@@ -337,12 +334,6 @@
     <t>Changer de langue</t>
   </si>
   <si>
-    <t>map_tooltip</t>
-  </si>
-  <si>
-    <t>map filter tooltip</t>
-  </si>
-  <si>
     <t>Filters affect each other by limiting subsequent options. Reset to clear all filters.</t>
   </si>
   <si>
@@ -433,9 +424,6 @@
     <t>date_range_lab</t>
   </si>
   <si>
-    <t>label for date range picker</t>
-  </si>
-  <si>
     <t>Date Range</t>
   </si>
   <si>
@@ -713,6 +701,66 @@
   </si>
   <si>
     <t>à</t>
+  </si>
+  <si>
+    <t>choose_locs</t>
+  </si>
+  <si>
+    <t>Map/data/plot module common</t>
+  </si>
+  <si>
+    <t>tooltip_reset</t>
+  </si>
+  <si>
+    <t>tooltip text for resetting filters</t>
+  </si>
+  <si>
+    <t>download data button</t>
+  </si>
+  <si>
+    <t>year filter title</t>
+  </si>
+  <si>
+    <t>location selection title</t>
+  </si>
+  <si>
+    <t>Or choose one of more locations</t>
+  </si>
+  <si>
+    <t>Ou choisissez une ou plusieures stations</t>
+  </si>
+  <si>
+    <t>Plage de dates</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Groupe</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Unités</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>period</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Catégorie</t>
   </si>
 </sst>
 </file>
@@ -863,7 +911,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1088,6 +1136,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1253,7 +1307,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1264,6 +1318,7 @@
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1640,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,6 +1706,7 @@
     <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="4" max="4" width="70.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1683,21 +1739,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s">
         <v>101</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>102</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>103</v>
-      </c>
-      <c r="D3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1803,7 +1859,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1817,7 +1873,7 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="D13" t="s">
         <v>42</v>
@@ -1839,7 +1895,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1860,150 +1916,144 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>82</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" t="s">
-        <v>83</v>
-      </c>
-      <c r="D17" t="s">
-        <v>84</v>
-      </c>
+      <c r="A17" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C18" t="s">
-        <v>107</v>
+        <v>52</v>
       </c>
       <c r="D18" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="A19" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" t="s">
+        <v>231</v>
+      </c>
+      <c r="C19" t="s">
+        <v>98</v>
+      </c>
+      <c r="D19" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" t="s">
-        <v>52</v>
-      </c>
-      <c r="D20" t="s">
-        <v>53</v>
-      </c>
+      <c r="A20" s="10" t="s">
+        <v>228</v>
+      </c>
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>229</v>
       </c>
       <c r="B21" t="s">
-        <v>98</v>
+        <v>230</v>
       </c>
       <c r="C21" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="D21" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>82</v>
       </c>
       <c r="B22" t="s">
-        <v>137</v>
+        <v>232</v>
       </c>
       <c r="C22" t="s">
-        <v>138</v>
+        <v>83</v>
       </c>
       <c r="D22" t="s">
-        <v>139</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
+      <c r="A23" t="s">
+        <v>227</v>
+      </c>
+      <c r="B23" t="s">
+        <v>233</v>
+      </c>
+      <c r="C23" t="s">
+        <v>234</v>
+      </c>
+      <c r="D23" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="A24" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>54</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>48</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>55</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D25" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6"/>
-    </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B26" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26" t="s">
-        <v>57</v>
-      </c>
+      <c r="A26" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>109</v>
+        <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>110</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="D27" t="s">
-        <v>119</v>
+        <v>57</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C28" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="D28" t="s">
         <v>116</v>
@@ -2011,685 +2061,769 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>108</v>
+      </c>
+      <c r="B29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
         <v>113</v>
-      </c>
-      <c r="B29" t="s">
-        <v>112</v>
-      </c>
-      <c r="C29" t="s">
-        <v>115</v>
-      </c>
-      <c r="D29" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="C30" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="D30" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
+      <c r="A31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B31" t="s">
+        <v>107</v>
+      </c>
+      <c r="C31" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" t="s">
+        <v>236</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="B32" t="s">
-        <v>48</v>
+        <v>118</v>
       </c>
       <c r="C32" t="s">
-        <v>59</v>
+        <v>119</v>
       </c>
       <c r="D32" t="s">
-        <v>60</v>
+        <v>120</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="B33" s="4"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4"/>
+      <c r="A33" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B33" s="7"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="7"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>169</v>
+        <v>58</v>
       </c>
       <c r="B34" t="s">
         <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>170</v>
+        <v>59</v>
       </c>
       <c r="D34" t="s">
-        <v>171</v>
+        <v>60</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>175</v>
-      </c>
-      <c r="B35" t="s">
-        <v>172</v>
-      </c>
-      <c r="C35" t="s">
-        <v>173</v>
-      </c>
-      <c r="D35" t="s">
-        <v>174</v>
-      </c>
+      <c r="A35" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>178</v>
+        <v>165</v>
       </c>
       <c r="B36" t="s">
-        <v>179</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>190</v>
+        <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>191</v>
+        <v>167</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B37" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C37" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D37" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="B38" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C38" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="D38" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B39" t="s">
-        <v>183</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>185</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>185</v>
+        <v>168</v>
+      </c>
+      <c r="C39" t="s">
+        <v>172</v>
+      </c>
+      <c r="D39" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="B40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C40" t="s">
+        <v>185</v>
+      </c>
+      <c r="D40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" t="s">
         <v>179</v>
       </c>
-      <c r="C40" t="s">
-        <v>184</v>
-      </c>
-      <c r="D40" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
+      <c r="C41" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>61</v>
+        <v>178</v>
       </c>
       <c r="B42" t="s">
-        <v>9</v>
+        <v>175</v>
       </c>
       <c r="C42" t="s">
-        <v>62</v>
+        <v>180</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>124</v>
-      </c>
-      <c r="B43" t="s">
-        <v>9</v>
-      </c>
-      <c r="C43" t="s">
-        <v>125</v>
-      </c>
-      <c r="D43" t="s">
-        <v>126</v>
-      </c>
+      <c r="A43" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
         <v>9</v>
       </c>
       <c r="C44" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D44" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>67</v>
+        <v>121</v>
       </c>
       <c r="B45" t="s">
         <v>9</v>
       </c>
       <c r="C45" t="s">
-        <v>68</v>
+        <v>122</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B46" t="s">
         <v>9</v>
       </c>
       <c r="C46" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="D46" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>210</v>
+        <v>67</v>
       </c>
       <c r="B47" t="s">
         <v>9</v>
       </c>
       <c r="C47" t="s">
-        <v>211</v>
+        <v>68</v>
       </c>
       <c r="D47" t="s">
-        <v>212</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>215</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
         <v>9</v>
       </c>
       <c r="C48" t="s">
-        <v>213</v>
+        <v>71</v>
       </c>
       <c r="D48" t="s">
-        <v>214</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>196</v>
+        <v>206</v>
       </c>
       <c r="B49" t="s">
         <v>9</v>
       </c>
       <c r="C49" t="s">
-        <v>197</v>
+        <v>207</v>
       </c>
       <c r="D49" t="s">
-        <v>198</v>
+        <v>208</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="B50" t="s">
         <v>9</v>
       </c>
       <c r="C50" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D50" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>222</v>
+        <v>192</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
       </c>
       <c r="C51" t="s">
-        <v>223</v>
+        <v>193</v>
       </c>
       <c r="D51" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>73</v>
+        <v>203</v>
       </c>
       <c r="B52" t="s">
         <v>9</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>204</v>
       </c>
       <c r="D52" t="s">
-        <v>75</v>
+        <v>205</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>204</v>
+        <v>218</v>
       </c>
       <c r="B53" t="s">
         <v>9</v>
       </c>
       <c r="C53" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>220</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>216</v>
+        <v>190</v>
       </c>
       <c r="B54" t="s">
         <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>217</v>
+        <v>237</v>
       </c>
       <c r="D54" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B55" t="s">
         <v>9</v>
       </c>
       <c r="C55" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="D55" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D56" t="s">
-        <v>206</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="D57" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D58" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="D59" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D60" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D61" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>8</v>
+        <v>198</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>10</v>
+        <v>196</v>
       </c>
       <c r="D62" t="s">
-        <v>11</v>
+        <v>197</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="B63" t="s">
-        <v>229</v>
+        <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="D63" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>140</v>
+        <v>241</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>141</v>
+        <v>239</v>
       </c>
       <c r="D64" t="s">
-        <v>142</v>
+        <v>240</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>15</v>
+        <v>242</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>16</v>
+        <v>243</v>
       </c>
       <c r="D65" t="s">
-        <v>17</v>
+        <v>135</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="B66" s="2"/>
-      <c r="C66" s="2"/>
-      <c r="D66" s="2"/>
+      <c r="A66" t="s">
+        <v>244</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
+        <v>245</v>
+      </c>
+      <c r="D66" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>144</v>
+        <v>85</v>
       </c>
       <c r="B67" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>86</v>
       </c>
       <c r="D67" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>161</v>
+        <v>8</v>
       </c>
       <c r="B68" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="D68" t="s">
-        <v>167</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>145</v>
+        <v>224</v>
       </c>
       <c r="B69" t="s">
-        <v>143</v>
+        <v>225</v>
       </c>
       <c r="C69" t="s">
-        <v>146</v>
+        <v>224</v>
       </c>
       <c r="D69" t="s">
-        <v>153</v>
+        <v>226</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="B70" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="D70" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>147</v>
+        <v>15</v>
       </c>
       <c r="B71" t="s">
-        <v>143</v>
+        <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>148</v>
+        <v>16</v>
       </c>
       <c r="D71" t="s">
-        <v>149</v>
+        <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>154</v>
-      </c>
-      <c r="B72" t="s">
-        <v>143</v>
-      </c>
-      <c r="C72" t="s">
-        <v>166</v>
-      </c>
-      <c r="D72" t="s">
-        <v>155</v>
-      </c>
+      <c r="A72" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B72" s="2"/>
+      <c r="C72" s="2"/>
+      <c r="D72" s="2"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="B73" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C73" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D73" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B74" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C74" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="D74" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
+      <c r="A75" t="s">
+        <v>141</v>
+      </c>
+      <c r="B75" t="s">
+        <v>139</v>
+      </c>
+      <c r="C75" t="s">
+        <v>142</v>
+      </c>
+      <c r="D75" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>88</v>
+        <v>146</v>
       </c>
       <c r="B76" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="C76" t="s">
-        <v>90</v>
+        <v>147</v>
       </c>
       <c r="D76" t="s">
-        <v>91</v>
+        <v>148</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="B77" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="C77" t="s">
-        <v>70</v>
+        <v>144</v>
       </c>
       <c r="D77" t="s">
-        <v>93</v>
+        <v>145</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>193</v>
+        <v>150</v>
       </c>
       <c r="B78" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="C78" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="D78" t="s">
-        <v>195</v>
+        <v>151</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>152</v>
+      </c>
+      <c r="B79" t="s">
+        <v>139</v>
+      </c>
+      <c r="C79" t="s">
+        <v>161</v>
+      </c>
+      <c r="D79" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>154</v>
+      </c>
+      <c r="B80" t="s">
+        <v>139</v>
+      </c>
+      <c r="C80" t="s">
+        <v>155</v>
+      </c>
+      <c r="D80" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" s="4"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>88</v>
+      </c>
+      <c r="B82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82" t="s">
+        <v>90</v>
+      </c>
+      <c r="D82" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>92</v>
+      </c>
+      <c r="B83" t="s">
+        <v>89</v>
+      </c>
+      <c r="C83" t="s">
+        <v>70</v>
+      </c>
+      <c r="D83" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>189</v>
+      </c>
+      <c r="B84" t="s">
+        <v>89</v>
+      </c>
+      <c r="C84" t="s">
+        <v>190</v>
+      </c>
+      <c r="D84" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>94</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B85" t="s">
         <v>89</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C85" t="s">
         <v>95</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D85" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Table renders for data tab!!!
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53F4B54-2488-4EDE-97B7-CB4B9275ECBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFEBDCA-C3C2-4542-A4C9-520C1CEB9AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="258">
   <si>
     <t>id</t>
   </si>
@@ -761,6 +761,39 @@
   </si>
   <si>
     <t>Catégorie</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>de</t>
+  </si>
+  <si>
+    <t>from_utc_offset</t>
+  </si>
+  <si>
+    <t>to_utc_offset</t>
+  </si>
+  <si>
+    <t>From (UTC-7)</t>
+  </si>
+  <si>
+    <t>De (UTC-7)</t>
+  </si>
+  <si>
+    <t>To (UTC-7)</t>
+  </si>
+  <si>
+    <t>À (UTC-7)</t>
+  </si>
+  <si>
+    <t>datetime_utc_offset</t>
+  </si>
+  <si>
+    <t>Date/Time (UTC-7)</t>
+  </si>
+  <si>
+    <t>Date/temps (UTC-7)</t>
   </si>
 </sst>
 </file>
@@ -1695,10 +1728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D85"/>
+  <dimension ref="A1:D89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="A65" sqref="A65:XFD65"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +1739,8 @@
     <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="43.5703125" customWidth="1"/>
-    <col min="4" max="4" width="70.140625" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="5" max="5" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -2603,227 +2637,283 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="B69" t="s">
-        <v>225</v>
+        <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>224</v>
+        <v>247</v>
       </c>
       <c r="D69" t="s">
-        <v>226</v>
+        <v>248</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>136</v>
+        <v>224</v>
       </c>
       <c r="B70" t="s">
-        <v>9</v>
+        <v>225</v>
       </c>
       <c r="C70" t="s">
-        <v>137</v>
+        <v>224</v>
       </c>
       <c r="D70" t="s">
-        <v>138</v>
+        <v>226</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>15</v>
+        <v>249</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>16</v>
+        <v>251</v>
       </c>
       <c r="D71" t="s">
-        <v>17</v>
+        <v>252</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B72" s="2"/>
-      <c r="C72" s="2"/>
-      <c r="D72" s="2"/>
+      <c r="A72" t="s">
+        <v>250</v>
+      </c>
+      <c r="B72" t="s">
+        <v>225</v>
+      </c>
+      <c r="C72" t="s">
+        <v>253</v>
+      </c>
+      <c r="D72" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="B73" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="D73" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>157</v>
+        <v>255</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>160</v>
+        <v>256</v>
       </c>
       <c r="D74" t="s">
-        <v>163</v>
+        <v>257</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>141</v>
+        <v>15</v>
       </c>
       <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
+        <v>16</v>
+      </c>
+      <c r="D75" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C75" t="s">
-        <v>142</v>
-      </c>
-      <c r="D75" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>146</v>
-      </c>
-      <c r="B76" t="s">
-        <v>139</v>
-      </c>
-      <c r="C76" t="s">
-        <v>147</v>
-      </c>
-      <c r="D76" t="s">
-        <v>148</v>
-      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B77" t="s">
         <v>139</v>
       </c>
       <c r="C77" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="D77" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B78" t="s">
         <v>139</v>
       </c>
       <c r="C78" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D78" t="s">
-        <v>151</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>152</v>
+        <v>141</v>
       </c>
       <c r="B79" t="s">
         <v>139</v>
       </c>
       <c r="C79" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="D79" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="B80" t="s">
         <v>139</v>
       </c>
       <c r="C80" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
+      <c r="A81" t="s">
+        <v>143</v>
+      </c>
+      <c r="B81" t="s">
+        <v>139</v>
+      </c>
+      <c r="C81" t="s">
+        <v>144</v>
+      </c>
+      <c r="D81" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>88</v>
+        <v>150</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="C82" t="s">
-        <v>90</v>
+        <v>162</v>
       </c>
       <c r="D82" t="s">
-        <v>91</v>
+        <v>151</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>92</v>
+        <v>152</v>
       </c>
       <c r="B83" t="s">
-        <v>89</v>
+        <v>139</v>
       </c>
       <c r="C83" t="s">
-        <v>70</v>
+        <v>161</v>
       </c>
       <c r="D83" t="s">
-        <v>93</v>
+        <v>153</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" t="s">
+        <v>139</v>
+      </c>
+      <c r="C84" t="s">
+        <v>155</v>
+      </c>
+      <c r="D84" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="4"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>88</v>
+      </c>
+      <c r="B86" t="s">
+        <v>89</v>
+      </c>
+      <c r="C86" t="s">
+        <v>90</v>
+      </c>
+      <c r="D86" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>92</v>
+      </c>
+      <c r="B87" t="s">
+        <v>89</v>
+      </c>
+      <c r="C87" t="s">
+        <v>70</v>
+      </c>
+      <c r="D87" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
         <v>189</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B88" t="s">
         <v>89</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C88" t="s">
         <v>190</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D88" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
         <v>94</v>
       </c>
-      <c r="B85" t="s">
+      <c r="B89" t="s">
         <v>89</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C89" t="s">
         <v>95</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D89" t="s">
         <v>96</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added tooltips to the data table headers
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AFEBDCA-C3C2-4542-A4C9-520C1CEB9AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FEB587-94D1-4297-A5BF-54C990B48D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="279">
   <si>
     <t>id</t>
   </si>
@@ -229,9 +229,6 @@
     <t>Discrete</t>
   </si>
   <si>
-    <t>Discrets</t>
-  </si>
-  <si>
     <t>param_type</t>
   </si>
   <si>
@@ -794,6 +791,72 @@
   </si>
   <si>
     <t>Date/temps (UTC-7)</t>
+  </si>
+  <si>
+    <t>start_utc_offset</t>
+  </si>
+  <si>
+    <t>end_utc_offset</t>
+  </si>
+  <si>
+    <t>Start (UTC-7)</t>
+  </si>
+  <si>
+    <t>End (UTC-7)</t>
+  </si>
+  <si>
+    <t>Début (UTC-7)</t>
+  </si>
+  <si>
+    <t>Fin (UTC-7)</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>tooltip1</t>
+  </si>
+  <si>
+    <t>table tool tips</t>
+  </si>
+  <si>
+    <t>tooltip2</t>
+  </si>
+  <si>
+    <t>UTC-7 or Mountain Standard Time</t>
+  </si>
+  <si>
+    <t>Discrètes</t>
+  </si>
+  <si>
+    <t>UTC-7 ou Heure Normalle des Rocheuses</t>
+  </si>
+  <si>
+    <t>Continuous = recorded at regular intervals automatically; Discrete =  measurements or sample acquisition at variable time intervals.</t>
+  </si>
+  <si>
+    <t>Continues = enregistré à intervalles réguliers automatiquement ; Discrètes = mesures  ou acquisition d'échantillons à  intervalles de temps variables.</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Début</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>end</t>
   </si>
 </sst>
 </file>
@@ -1728,22 +1791,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D89"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="D74" sqref="D74"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" customWidth="1"/>
-    <col min="5" max="5" width="54.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" customWidth="1"/>
+    <col min="4" max="4" width="49.88671875" customWidth="1"/>
+    <col min="5" max="5" width="54.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1757,7 +1820,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1771,29 +1834,29 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B3" t="s">
         <v>100</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>101</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>102</v>
       </c>
-      <c r="D3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1807,7 +1870,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1821,7 +1884,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1835,7 +1898,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1849,7 +1912,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1863,7 +1926,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1877,7 +1940,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1891,15 +1954,15 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1907,13 +1970,13 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D13" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1927,15 +1990,15 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -1949,15 +2012,15 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1971,531 +2034,528 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" t="s">
         <v>97</v>
       </c>
-      <c r="B19" t="s">
-        <v>231</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>98</v>
       </c>
-      <c r="D19" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>228</v>
+      </c>
+      <c r="B21" t="s">
         <v>229</v>
       </c>
-      <c r="B21" t="s">
-        <v>230</v>
-      </c>
       <c r="C21" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" t="s">
         <v>104</v>
       </c>
-      <c r="D21" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>231</v>
+      </c>
+      <c r="C22" t="s">
         <v>82</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>226</v>
+      </c>
+      <c r="B23" t="s">
         <v>232</v>
       </c>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>227</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>233</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>234</v>
       </c>
-      <c r="D23" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>265</v>
+      </c>
+      <c r="B24" t="s">
+        <v>266</v>
+      </c>
+      <c r="C24" t="s">
+        <v>271</v>
+      </c>
+      <c r="D24" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>267</v>
+      </c>
+      <c r="C25" t="s">
+        <v>268</v>
+      </c>
+      <c r="D25" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
         <v>54</v>
-      </c>
-      <c r="B25" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" t="s">
-        <v>55</v>
-      </c>
-      <c r="D25" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>56</v>
       </c>
       <c r="B27" t="s">
         <v>48</v>
       </c>
       <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" t="s">
         <v>57</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>105</v>
+      </c>
+      <c r="B30" t="s">
         <v>106</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C30" t="s">
+        <v>114</v>
+      </c>
+      <c r="D30" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
         <v>107</v>
       </c>
-      <c r="C28" t="s">
-        <v>115</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>109</v>
+      </c>
+      <c r="B32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>132</v>
+      </c>
+      <c r="B33" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" t="s">
+        <v>133</v>
+      </c>
+      <c r="D33" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>108</v>
-      </c>
-      <c r="B29" t="s">
-        <v>109</v>
-      </c>
-      <c r="C29" t="s">
-        <v>111</v>
-      </c>
-      <c r="D29" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>110</v>
-      </c>
-      <c r="B30" t="s">
-        <v>109</v>
-      </c>
-      <c r="C30" t="s">
-        <v>112</v>
-      </c>
-      <c r="D30" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>133</v>
-      </c>
-      <c r="B31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C31" t="s">
-        <v>134</v>
-      </c>
-      <c r="D31" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+      <c r="B34" t="s">
         <v>117</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C34" t="s">
         <v>118</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D34" t="s">
         <v>119</v>
       </c>
-      <c r="D32" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="7" t="s">
-        <v>129</v>
-      </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="7"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>58</v>
-      </c>
-      <c r="B34" t="s">
-        <v>48</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>165</v>
       </c>
       <c r="B36" t="s">
         <v>48</v>
       </c>
       <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>164</v>
+      </c>
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" t="s">
+        <v>165</v>
+      </c>
+      <c r="D38" t="s">
         <v>166</v>
       </c>
-      <c r="D36" t="s">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>170</v>
+      </c>
+      <c r="B39" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>171</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C39" t="s">
         <v>168</v>
       </c>
-      <c r="C37" t="s">
+      <c r="D39" t="s">
         <v>169</v>
       </c>
-      <c r="D37" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>173</v>
+      </c>
+      <c r="B40" t="s">
         <v>174</v>
-      </c>
-      <c r="B38" t="s">
-        <v>175</v>
-      </c>
-      <c r="C38" t="s">
-        <v>186</v>
-      </c>
-      <c r="D38" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>183</v>
-      </c>
-      <c r="B39" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" t="s">
-        <v>172</v>
-      </c>
-      <c r="D39" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>176</v>
-      </c>
-      <c r="B40" t="s">
-        <v>175</v>
       </c>
       <c r="C40" t="s">
         <v>185</v>
       </c>
       <c r="D40" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>182</v>
+      </c>
+      <c r="B41" t="s">
+        <v>167</v>
+      </c>
+      <c r="C41" t="s">
+        <v>171</v>
+      </c>
+      <c r="D41" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>175</v>
+      </c>
+      <c r="B42" t="s">
+        <v>174</v>
+      </c>
+      <c r="C42" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="D42" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>176</v>
+      </c>
+      <c r="B43" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>177</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
+        <v>174</v>
+      </c>
+      <c r="C44" t="s">
         <v>179</v>
       </c>
-      <c r="C41" s="9" t="s">
+      <c r="D44" t="s">
         <v>181</v>
       </c>
-      <c r="D41" s="9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>178</v>
-      </c>
-      <c r="B42" t="s">
-        <v>175</v>
-      </c>
-      <c r="C42" t="s">
-        <v>180</v>
-      </c>
-      <c r="D42" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="8" t="s">
-        <v>130</v>
-      </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>61</v>
       </c>
-      <c r="B44" t="s">
-        <v>9</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
         <v>62</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D46" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>120</v>
+      </c>
+      <c r="B47" t="s">
+        <v>9</v>
+      </c>
+      <c r="C47" t="s">
         <v>121</v>
       </c>
-      <c r="B45" t="s">
-        <v>9</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D47" t="s">
         <v>122</v>
       </c>
-      <c r="D45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>64</v>
       </c>
-      <c r="B46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B48" t="s">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
         <v>65</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D48" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>67</v>
       </c>
-      <c r="B47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
         <v>68</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D49" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>263</v>
+      </c>
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
+        <v>264</v>
+      </c>
+      <c r="D50" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
         <v>70</v>
       </c>
-      <c r="B48" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="D51" t="s">
         <v>71</v>
       </c>
-      <c r="D48" t="s">
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>205</v>
+      </c>
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
+        <v>206</v>
+      </c>
+      <c r="D52" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>210</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
+        <v>208</v>
+      </c>
+      <c r="D53" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>191</v>
+      </c>
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
+        <v>192</v>
+      </c>
+      <c r="D54" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>202</v>
+      </c>
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
+        <v>203</v>
+      </c>
+      <c r="D55" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>217</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D56" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
+        <v>236</v>
+      </c>
+      <c r="D57" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>206</v>
-      </c>
-      <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" t="s">
-        <v>207</v>
-      </c>
-      <c r="D49" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>211</v>
-      </c>
-      <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" t="s">
-        <v>209</v>
-      </c>
-      <c r="D50" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>192</v>
-      </c>
-      <c r="B51" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" t="s">
-        <v>193</v>
-      </c>
-      <c r="D51" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>203</v>
-      </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
-        <v>204</v>
-      </c>
-      <c r="D52" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>218</v>
-      </c>
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" t="s">
-        <v>219</v>
-      </c>
-      <c r="D53" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>190</v>
-      </c>
-      <c r="B54" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" t="s">
-        <v>237</v>
-      </c>
-      <c r="D54" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
         <v>73</v>
       </c>
-      <c r="B55" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="D58" t="s">
         <v>74</v>
       </c>
-      <c r="D55" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>200</v>
-      </c>
-      <c r="B56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" t="s">
-        <v>195</v>
-      </c>
-      <c r="D56" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>212</v>
-      </c>
-      <c r="B57" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" t="s">
-        <v>213</v>
-      </c>
-      <c r="D57" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>76</v>
-      </c>
-      <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
-        <v>77</v>
-      </c>
-      <c r="D58" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>199</v>
       </c>
@@ -2503,41 +2563,41 @@
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="D59" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="D60" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="D61" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>198</v>
       </c>
@@ -2545,376 +2605,474 @@
         <v>9</v>
       </c>
       <c r="C62" t="s">
+        <v>200</v>
+      </c>
+      <c r="D62" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>214</v>
+      </c>
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
+        <v>215</v>
+      </c>
+      <c r="D63" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>78</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
+        <v>79</v>
+      </c>
+      <c r="D64" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>197</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
+        <v>195</v>
+      </c>
+      <c r="D65" t="s">
         <v>196</v>
       </c>
-      <c r="D62" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>220</v>
+      </c>
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
         <v>221</v>
       </c>
-      <c r="B63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="D66" t="s">
         <v>222</v>
       </c>
-      <c r="D63" t="s">
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>240</v>
+      </c>
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
+        <v>238</v>
+      </c>
+      <c r="D67" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>241</v>
+      </c>
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>242</v>
+      </c>
+      <c r="D68" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>243</v>
+      </c>
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
+        <v>244</v>
+      </c>
+      <c r="D69" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>84</v>
+      </c>
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
+        <v>85</v>
+      </c>
+      <c r="D70" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>8</v>
+      </c>
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
+        <v>10</v>
+      </c>
+      <c r="D71" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>246</v>
+      </c>
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
+        <v>246</v>
+      </c>
+      <c r="D72" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>241</v>
-      </c>
-      <c r="B64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" t="s">
-        <v>239</v>
-      </c>
-      <c r="D64" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>242</v>
-      </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" t="s">
-        <v>243</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="B73" t="s">
+        <v>224</v>
+      </c>
+      <c r="C73" t="s">
+        <v>223</v>
+      </c>
+      <c r="D73" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>248</v>
+      </c>
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
+        <v>250</v>
+      </c>
+      <c r="D74" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>249</v>
+      </c>
+      <c r="B75" t="s">
+        <v>224</v>
+      </c>
+      <c r="C75" t="s">
+        <v>252</v>
+      </c>
+      <c r="D75" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>277</v>
+      </c>
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
+        <v>273</v>
+      </c>
+      <c r="D76" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>278</v>
+      </c>
+      <c r="B77" t="s">
+        <v>224</v>
+      </c>
+      <c r="C77" t="s">
+        <v>274</v>
+      </c>
+      <c r="D77" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>257</v>
+      </c>
+      <c r="B78" t="s">
+        <v>9</v>
+      </c>
+      <c r="C78" t="s">
+        <v>259</v>
+      </c>
+      <c r="D78" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>258</v>
+      </c>
+      <c r="B79" t="s">
+        <v>224</v>
+      </c>
+      <c r="C79" t="s">
+        <v>260</v>
+      </c>
+      <c r="D79" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>244</v>
-      </c>
-      <c r="B66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" t="s">
-        <v>245</v>
-      </c>
-      <c r="D66" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>85</v>
-      </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" t="s">
-        <v>86</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="B80" t="s">
+        <v>9</v>
+      </c>
+      <c r="C80" t="s">
+        <v>136</v>
+      </c>
+      <c r="D80" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>254</v>
+      </c>
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
+        <v>255</v>
+      </c>
+      <c r="D81" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>15</v>
+      </c>
+      <c r="B82" t="s">
+        <v>9</v>
+      </c>
+      <c r="C82" t="s">
+        <v>16</v>
+      </c>
+      <c r="D82" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B83" s="2"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>139</v>
+      </c>
+      <c r="B84" t="s">
+        <v>138</v>
+      </c>
+      <c r="C84" t="s">
+        <v>158</v>
+      </c>
+      <c r="D84" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>156</v>
+      </c>
+      <c r="B85" t="s">
+        <v>138</v>
+      </c>
+      <c r="C85" t="s">
+        <v>159</v>
+      </c>
+      <c r="D85" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>140</v>
+      </c>
+      <c r="B86" t="s">
+        <v>138</v>
+      </c>
+      <c r="C86" t="s">
+        <v>141</v>
+      </c>
+      <c r="D86" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>145</v>
+      </c>
+      <c r="B87" t="s">
+        <v>138</v>
+      </c>
+      <c r="C87" t="s">
+        <v>146</v>
+      </c>
+      <c r="D87" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>142</v>
+      </c>
+      <c r="B88" t="s">
+        <v>138</v>
+      </c>
+      <c r="C88" t="s">
+        <v>143</v>
+      </c>
+      <c r="D88" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>149</v>
+      </c>
+      <c r="B89" t="s">
+        <v>138</v>
+      </c>
+      <c r="C89" t="s">
+        <v>161</v>
+      </c>
+      <c r="D89" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>151</v>
+      </c>
+      <c r="B90" t="s">
+        <v>138</v>
+      </c>
+      <c r="C90" t="s">
+        <v>160</v>
+      </c>
+      <c r="D90" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>153</v>
+      </c>
+      <c r="B91" t="s">
+        <v>138</v>
+      </c>
+      <c r="C91" t="s">
+        <v>154</v>
+      </c>
+      <c r="D91" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B92" s="4"/>
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>8</v>
-      </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" t="s">
-        <v>10</v>
-      </c>
-      <c r="D68" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>247</v>
-      </c>
-      <c r="B69" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69" t="s">
-        <v>247</v>
-      </c>
-      <c r="D69" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>224</v>
-      </c>
-      <c r="B70" t="s">
-        <v>225</v>
-      </c>
-      <c r="C70" t="s">
-        <v>224</v>
-      </c>
-      <c r="D70" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>249</v>
-      </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" t="s">
-        <v>251</v>
-      </c>
-      <c r="D71" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>250</v>
-      </c>
-      <c r="B72" t="s">
-        <v>225</v>
-      </c>
-      <c r="C72" t="s">
-        <v>253</v>
-      </c>
-      <c r="D72" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>136</v>
-      </c>
-      <c r="B73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" t="s">
-        <v>137</v>
-      </c>
-      <c r="D73" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>255</v>
-      </c>
-      <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" t="s">
-        <v>256</v>
-      </c>
-      <c r="D74" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>15</v>
-      </c>
-      <c r="B75" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" t="s">
-        <v>16</v>
-      </c>
-      <c r="D75" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="B76" s="2"/>
-      <c r="C76" s="2"/>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>140</v>
-      </c>
-      <c r="B77" t="s">
-        <v>139</v>
-      </c>
-      <c r="C77" t="s">
-        <v>159</v>
-      </c>
-      <c r="D77" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>157</v>
-      </c>
-      <c r="B78" t="s">
-        <v>139</v>
-      </c>
-      <c r="C78" t="s">
-        <v>160</v>
-      </c>
-      <c r="D78" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>141</v>
-      </c>
-      <c r="B79" t="s">
-        <v>139</v>
-      </c>
-      <c r="C79" t="s">
-        <v>142</v>
-      </c>
-      <c r="D79" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>146</v>
-      </c>
-      <c r="B80" t="s">
-        <v>139</v>
-      </c>
-      <c r="C80" t="s">
-        <v>147</v>
-      </c>
-      <c r="D80" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>143</v>
-      </c>
-      <c r="B81" t="s">
-        <v>139</v>
-      </c>
-      <c r="C81" t="s">
-        <v>144</v>
-      </c>
-      <c r="D81" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>150</v>
-      </c>
-      <c r="B82" t="s">
-        <v>139</v>
-      </c>
-      <c r="C82" t="s">
-        <v>162</v>
-      </c>
-      <c r="D82" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>152</v>
-      </c>
-      <c r="B83" t="s">
-        <v>139</v>
-      </c>
-      <c r="C83" t="s">
-        <v>161</v>
-      </c>
-      <c r="D83" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>154</v>
-      </c>
-      <c r="B84" t="s">
-        <v>139</v>
-      </c>
-      <c r="C84" t="s">
-        <v>155</v>
-      </c>
-      <c r="D84" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="B93" t="s">
         <v>88</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C93" t="s">
         <v>89</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D93" t="s">
         <v>90</v>
       </c>
-      <c r="D86" t="s">
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="B94" t="s">
+        <v>88</v>
+      </c>
+      <c r="C94" t="s">
+        <v>69</v>
+      </c>
+      <c r="D94" t="s">
         <v>92</v>
       </c>
-      <c r="B87" t="s">
-        <v>89</v>
-      </c>
-      <c r="C87" t="s">
-        <v>70</v>
-      </c>
-      <c r="D87" t="s">
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" t="s">
+        <v>88</v>
+      </c>
+      <c r="C95" t="s">
+        <v>189</v>
+      </c>
+      <c r="D95" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>189</v>
-      </c>
-      <c r="B88" t="s">
-        <v>89</v>
-      </c>
-      <c r="C88" t="s">
-        <v>190</v>
-      </c>
-      <c r="D88" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+      <c r="B96" t="s">
+        <v>88</v>
+      </c>
+      <c r="C96" t="s">
         <v>94</v>
       </c>
-      <c r="B89" t="s">
-        <v>89</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="D96" t="s">
         <v>95</v>
-      </c>
-      <c r="D89" t="s">
-        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gradually working on transitioning functions to use database spatial files; updates to Shiny app data module.
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8FEB587-94D1-4297-A5BF-54C990B48D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B15484-B128-4A02-8A8A-B51EDC1A42FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="287">
   <si>
     <t>id</t>
   </si>
@@ -857,6 +857,30 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>instructions</t>
+  </si>
+  <si>
+    <t>button text</t>
+  </si>
+  <si>
+    <t>view_data_instructions</t>
+  </si>
+  <si>
+    <t>view_data</t>
+  </si>
+  <si>
+    <t>You can select up to 5 timeseries by clicking on rows. Once you've made a selection you can click "View data" below the table to see a sample of the data and optionally download all of it.</t>
+  </si>
+  <si>
+    <t>Vous pouvez sélectionner jusqu'à 5 séries temporelles en cliquant sur les lignes. Une fois votre sélection effectuée, vous pouvez cliquer sur « Voir les données » sous le tableau pour voir un échantillon des données et, si vous le souhaitez, télécharger l'ensemble.</t>
+  </si>
+  <si>
+    <t>View data</t>
+  </si>
+  <si>
+    <t>Voir les données</t>
   </si>
 </sst>
 </file>
@@ -1007,7 +1031,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1238,6 +1262,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1403,7 +1433,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1415,6 +1445,7 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1791,22 +1822,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="D75" sqref="D75"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="43.5546875" customWidth="1"/>
-    <col min="4" max="4" width="49.88671875" customWidth="1"/>
-    <col min="5" max="5" width="54.44140625" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="5" max="5" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1820,7 +1851,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1834,7 +1865,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -1848,7 +1879,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>131</v>
       </c>
@@ -1856,7 +1887,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1870,7 +1901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1884,7 +1915,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1898,7 +1929,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1912,7 +1943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1926,7 +1957,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1940,7 +1971,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1954,7 +1985,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>123</v>
       </c>
@@ -1962,7 +1993,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -1976,7 +2007,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -1990,7 +2021,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>124</v>
       </c>
@@ -1998,7 +2029,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2012,7 +2043,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>125</v>
       </c>
@@ -2020,7 +2051,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -2034,7 +2065,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -2048,7 +2079,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>227</v>
       </c>
@@ -2056,7 +2087,7 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>228</v>
       </c>
@@ -2070,7 +2101,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -2084,7 +2115,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -2098,7 +2129,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>265</v>
       </c>
@@ -2112,7 +2143,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>267</v>
       </c>
@@ -2123,7 +2154,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
         <v>126</v>
       </c>
@@ -2131,7 +2162,7 @@
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>54</v>
       </c>
@@ -2145,7 +2176,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>127</v>
       </c>
@@ -2153,7 +2184,7 @@
       <c r="C28" s="6"/>
       <c r="D28" s="6"/>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -2167,7 +2198,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>105</v>
       </c>
@@ -2181,7 +2212,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>107</v>
       </c>
@@ -2195,7 +2226,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>109</v>
       </c>
@@ -2209,7 +2240,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>132</v>
       </c>
@@ -2223,7 +2254,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>116</v>
       </c>
@@ -2237,7 +2268,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>128</v>
       </c>
@@ -2245,7 +2276,7 @@
       <c r="C35" s="7"/>
       <c r="D35" s="7"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>58</v>
       </c>
@@ -2259,819 +2290,855 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>281</v>
+      </c>
+      <c r="B38" t="s">
+        <v>279</v>
+      </c>
+      <c r="C38" t="s">
+        <v>283</v>
+      </c>
+      <c r="D38" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>282</v>
+      </c>
+      <c r="B39" t="s">
+        <v>280</v>
+      </c>
+      <c r="C39" t="s">
+        <v>285</v>
+      </c>
+      <c r="D39" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+      <c r="B40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>164</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B41" t="s">
         <v>48</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C41" t="s">
         <v>165</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D41" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>170</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B42" t="s">
         <v>167</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C42" t="s">
         <v>168</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D42" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>173</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B43" t="s">
         <v>174</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C43" t="s">
         <v>185</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D43" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>182</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B44" t="s">
         <v>167</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C44" t="s">
         <v>171</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D44" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>175</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B45" t="s">
         <v>174</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C45" t="s">
         <v>184</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D45" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>176</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B46" t="s">
         <v>178</v>
       </c>
-      <c r="C43" s="9" t="s">
+      <c r="C46" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D46" s="9" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>177</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B47" t="s">
         <v>174</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C47" t="s">
         <v>179</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D47" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="8" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>61</v>
       </c>
-      <c r="B46" t="s">
-        <v>9</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="B49" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" t="s">
         <v>62</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D49" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>120</v>
       </c>
-      <c r="B47" t="s">
-        <v>9</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="B50" t="s">
+        <v>9</v>
+      </c>
+      <c r="C50" t="s">
         <v>121</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D50" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>64</v>
       </c>
-      <c r="B48" t="s">
-        <v>9</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
         <v>65</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D51" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>67</v>
       </c>
-      <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
         <v>68</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D52" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>263</v>
       </c>
-      <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
         <v>264</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D53" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>69</v>
       </c>
-      <c r="B51" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
         <v>70</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D54" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>205</v>
       </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
         <v>206</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D55" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>210</v>
       </c>
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
         <v>208</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D56" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>191</v>
       </c>
-      <c r="B54" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
         <v>192</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D57" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
         <v>202</v>
       </c>
-      <c r="B55" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
         <v>203</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D58" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
         <v>217</v>
       </c>
-      <c r="B56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
         <v>218</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D59" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>189</v>
       </c>
-      <c r="B57" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
         <v>236</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D60" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
         <v>72</v>
       </c>
-      <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
         <v>73</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D61" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>199</v>
       </c>
-      <c r="B59" t="s">
-        <v>9</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
         <v>194</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D62" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
         <v>211</v>
       </c>
-      <c r="B60" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
         <v>212</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D63" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>75</v>
       </c>
-      <c r="B61" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
         <v>76</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D64" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
         <v>198</v>
       </c>
-      <c r="B62" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
         <v>200</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D65" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
         <v>214</v>
       </c>
-      <c r="B63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
         <v>215</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D66" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
         <v>78</v>
       </c>
-      <c r="B64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
         <v>79</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D67" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>197</v>
       </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
         <v>195</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D68" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>220</v>
       </c>
-      <c r="B66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
         <v>221</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D69" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>240</v>
       </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
         <v>238</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D70" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>241</v>
       </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
         <v>242</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D71" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>243</v>
       </c>
-      <c r="B69" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
         <v>244</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D72" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>84</v>
       </c>
-      <c r="B70" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
         <v>85</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D73" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>8</v>
       </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
         <v>10</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D74" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>246</v>
       </c>
-      <c r="B72" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
         <v>246</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D75" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
         <v>223</v>
       </c>
-      <c r="B73" t="s">
+      <c r="B76" t="s">
         <v>224</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C76" t="s">
         <v>223</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D76" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>248</v>
       </c>
-      <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
         <v>250</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D77" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
         <v>249</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B78" t="s">
         <v>224</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C78" t="s">
         <v>252</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D78" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
         <v>277</v>
       </c>
-      <c r="B76" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="B79" t="s">
+        <v>9</v>
+      </c>
+      <c r="C79" t="s">
         <v>273</v>
       </c>
-      <c r="D76" t="s">
+      <c r="D79" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
         <v>278</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B80" t="s">
         <v>224</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C80" t="s">
         <v>274</v>
       </c>
-      <c r="D77" t="s">
+      <c r="D80" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
         <v>257</v>
       </c>
-      <c r="B78" t="s">
-        <v>9</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
         <v>259</v>
       </c>
-      <c r="D78" t="s">
+      <c r="D81" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
         <v>258</v>
       </c>
-      <c r="B79" t="s">
+      <c r="B82" t="s">
         <v>224</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C82" t="s">
         <v>260</v>
       </c>
-      <c r="D79" t="s">
+      <c r="D82" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
         <v>135</v>
       </c>
-      <c r="B80" t="s">
-        <v>9</v>
-      </c>
-      <c r="C80" t="s">
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
         <v>136</v>
       </c>
-      <c r="D80" t="s">
+      <c r="D83" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
         <v>254</v>
       </c>
-      <c r="B81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="B84" t="s">
+        <v>9</v>
+      </c>
+      <c r="C84" t="s">
         <v>255</v>
       </c>
-      <c r="D81" t="s">
+      <c r="D84" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
         <v>15</v>
       </c>
-      <c r="B82" t="s">
-        <v>9</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" t="s">
         <v>16</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D85" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A83" s="2" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B83" s="2"/>
-      <c r="C83" s="2"/>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
+      <c r="B86" s="2"/>
+      <c r="C86" s="2"/>
+      <c r="D86" s="2"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
         <v>139</v>
-      </c>
-      <c r="B84" t="s">
-        <v>138</v>
-      </c>
-      <c r="C84" t="s">
-        <v>158</v>
-      </c>
-      <c r="D84" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>156</v>
-      </c>
-      <c r="B85" t="s">
-        <v>138</v>
-      </c>
-      <c r="C85" t="s">
-        <v>159</v>
-      </c>
-      <c r="D85" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>140</v>
-      </c>
-      <c r="B86" t="s">
-        <v>138</v>
-      </c>
-      <c r="C86" t="s">
-        <v>141</v>
-      </c>
-      <c r="D86" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>145</v>
       </c>
       <c r="B87" t="s">
         <v>138</v>
       </c>
       <c r="C87" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="D87" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="B88" t="s">
         <v>138</v>
       </c>
       <c r="C88" t="s">
-        <v>143</v>
+        <v>159</v>
       </c>
       <c r="D88" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="B89" t="s">
         <v>138</v>
       </c>
       <c r="C89" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="D89" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="B90" t="s">
         <v>138</v>
       </c>
       <c r="C90" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="D90" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="B91" t="s">
         <v>138</v>
       </c>
       <c r="C91" t="s">
+        <v>143</v>
+      </c>
+      <c r="D91" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>149</v>
+      </c>
+      <c r="B92" t="s">
+        <v>138</v>
+      </c>
+      <c r="C92" t="s">
+        <v>161</v>
+      </c>
+      <c r="D92" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>151</v>
+      </c>
+      <c r="B93" t="s">
+        <v>138</v>
+      </c>
+      <c r="C93" t="s">
+        <v>160</v>
+      </c>
+      <c r="D93" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>153</v>
+      </c>
+      <c r="B94" t="s">
+        <v>138</v>
+      </c>
+      <c r="C94" t="s">
         <v>154</v>
       </c>
-      <c r="D91" t="s">
+      <c r="D94" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A92" s="4" t="s">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
+      <c r="B95" s="4"/>
+      <c r="C95" s="4"/>
+      <c r="D95" s="4"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>87</v>
-      </c>
-      <c r="B93" t="s">
-        <v>88</v>
-      </c>
-      <c r="C93" t="s">
-        <v>89</v>
-      </c>
-      <c r="D93" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>91</v>
-      </c>
-      <c r="B94" t="s">
-        <v>88</v>
-      </c>
-      <c r="C94" t="s">
-        <v>69</v>
-      </c>
-      <c r="D94" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>188</v>
-      </c>
-      <c r="B95" t="s">
-        <v>88</v>
-      </c>
-      <c r="C95" t="s">
-        <v>189</v>
-      </c>
-      <c r="D95" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A96" t="s">
-        <v>93</v>
       </c>
       <c r="B96" t="s">
         <v>88</v>
       </c>
       <c r="C96" t="s">
+        <v>89</v>
+      </c>
+      <c r="D96" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>91</v>
+      </c>
+      <c r="B97" t="s">
+        <v>88</v>
+      </c>
+      <c r="C97" t="s">
+        <v>69</v>
+      </c>
+      <c r="D97" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>188</v>
+      </c>
+      <c r="B98" t="s">
+        <v>88</v>
+      </c>
+      <c r="C98" t="s">
+        <v>189</v>
+      </c>
+      <c r="D98" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>93</v>
+      </c>
+      <c r="B99" t="s">
+        <v>88</v>
+      </c>
+      <c r="C99" t="s">
         <v>94</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D99" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
dataView modal is mostly functional
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B15484-B128-4A02-8A8A-B51EDC1A42FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35FF538-5D4F-466E-9692-96C52661D623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="289">
   <si>
     <t>id</t>
   </si>
@@ -826,15 +826,9 @@
     <t>tooltip2</t>
   </si>
   <si>
-    <t>UTC-7 or Mountain Standard Time</t>
-  </si>
-  <si>
     <t>Discrètes</t>
   </si>
   <si>
-    <t>UTC-7 ou Heure Normalle des Rocheuses</t>
-  </si>
-  <si>
     <t>Continuous = recorded at regular intervals automatically; Discrete =  measurements or sample acquisition at variable time intervals.</t>
   </si>
   <si>
@@ -871,16 +865,28 @@
     <t>view_data</t>
   </si>
   <si>
-    <t>You can select up to 5 timeseries by clicking on rows. Once you've made a selection you can click "View data" below the table to see a sample of the data and optionally download all of it.</t>
-  </si>
-  <si>
-    <t>Vous pouvez sélectionner jusqu'à 5 séries temporelles en cliquant sur les lignes. Une fois votre sélection effectuée, vous pouvez cliquer sur « Voir les données » sous le tableau pour voir un échantillon des données et, si vous le souhaitez, télécharger l'ensemble.</t>
-  </si>
-  <si>
     <t>View data</t>
   </si>
   <si>
     <t>Voir les données</t>
+  </si>
+  <si>
+    <t>view_plots</t>
+  </si>
+  <si>
+    <t>View plots</t>
+  </si>
+  <si>
+    <t>Voir les graphiques</t>
+  </si>
+  <si>
+    <t>UTC-7</t>
+  </si>
+  <si>
+    <t>Once you've made a selection you can click "View data" below the table to see a sample of the data and optionally download all of it.</t>
+  </si>
+  <si>
+    <t>Une fois votre sélection effectuée, vous pouvez cliquer sur « Voir les données » sous le tableau pour voir un échantillon des données et, si vous le souhaitez, télécharger l'ensemble.</t>
   </si>
 </sst>
 </file>
@@ -1822,22 +1828,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D99"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.109375" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="43.5703125" customWidth="1"/>
-    <col min="4" max="4" width="49.85546875" customWidth="1"/>
-    <col min="5" max="5" width="54.42578125" customWidth="1"/>
+    <col min="3" max="3" width="43.5546875" customWidth="1"/>
+    <col min="4" max="4" width="49.88671875" customWidth="1"/>
+    <col min="5" max="5" width="54.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1851,7 +1857,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1865,7 +1871,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>131</v>
       </c>
@@ -1887,7 +1893,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -1901,7 +1907,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -1915,7 +1921,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1943,7 +1949,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1957,7 +1963,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -1971,7 +1977,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -1985,7 +1991,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>123</v>
       </c>
@@ -1993,7 +1999,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>40</v>
       </c>
@@ -2007,7 +2013,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>43</v>
       </c>
@@ -2021,7 +2027,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>124</v>
       </c>
@@ -2029,7 +2035,7 @@
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -2043,7 +2049,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>125</v>
       </c>
@@ -2051,7 +2057,7 @@
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -2065,7 +2071,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>96</v>
       </c>
@@ -2079,7 +2085,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>227</v>
       </c>
@@ -2087,7 +2093,7 @@
       <c r="C20" s="10"/>
       <c r="D20" s="10"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>228</v>
       </c>
@@ -2101,7 +2107,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>81</v>
       </c>
@@ -2115,7 +2121,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>226</v>
       </c>
@@ -2129,7 +2135,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>265</v>
       </c>
@@ -2137,1008 +2143,1025 @@
         <v>266</v>
       </c>
       <c r="C24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D24" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>267</v>
       </c>
+      <c r="B25" t="s">
+        <v>266</v>
+      </c>
       <c r="C25" t="s">
-        <v>268</v>
+        <v>286</v>
       </c>
       <c r="D25" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>280</v>
+      </c>
+      <c r="B26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C26" t="s">
+        <v>281</v>
+      </c>
+      <c r="D26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>283</v>
+      </c>
+      <c r="B27" t="s">
+        <v>278</v>
+      </c>
+      <c r="C27" t="s">
+        <v>284</v>
+      </c>
+      <c r="D27" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
         <v>54</v>
-      </c>
-      <c r="B27" t="s">
-        <v>48</v>
-      </c>
-      <c r="C27" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B28" s="6"/>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>56</v>
       </c>
       <c r="B29" t="s">
         <v>48</v>
       </c>
       <c r="C29" t="s">
+        <v>55</v>
+      </c>
+      <c r="D29" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>56</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
         <v>57</v>
       </c>
-      <c r="D29" t="s">
+      <c r="D31" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>105</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B32" t="s">
         <v>106</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C32" t="s">
         <v>114</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D32" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
         <v>107</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B33" t="s">
         <v>108</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" t="s">
         <v>110</v>
       </c>
-      <c r="D31" t="s">
+      <c r="D33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
         <v>109</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B34" t="s">
         <v>108</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" t="s">
         <v>111</v>
       </c>
-      <c r="D32" t="s">
+      <c r="D34" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
         <v>132</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B35" t="s">
         <v>106</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C35" t="s">
         <v>133</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D35" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
         <v>116</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B36" t="s">
         <v>117</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C36" t="s">
         <v>118</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D36" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="7" t="s">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
         <v>58</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B38" t="s">
         <v>48</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C38" t="s">
         <v>59</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D38" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="11" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>281</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
         <v>279</v>
       </c>
-      <c r="C38" t="s">
-        <v>283</v>
-      </c>
-      <c r="D38" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>282</v>
-      </c>
-      <c r="B39" t="s">
-        <v>280</v>
-      </c>
-      <c r="C39" t="s">
-        <v>285</v>
-      </c>
-      <c r="D39" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="4" t="s">
+      <c r="B40" t="s">
+        <v>277</v>
+      </c>
+      <c r="C40" t="s">
+        <v>287</v>
+      </c>
+      <c r="D40" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="B42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>164</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B43" t="s">
         <v>48</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C43" t="s">
         <v>165</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D43" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>170</v>
-      </c>
-      <c r="B42" t="s">
-        <v>167</v>
-      </c>
-      <c r="C42" t="s">
-        <v>168</v>
-      </c>
-      <c r="D42" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>173</v>
-      </c>
-      <c r="B43" t="s">
-        <v>174</v>
-      </c>
-      <c r="C43" t="s">
-        <v>185</v>
-      </c>
-      <c r="D43" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>182</v>
       </c>
       <c r="B44" t="s">
         <v>167</v>
       </c>
       <c r="C44" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D44" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B45" t="s">
         <v>174</v>
       </c>
       <c r="C45" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="D45" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="B46" t="s">
-        <v>178</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+      <c r="C46" t="s">
+        <v>171</v>
+      </c>
+      <c r="D46" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B47" t="s">
         <v>174</v>
       </c>
       <c r="C47" t="s">
+        <v>184</v>
+      </c>
+      <c r="D47" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>176</v>
+      </c>
+      <c r="B48" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D48" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>177</v>
+      </c>
+      <c r="B49" t="s">
+        <v>174</v>
+      </c>
+      <c r="C49" t="s">
         <v>179</v>
       </c>
-      <c r="D47" t="s">
+      <c r="D49" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="8" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>61</v>
       </c>
-      <c r="B49" t="s">
-        <v>9</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="B51" t="s">
+        <v>9</v>
+      </c>
+      <c r="C51" t="s">
         <v>62</v>
       </c>
-      <c r="D49" t="s">
+      <c r="D51" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>120</v>
       </c>
-      <c r="B50" t="s">
-        <v>9</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="B52" t="s">
+        <v>9</v>
+      </c>
+      <c r="C52" t="s">
         <v>121</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D52" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>64</v>
       </c>
-      <c r="B51" t="s">
-        <v>9</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+      <c r="C53" t="s">
         <v>65</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D53" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>67</v>
       </c>
-      <c r="B52" t="s">
-        <v>9</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="B54" t="s">
+        <v>9</v>
+      </c>
+      <c r="C54" t="s">
         <v>68</v>
       </c>
-      <c r="D52" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="D54" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
         <v>263</v>
       </c>
-      <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B55" t="s">
+        <v>9</v>
+      </c>
+      <c r="C55" t="s">
         <v>264</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D55" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
         <v>69</v>
       </c>
-      <c r="B54" t="s">
-        <v>9</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56" t="s">
         <v>70</v>
       </c>
-      <c r="D54" t="s">
+      <c r="D56" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
         <v>205</v>
       </c>
-      <c r="B55" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" t="s">
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" t="s">
         <v>206</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D57" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
         <v>210</v>
       </c>
-      <c r="B56" t="s">
-        <v>9</v>
-      </c>
-      <c r="C56" t="s">
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58" t="s">
         <v>208</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D58" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
         <v>191</v>
       </c>
-      <c r="B57" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" t="s">
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59" t="s">
         <v>192</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D59" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
         <v>202</v>
       </c>
-      <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
+      <c r="B60" t="s">
+        <v>9</v>
+      </c>
+      <c r="C60" t="s">
         <v>203</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D60" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
         <v>217</v>
       </c>
-      <c r="B59" t="s">
-        <v>9</v>
-      </c>
-      <c r="C59" t="s">
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61" t="s">
         <v>218</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D61" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>189</v>
       </c>
-      <c r="B60" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" t="s">
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
         <v>236</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D62" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
         <v>72</v>
       </c>
-      <c r="B61" t="s">
-        <v>9</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="s">
         <v>73</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
         <v>199</v>
       </c>
-      <c r="B62" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" t="s">
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="s">
         <v>194</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D64" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
         <v>211</v>
       </c>
-      <c r="B63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63" t="s">
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="s">
         <v>212</v>
       </c>
-      <c r="D63" t="s">
+      <c r="D65" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>75</v>
       </c>
-      <c r="B64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" t="s">
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="s">
         <v>76</v>
       </c>
-      <c r="D64" t="s">
+      <c r="D66" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
         <v>198</v>
       </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" t="s">
+      <c r="B67" t="s">
+        <v>9</v>
+      </c>
+      <c r="C67" t="s">
         <v>200</v>
       </c>
-      <c r="D65" t="s">
+      <c r="D67" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
         <v>214</v>
       </c>
-      <c r="B66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" t="s">
+      <c r="B68" t="s">
+        <v>9</v>
+      </c>
+      <c r="C68" t="s">
         <v>215</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D68" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
         <v>78</v>
       </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" t="s">
+      <c r="B69" t="s">
+        <v>9</v>
+      </c>
+      <c r="C69" t="s">
         <v>79</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D69" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
         <v>197</v>
       </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" t="s">
+      <c r="B70" t="s">
+        <v>9</v>
+      </c>
+      <c r="C70" t="s">
         <v>195</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D70" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
         <v>220</v>
       </c>
-      <c r="B69" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="B71" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" t="s">
         <v>221</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D71" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
         <v>240</v>
       </c>
-      <c r="B70" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" t="s">
+      <c r="B72" t="s">
+        <v>9</v>
+      </c>
+      <c r="C72" t="s">
         <v>238</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D72" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
         <v>241</v>
       </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" t="s">
+      <c r="B73" t="s">
+        <v>9</v>
+      </c>
+      <c r="C73" t="s">
         <v>242</v>
       </c>
-      <c r="D71" t="s">
+      <c r="D73" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
         <v>243</v>
       </c>
-      <c r="B72" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" t="s">
+      <c r="B74" t="s">
+        <v>9</v>
+      </c>
+      <c r="C74" t="s">
         <v>244</v>
       </c>
-      <c r="D72" t="s">
+      <c r="D74" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
         <v>84</v>
       </c>
-      <c r="B73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" t="s">
+      <c r="B75" t="s">
+        <v>9</v>
+      </c>
+      <c r="C75" t="s">
         <v>85</v>
       </c>
-      <c r="D73" t="s">
+      <c r="D75" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
         <v>8</v>
       </c>
-      <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="B76" t="s">
+        <v>9</v>
+      </c>
+      <c r="C76" t="s">
         <v>10</v>
       </c>
-      <c r="D74" t="s">
+      <c r="D76" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
         <v>246</v>
       </c>
-      <c r="B75" t="s">
-        <v>9</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="B77" t="s">
+        <v>9</v>
+      </c>
+      <c r="C77" t="s">
         <v>246</v>
       </c>
-      <c r="D75" t="s">
+      <c r="D77" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
         <v>223</v>
-      </c>
-      <c r="B76" t="s">
-        <v>224</v>
-      </c>
-      <c r="C76" t="s">
-        <v>223</v>
-      </c>
-      <c r="D76" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>248</v>
-      </c>
-      <c r="B77" t="s">
-        <v>9</v>
-      </c>
-      <c r="C77" t="s">
-        <v>250</v>
-      </c>
-      <c r="D77" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>249</v>
       </c>
       <c r="B78" t="s">
         <v>224</v>
       </c>
       <c r="C78" t="s">
-        <v>252</v>
+        <v>223</v>
       </c>
       <c r="D78" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>277</v>
+        <v>248</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="D79" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>278</v>
+        <v>249</v>
       </c>
       <c r="B80" t="s">
         <v>224</v>
       </c>
       <c r="C80" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="D80" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>275</v>
+      </c>
+      <c r="B81" t="s">
+        <v>9</v>
+      </c>
+      <c r="C81" t="s">
+        <v>271</v>
+      </c>
+      <c r="D81" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>257</v>
-      </c>
-      <c r="B81" t="s">
-        <v>9</v>
-      </c>
-      <c r="C81" t="s">
-        <v>259</v>
-      </c>
-      <c r="D81" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>258</v>
       </c>
       <c r="B82" t="s">
         <v>224</v>
       </c>
       <c r="C82" t="s">
+        <v>272</v>
+      </c>
+      <c r="D82" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>257</v>
+      </c>
+      <c r="B83" t="s">
+        <v>9</v>
+      </c>
+      <c r="C83" t="s">
+        <v>259</v>
+      </c>
+      <c r="D83" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>258</v>
+      </c>
+      <c r="B84" t="s">
+        <v>224</v>
+      </c>
+      <c r="C84" t="s">
         <v>260</v>
       </c>
-      <c r="D82" t="s">
+      <c r="D84" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
         <v>135</v>
       </c>
-      <c r="B83" t="s">
-        <v>9</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="B85" t="s">
+        <v>9</v>
+      </c>
+      <c r="C85" t="s">
         <v>136</v>
       </c>
-      <c r="D83" t="s">
+      <c r="D85" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
         <v>254</v>
       </c>
-      <c r="B84" t="s">
-        <v>9</v>
-      </c>
-      <c r="C84" t="s">
+      <c r="B86" t="s">
+        <v>9</v>
+      </c>
+      <c r="C86" t="s">
         <v>255</v>
       </c>
-      <c r="D84" t="s">
+      <c r="D86" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
         <v>15</v>
       </c>
-      <c r="B85" t="s">
-        <v>9</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="B87" t="s">
+        <v>9</v>
+      </c>
+      <c r="C87" t="s">
         <v>16</v>
       </c>
-      <c r="D85" t="s">
+      <c r="D87" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="2" t="s">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B86" s="2"/>
-      <c r="C86" s="2"/>
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="B88" s="2"/>
+      <c r="C88" s="2"/>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
         <v>139</v>
-      </c>
-      <c r="B87" t="s">
-        <v>138</v>
-      </c>
-      <c r="C87" t="s">
-        <v>158</v>
-      </c>
-      <c r="D87" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>156</v>
-      </c>
-      <c r="B88" t="s">
-        <v>138</v>
-      </c>
-      <c r="C88" t="s">
-        <v>159</v>
-      </c>
-      <c r="D88" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>140</v>
       </c>
       <c r="B89" t="s">
         <v>138</v>
       </c>
       <c r="C89" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="D89" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B90" t="s">
         <v>138</v>
       </c>
       <c r="C90" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="D90" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B91" t="s">
         <v>138</v>
       </c>
       <c r="C91" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D91" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B92" t="s">
         <v>138</v>
       </c>
       <c r="C92" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="D92" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B93" t="s">
         <v>138</v>
       </c>
       <c r="C93" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D93" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B94" t="s">
         <v>138</v>
       </c>
       <c r="C94" t="s">
+        <v>161</v>
+      </c>
+      <c r="D94" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>151</v>
+      </c>
+      <c r="B95" t="s">
+        <v>138</v>
+      </c>
+      <c r="C95" t="s">
+        <v>160</v>
+      </c>
+      <c r="D95" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>153</v>
+      </c>
+      <c r="B96" t="s">
+        <v>138</v>
+      </c>
+      <c r="C96" t="s">
         <v>154</v>
       </c>
-      <c r="D94" t="s">
+      <c r="D96" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="4" t="s">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B95" s="4"/>
-      <c r="C95" s="4"/>
-      <c r="D95" s="4"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="B97" s="4"/>
+      <c r="C97" s="4"/>
+      <c r="D97" s="4"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
         <v>87</v>
-      </c>
-      <c r="B96" t="s">
-        <v>88</v>
-      </c>
-      <c r="C96" t="s">
-        <v>89</v>
-      </c>
-      <c r="D96" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>91</v>
-      </c>
-      <c r="B97" t="s">
-        <v>88</v>
-      </c>
-      <c r="C97" t="s">
-        <v>69</v>
-      </c>
-      <c r="D97" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>188</v>
       </c>
       <c r="B98" t="s">
         <v>88</v>
       </c>
       <c r="C98" t="s">
-        <v>189</v>
+        <v>89</v>
       </c>
       <c r="D98" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B99" t="s">
         <v>88</v>
       </c>
       <c r="C99" t="s">
+        <v>69</v>
+      </c>
+      <c r="D99" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>188</v>
+      </c>
+      <c r="B100" t="s">
+        <v>88</v>
+      </c>
+      <c r="C100" t="s">
+        <v>189</v>
+      </c>
+      <c r="D100" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>93</v>
+      </c>
+      <c r="B101" t="s">
+        <v>88</v>
+      </c>
+      <c r="C101" t="s">
         <v>94</v>
       </c>
-      <c r="D99" t="s">
+      <c r="D101" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
data view modal is now ready
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A35FF538-5D4F-466E-9692-96C52661D623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CBB31B-768A-4C2A-A7C8-E80D990AF98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="307">
   <si>
     <t>id</t>
   </si>
@@ -887,6 +887,60 @@
   </si>
   <si>
     <t>Une fois votre sélection effectuée, vous pouvez cliquer sur « Voir les données » sous le tableau pour voir un échantillon des données et, si vous le souhaitez, télécharger l'ensemble.</t>
+  </si>
+  <si>
+    <t>dl_num_rows</t>
+  </si>
+  <si>
+    <t>Number of rows that will be returned:</t>
+  </si>
+  <si>
+    <t>Nombre de rangées à télécharger:</t>
+  </si>
+  <si>
+    <t>advice about number of rows selected (modal)</t>
+  </si>
+  <si>
+    <t>daily</t>
+  </si>
+  <si>
+    <t>hourly</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>Daily</t>
+  </si>
+  <si>
+    <t>Hourly</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>Horaire</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Journalière</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>Frequency:</t>
+  </si>
+  <si>
+    <t>Fréquence:</t>
+  </si>
+  <si>
+    <t>modal selection title</t>
+  </si>
+  <si>
+    <t>modal selection</t>
   </si>
 </sst>
 </file>
@@ -1828,10 +1882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:D106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2086,1082 +2140,1152 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="B20" s="10"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
+      <c r="A20" t="s">
+        <v>289</v>
+      </c>
+      <c r="B20" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" t="s">
+        <v>290</v>
+      </c>
+      <c r="D20" t="s">
+        <v>291</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>228</v>
+        <v>302</v>
       </c>
       <c r="B21" t="s">
-        <v>229</v>
+        <v>305</v>
       </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>303</v>
       </c>
       <c r="D21" t="s">
-        <v>104</v>
+        <v>304</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>81</v>
+        <v>293</v>
       </c>
       <c r="B22" t="s">
-        <v>231</v>
+        <v>306</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>296</v>
       </c>
       <c r="D22" t="s">
-        <v>83</v>
+        <v>301</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>226</v>
+        <v>294</v>
       </c>
       <c r="B23" t="s">
-        <v>232</v>
+        <v>306</v>
       </c>
       <c r="C23" t="s">
-        <v>233</v>
+        <v>297</v>
       </c>
       <c r="D23" t="s">
-        <v>234</v>
+        <v>299</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>265</v>
+        <v>295</v>
       </c>
       <c r="B24" t="s">
-        <v>266</v>
+        <v>306</v>
       </c>
       <c r="C24" t="s">
-        <v>269</v>
+        <v>298</v>
       </c>
       <c r="D24" t="s">
-        <v>270</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>267</v>
-      </c>
-      <c r="B25" t="s">
-        <v>266</v>
-      </c>
-      <c r="C25" t="s">
-        <v>286</v>
-      </c>
-      <c r="D25" t="s">
-        <v>286</v>
-      </c>
+      <c r="A25" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>280</v>
+        <v>228</v>
       </c>
       <c r="B26" t="s">
-        <v>278</v>
+        <v>229</v>
       </c>
       <c r="C26" t="s">
-        <v>281</v>
+        <v>103</v>
       </c>
       <c r="D26" t="s">
-        <v>282</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>283</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>278</v>
+        <v>231</v>
       </c>
       <c r="C27" t="s">
-        <v>284</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>285</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B28" s="5"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="A28" t="s">
+        <v>226</v>
+      </c>
+      <c r="B28" t="s">
+        <v>232</v>
+      </c>
+      <c r="C28" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>265</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>266</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>269</v>
       </c>
       <c r="D29" t="s">
-        <v>55</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B30" s="6"/>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
+      <c r="A30" t="s">
+        <v>267</v>
+      </c>
+      <c r="B30" t="s">
+        <v>266</v>
+      </c>
+      <c r="C30" t="s">
+        <v>286</v>
+      </c>
+      <c r="D30" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>56</v>
+        <v>280</v>
       </c>
       <c r="B31" t="s">
-        <v>48</v>
+        <v>278</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>281</v>
       </c>
       <c r="D31" t="s">
-        <v>57</v>
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>105</v>
+        <v>283</v>
       </c>
       <c r="B32" t="s">
-        <v>106</v>
+        <v>278</v>
       </c>
       <c r="C32" t="s">
-        <v>114</v>
+        <v>284</v>
       </c>
       <c r="D32" t="s">
-        <v>115</v>
+        <v>285</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" t="s">
-        <v>110</v>
-      </c>
-      <c r="D33" t="s">
-        <v>112</v>
-      </c>
+      <c r="A33" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" s="5"/>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="B34" t="s">
-        <v>108</v>
+        <v>48</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>113</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>132</v>
-      </c>
-      <c r="B35" t="s">
-        <v>106</v>
-      </c>
-      <c r="C35" t="s">
-        <v>133</v>
-      </c>
-      <c r="D35" t="s">
-        <v>235</v>
-      </c>
+      <c r="A35" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="B36" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="C36" t="s">
-        <v>118</v>
+        <v>57</v>
       </c>
       <c r="D36" t="s">
-        <v>119</v>
+        <v>57</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B37" s="7"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="7"/>
+      <c r="A37" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" t="s">
+        <v>114</v>
+      </c>
+      <c r="D37" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>107</v>
       </c>
       <c r="B38" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="C38" t="s">
-        <v>59</v>
+        <v>110</v>
       </c>
       <c r="D38" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B39" s="11"/>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11"/>
+      <c r="A39" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" t="s">
+        <v>108</v>
+      </c>
+      <c r="C39" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>279</v>
+        <v>132</v>
       </c>
       <c r="B40" t="s">
-        <v>277</v>
+        <v>106</v>
       </c>
       <c r="C40" t="s">
-        <v>287</v>
+        <v>133</v>
       </c>
       <c r="D40" t="s">
-        <v>288</v>
+        <v>235</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>116</v>
+      </c>
+      <c r="B41" t="s">
+        <v>117</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+      <c r="D41" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
+      <c r="A42" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="7"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="7"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>164</v>
+        <v>58</v>
       </c>
       <c r="B43" t="s">
         <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>165</v>
+        <v>59</v>
       </c>
       <c r="D43" t="s">
-        <v>166</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>170</v>
-      </c>
-      <c r="B44" t="s">
-        <v>167</v>
-      </c>
-      <c r="C44" t="s">
-        <v>168</v>
-      </c>
-      <c r="D44" t="s">
-        <v>169</v>
-      </c>
+      <c r="A44" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>173</v>
+        <v>279</v>
       </c>
       <c r="B45" t="s">
-        <v>174</v>
+        <v>277</v>
       </c>
       <c r="C45" t="s">
-        <v>185</v>
+        <v>287</v>
       </c>
       <c r="D45" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>182</v>
-      </c>
-      <c r="B46" t="s">
-        <v>167</v>
-      </c>
-      <c r="C46" t="s">
-        <v>171</v>
-      </c>
-      <c r="D46" t="s">
-        <v>172</v>
+        <v>288</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>175</v>
-      </c>
-      <c r="B47" t="s">
-        <v>174</v>
-      </c>
-      <c r="C47" t="s">
-        <v>184</v>
-      </c>
-      <c r="D47" t="s">
-        <v>183</v>
-      </c>
+      <c r="A47" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="B48" t="s">
-        <v>178</v>
-      </c>
-      <c r="C48" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D48" s="9" t="s">
-        <v>180</v>
+        <v>48</v>
+      </c>
+      <c r="C48" t="s">
+        <v>165</v>
+      </c>
+      <c r="D48" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="B49" t="s">
+        <v>167</v>
+      </c>
+      <c r="C49" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>173</v>
+      </c>
+      <c r="B50" t="s">
         <v>174</v>
       </c>
-      <c r="C49" t="s">
-        <v>179</v>
-      </c>
-      <c r="D49" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B50" s="8"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="8"/>
+      <c r="C50" t="s">
+        <v>185</v>
+      </c>
+      <c r="D50" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>61</v>
+        <v>182</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
       <c r="C51" t="s">
-        <v>62</v>
+        <v>171</v>
       </c>
       <c r="D51" t="s">
-        <v>63</v>
+        <v>172</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>175</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="C52" t="s">
-        <v>121</v>
+        <v>184</v>
       </c>
       <c r="D52" t="s">
-        <v>122</v>
+        <v>183</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>64</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
-      </c>
-      <c r="C53" t="s">
-        <v>65</v>
-      </c>
-      <c r="D53" t="s">
-        <v>66</v>
+        <v>178</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>67</v>
+        <v>177</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="C54" t="s">
-        <v>68</v>
+        <v>179</v>
       </c>
       <c r="D54" t="s">
-        <v>268</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>263</v>
-      </c>
-      <c r="B55" t="s">
-        <v>9</v>
-      </c>
-      <c r="C55" t="s">
-        <v>264</v>
-      </c>
-      <c r="D55" t="s">
-        <v>264</v>
-      </c>
+      <c r="A55" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
       </c>
       <c r="C56" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D56" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>205</v>
+        <v>120</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
       </c>
       <c r="C57" t="s">
-        <v>206</v>
+        <v>121</v>
       </c>
       <c r="D57" t="s">
-        <v>207</v>
+        <v>122</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>210</v>
+        <v>64</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>208</v>
+        <v>65</v>
       </c>
       <c r="D58" t="s">
-        <v>209</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>191</v>
+        <v>67</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
       </c>
       <c r="C59" t="s">
-        <v>192</v>
+        <v>68</v>
       </c>
       <c r="D59" t="s">
-        <v>193</v>
+        <v>268</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>202</v>
+        <v>263</v>
       </c>
       <c r="B60" t="s">
         <v>9</v>
       </c>
       <c r="C60" t="s">
-        <v>203</v>
+        <v>264</v>
       </c>
       <c r="D60" t="s">
-        <v>204</v>
+        <v>264</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>217</v>
+        <v>69</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
       </c>
       <c r="C61" t="s">
-        <v>218</v>
+        <v>70</v>
       </c>
       <c r="D61" t="s">
-        <v>219</v>
+        <v>71</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="B62" t="s">
         <v>9</v>
       </c>
       <c r="C62" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="D62" t="s">
-        <v>237</v>
+        <v>207</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>72</v>
+        <v>210</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>73</v>
+        <v>208</v>
       </c>
       <c r="D63" t="s">
-        <v>74</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D64" t="s">
-        <v>17</v>
+        <v>193</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D65" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>75</v>
+        <v>217</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>76</v>
+        <v>218</v>
       </c>
       <c r="D66" t="s">
-        <v>77</v>
+        <v>219</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>200</v>
+        <v>236</v>
       </c>
       <c r="D67" t="s">
-        <v>201</v>
+        <v>237</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>214</v>
+        <v>72</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>215</v>
+        <v>73</v>
       </c>
       <c r="D68" t="s">
-        <v>216</v>
+        <v>74</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>199</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>79</v>
+        <v>194</v>
       </c>
       <c r="D69" t="s">
-        <v>80</v>
+        <v>17</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>197</v>
+        <v>211</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="D70" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>220</v>
+        <v>75</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>221</v>
+        <v>76</v>
       </c>
       <c r="D71" t="s">
-        <v>222</v>
+        <v>77</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>240</v>
+        <v>198</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>238</v>
+        <v>200</v>
       </c>
       <c r="D72" t="s">
-        <v>239</v>
+        <v>201</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>241</v>
+        <v>214</v>
       </c>
       <c r="B73" t="s">
         <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>242</v>
+        <v>215</v>
       </c>
       <c r="D73" t="s">
-        <v>134</v>
+        <v>216</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>243</v>
+        <v>78</v>
       </c>
       <c r="B74" t="s">
         <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>244</v>
+        <v>79</v>
       </c>
       <c r="D74" t="s">
-        <v>245</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>84</v>
+        <v>197</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>85</v>
+        <v>195</v>
       </c>
       <c r="D75" t="s">
-        <v>86</v>
+        <v>196</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>8</v>
+        <v>220</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>10</v>
+        <v>221</v>
       </c>
       <c r="D76" t="s">
-        <v>11</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D77" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>223</v>
+        <v>241</v>
       </c>
       <c r="B78" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>223</v>
+        <v>242</v>
       </c>
       <c r="D78" t="s">
-        <v>225</v>
+        <v>134</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="D79" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>249</v>
+        <v>84</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>252</v>
+        <v>85</v>
       </c>
       <c r="D80" t="s">
-        <v>253</v>
+        <v>86</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>275</v>
+        <v>8</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>271</v>
+        <v>10</v>
       </c>
       <c r="D81" t="s">
-        <v>273</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>276</v>
+        <v>246</v>
       </c>
       <c r="B82" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>272</v>
+        <v>246</v>
       </c>
       <c r="D82" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>257</v>
+        <v>223</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="C83" t="s">
-        <v>259</v>
+        <v>223</v>
       </c>
       <c r="D83" t="s">
-        <v>261</v>
+        <v>225</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="B84" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D84" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>135</v>
+        <v>249</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="C85" t="s">
-        <v>136</v>
+        <v>252</v>
       </c>
       <c r="D85" t="s">
-        <v>137</v>
+        <v>253</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>254</v>
+        <v>275</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>255</v>
+        <v>271</v>
       </c>
       <c r="D86" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>15</v>
+        <v>276</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="C87" t="s">
-        <v>16</v>
+        <v>272</v>
       </c>
       <c r="D87" t="s">
-        <v>17</v>
+        <v>274</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A88" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B88" s="2"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
+      <c r="A88" t="s">
+        <v>257</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
+      </c>
+      <c r="C88" t="s">
+        <v>259</v>
+      </c>
+      <c r="D88" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>139</v>
+        <v>258</v>
       </c>
       <c r="B89" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
       <c r="C89" t="s">
-        <v>158</v>
+        <v>260</v>
       </c>
       <c r="D89" t="s">
-        <v>157</v>
+        <v>262</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B90" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>159</v>
+        <v>136</v>
       </c>
       <c r="D90" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>140</v>
+        <v>254</v>
       </c>
       <c r="B91" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>141</v>
+        <v>255</v>
       </c>
       <c r="D91" t="s">
-        <v>148</v>
+        <v>256</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>145</v>
+        <v>15</v>
       </c>
       <c r="B92" t="s">
+        <v>9</v>
+      </c>
+      <c r="C92" t="s">
+        <v>16</v>
+      </c>
+      <c r="D92" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C92" t="s">
-        <v>146</v>
-      </c>
-      <c r="D92" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>142</v>
-      </c>
-      <c r="B93" t="s">
-        <v>138</v>
-      </c>
-      <c r="C93" t="s">
-        <v>143</v>
-      </c>
-      <c r="D93" t="s">
-        <v>144</v>
-      </c>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B94" t="s">
         <v>138</v>
       </c>
       <c r="C94" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D94" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="B95" t="s">
         <v>138</v>
       </c>
       <c r="C95" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D95" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
       <c r="B96" t="s">
         <v>138</v>
       </c>
       <c r="C96" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="D96" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A97" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B97" s="4"/>
-      <c r="C97" s="4"/>
-      <c r="D97" s="4"/>
+      <c r="A97" t="s">
+        <v>145</v>
+      </c>
+      <c r="B97" t="s">
+        <v>138</v>
+      </c>
+      <c r="C97" t="s">
+        <v>146</v>
+      </c>
+      <c r="D97" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>87</v>
+        <v>142</v>
       </c>
       <c r="B98" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C98" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="D98" t="s">
-        <v>90</v>
+        <v>144</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>91</v>
+        <v>149</v>
       </c>
       <c r="B99" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C99" t="s">
-        <v>69</v>
+        <v>161</v>
       </c>
       <c r="D99" t="s">
-        <v>92</v>
+        <v>150</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="B100" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C100" t="s">
-        <v>189</v>
+        <v>160</v>
       </c>
       <c r="D100" t="s">
-        <v>190</v>
+        <v>152</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>153</v>
+      </c>
+      <c r="B101" t="s">
+        <v>138</v>
+      </c>
+      <c r="C101" t="s">
+        <v>154</v>
+      </c>
+      <c r="D101" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>87</v>
+      </c>
+      <c r="B103" t="s">
+        <v>88</v>
+      </c>
+      <c r="C103" t="s">
+        <v>89</v>
+      </c>
+      <c r="D103" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>91</v>
+      </c>
+      <c r="B104" t="s">
+        <v>88</v>
+      </c>
+      <c r="C104" t="s">
+        <v>69</v>
+      </c>
+      <c r="D104" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>188</v>
+      </c>
+      <c r="B105" t="s">
+        <v>88</v>
+      </c>
+      <c r="C105" t="s">
+        <v>189</v>
+      </c>
+      <c r="D105" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
         <v>93</v>
       </c>
-      <c r="B101" t="s">
+      <c r="B106" t="s">
         <v>88</v>
       </c>
-      <c r="C101" t="s">
+      <c r="C106" t="s">
         <v>94</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D106" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more download modal work
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CBB31B-768A-4C2A-A7C8-E80D990AF98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F9CD95-1204-4DF7-B9F2-985240F37C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="335">
   <si>
     <t>id</t>
   </si>
@@ -727,9 +727,6 @@
     <t>Ou choisissez une ou plusieures stations</t>
   </si>
   <si>
-    <t>Plage de dates</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -910,37 +907,124 @@
     <t>max</t>
   </si>
   <si>
-    <t>Daily</t>
-  </si>
-  <si>
-    <t>Hourly</t>
-  </si>
-  <si>
-    <t>Max</t>
-  </si>
-  <si>
-    <t>Horaire</t>
-  </si>
-  <si>
-    <t>Maximum</t>
-  </si>
-  <si>
-    <t>Journalière</t>
-  </si>
-  <si>
     <t>frequency</t>
   </si>
   <si>
     <t>Frequency:</t>
   </si>
   <si>
-    <t>Fréquence:</t>
-  </si>
-  <si>
     <t>modal selection title</t>
   </si>
   <si>
     <t>modal selection</t>
+  </si>
+  <si>
+    <t>data_subset_msg</t>
+  </si>
+  <si>
+    <t>modal message</t>
+  </si>
+  <si>
+    <t>Subset of data (3 rows per timeseries)</t>
+  </si>
+  <si>
+    <t>Journalière (avec statistiques)</t>
+  </si>
+  <si>
+    <t>Daily (with statistics)</t>
+  </si>
+  <si>
+    <t>Sous-ensemble de données (3 lignes par série temporelle)</t>
+  </si>
+  <si>
+    <t>Location metadata (up to first three rows)</t>
+  </si>
+  <si>
+    <t>Métadonnées des sites (jusqu'aux trois premières lignes)</t>
+  </si>
+  <si>
+    <t>extra_tbl_msg</t>
+  </si>
+  <si>
+    <t>Tables for grades and approvals will also be included as part of your download.</t>
+  </si>
+  <si>
+    <t>Des tableaux pour les notes de qualité et les approbations seront également inclus dans votre téléchargement.</t>
+  </si>
+  <si>
+    <t>date_range_select</t>
+  </si>
+  <si>
+    <t>Select a date range</t>
+  </si>
+  <si>
+    <t>Choissez la plage temporelle</t>
+  </si>
+  <si>
+    <t>Plage temporelle</t>
+  </si>
+  <si>
+    <t>dl_format</t>
+  </si>
+  <si>
+    <t>Choose a format</t>
+  </si>
+  <si>
+    <t>Sélectionnez un format</t>
+  </si>
+  <si>
+    <t>dl_format_xlsx</t>
+  </si>
+  <si>
+    <t>dl_format_csv</t>
+  </si>
+  <si>
+    <t>.xlsx (Microsoft Excel workbook)</t>
+  </si>
+  <si>
+    <t>.xlsx (fichier Microsoft Excel)</t>
+  </si>
+  <si>
+    <t>.csv (multiple zipped files)</t>
+  </si>
+  <si>
+    <t>.csv (multiples fichiers zippés)</t>
+  </si>
+  <si>
+    <t>dl_format_sqlite</t>
+  </si>
+  <si>
+    <t>.sqlite (database)</t>
+  </si>
+  <si>
+    <t>.sqlite (base de données)</t>
+  </si>
+  <si>
+    <t>loc_meta_msg</t>
+  </si>
+  <si>
+    <t>Hourly + daily</t>
+  </si>
+  <si>
+    <t>Max + daily</t>
+  </si>
+  <si>
+    <t>Horaire + journalière</t>
+  </si>
+  <si>
+    <t>Maximum + journalière</t>
+  </si>
+  <si>
+    <t>Résolution:</t>
+  </si>
+  <si>
+    <t>dl_format_no_xlsx</t>
+  </si>
+  <si>
+    <t>Choose a format (.xlsx not available over 1 million rows)</t>
+  </si>
+  <si>
+    <t>Sélectionnez un format (.xlsx non disponible au-delà d'un million de lignes)</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1175,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="43">
+  <fills count="42">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1322,12 +1406,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1493,7 +1571,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -1505,7 +1583,6 @@
     <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="42" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1882,10 +1959,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D106"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2127,1165 +2204,1283 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>278</v>
       </c>
       <c r="B19" t="s">
-        <v>230</v>
+        <v>276</v>
       </c>
       <c r="C19" t="s">
-        <v>97</v>
+        <v>286</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>287</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>289</v>
+        <v>96</v>
       </c>
       <c r="B20" t="s">
-        <v>292</v>
+        <v>230</v>
       </c>
       <c r="C20" t="s">
-        <v>290</v>
+        <v>97</v>
       </c>
       <c r="D20" t="s">
-        <v>291</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="B21" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C21" t="s">
-        <v>303</v>
+        <v>289</v>
       </c>
       <c r="D21" t="s">
-        <v>304</v>
+        <v>290</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="B22" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C22" t="s">
         <v>296</v>
       </c>
       <c r="D22" t="s">
-        <v>301</v>
+        <v>331</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="B23" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C23" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="D23" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B24" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C24" t="s">
+        <v>327</v>
+      </c>
+      <c r="D24" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>294</v>
+      </c>
+      <c r="B25" t="s">
         <v>298</v>
       </c>
-      <c r="D24" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
+      <c r="C25" t="s">
+        <v>328</v>
+      </c>
+      <c r="D25" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>228</v>
+        <v>299</v>
       </c>
       <c r="B26" t="s">
-        <v>229</v>
+        <v>300</v>
       </c>
       <c r="C26" t="s">
-        <v>103</v>
+        <v>301</v>
       </c>
       <c r="D26" t="s">
-        <v>104</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>81</v>
+        <v>326</v>
       </c>
       <c r="B27" t="s">
-        <v>231</v>
+        <v>300</v>
       </c>
       <c r="C27" t="s">
-        <v>82</v>
+        <v>305</v>
       </c>
       <c r="D27" t="s">
-        <v>83</v>
+        <v>306</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>226</v>
+        <v>307</v>
       </c>
       <c r="B28" t="s">
-        <v>232</v>
+        <v>300</v>
       </c>
       <c r="C28" t="s">
-        <v>233</v>
+        <v>308</v>
       </c>
       <c r="D28" t="s">
-        <v>234</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>265</v>
+        <v>310</v>
       </c>
       <c r="B29" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="C29" t="s">
-        <v>269</v>
+        <v>311</v>
       </c>
       <c r="D29" t="s">
-        <v>270</v>
+        <v>312</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>267</v>
+        <v>314</v>
       </c>
       <c r="B30" t="s">
-        <v>266</v>
+        <v>297</v>
       </c>
       <c r="C30" t="s">
-        <v>286</v>
+        <v>315</v>
       </c>
       <c r="D30" t="s">
-        <v>286</v>
+        <v>316</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>280</v>
+        <v>332</v>
       </c>
       <c r="B31" t="s">
-        <v>278</v>
+        <v>297</v>
       </c>
       <c r="C31" t="s">
-        <v>281</v>
+        <v>333</v>
       </c>
       <c r="D31" t="s">
-        <v>282</v>
+        <v>334</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>283</v>
+        <v>317</v>
       </c>
       <c r="B32" t="s">
-        <v>278</v>
+        <v>298</v>
       </c>
       <c r="C32" t="s">
-        <v>284</v>
+        <v>319</v>
       </c>
       <c r="D32" t="s">
-        <v>285</v>
+        <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="A33" t="s">
+        <v>318</v>
+      </c>
+      <c r="B33" t="s">
+        <v>298</v>
+      </c>
+      <c r="C33" t="s">
+        <v>321</v>
+      </c>
+      <c r="D33" t="s">
+        <v>322</v>
+      </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>323</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>298</v>
       </c>
       <c r="C34" t="s">
-        <v>55</v>
+        <v>324</v>
       </c>
       <c r="D34" t="s">
-        <v>55</v>
+        <v>325</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
+      <c r="A35" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>228</v>
       </c>
       <c r="B36" t="s">
-        <v>48</v>
+        <v>229</v>
       </c>
       <c r="C36" t="s">
-        <v>57</v>
+        <v>103</v>
       </c>
       <c r="D36" t="s">
-        <v>57</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>106</v>
+        <v>231</v>
       </c>
       <c r="C37" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="D37" t="s">
-        <v>115</v>
+        <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>107</v>
+        <v>226</v>
       </c>
       <c r="B38" t="s">
-        <v>108</v>
+        <v>232</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>233</v>
       </c>
       <c r="D38" t="s">
-        <v>112</v>
+        <v>234</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>109</v>
+        <v>264</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>265</v>
       </c>
       <c r="C39" t="s">
-        <v>111</v>
+        <v>268</v>
       </c>
       <c r="D39" t="s">
-        <v>113</v>
+        <v>269</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>132</v>
+        <v>266</v>
       </c>
       <c r="B40" t="s">
-        <v>106</v>
+        <v>265</v>
       </c>
       <c r="C40" t="s">
-        <v>133</v>
+        <v>285</v>
       </c>
       <c r="D40" t="s">
-        <v>235</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>279</v>
       </c>
       <c r="B41" t="s">
-        <v>117</v>
+        <v>277</v>
       </c>
       <c r="C41" t="s">
-        <v>118</v>
+        <v>280</v>
       </c>
       <c r="D41" t="s">
-        <v>119</v>
+        <v>281</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" s="7"/>
-      <c r="C42" s="7"/>
-      <c r="D42" s="7"/>
+      <c r="A42" t="s">
+        <v>282</v>
+      </c>
+      <c r="B42" t="s">
+        <v>277</v>
+      </c>
+      <c r="C42" t="s">
+        <v>283</v>
+      </c>
+      <c r="D42" t="s">
+        <v>284</v>
+      </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>58</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="A43" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" t="s">
         <v>48</v>
       </c>
-      <c r="C43" t="s">
-        <v>59</v>
-      </c>
-      <c r="D43" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B44" s="11"/>
-      <c r="C44" s="11"/>
-      <c r="D44" s="11"/>
+      <c r="C44" t="s">
+        <v>55</v>
+      </c>
+      <c r="D44" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>279</v>
-      </c>
-      <c r="B45" t="s">
-        <v>277</v>
-      </c>
-      <c r="C45" t="s">
-        <v>287</v>
-      </c>
-      <c r="D45" t="s">
-        <v>288</v>
+      <c r="A45" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>56</v>
+      </c>
+      <c r="B46" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" t="s">
+        <v>57</v>
+      </c>
+      <c r="D46" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
+      <c r="A47" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C47" t="s">
+        <v>114</v>
+      </c>
+      <c r="D47" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>164</v>
+        <v>107</v>
       </c>
       <c r="B48" t="s">
-        <v>48</v>
+        <v>108</v>
       </c>
       <c r="C48" t="s">
-        <v>165</v>
+        <v>110</v>
       </c>
       <c r="D48" t="s">
-        <v>166</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>170</v>
+        <v>109</v>
       </c>
       <c r="B49" t="s">
-        <v>167</v>
+        <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>168</v>
+        <v>111</v>
       </c>
       <c r="D49" t="s">
-        <v>169</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>173</v>
+        <v>132</v>
       </c>
       <c r="B50" t="s">
-        <v>174</v>
+        <v>106</v>
       </c>
       <c r="C50" t="s">
-        <v>185</v>
+        <v>133</v>
       </c>
       <c r="D50" t="s">
-        <v>186</v>
+        <v>313</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>182</v>
+        <v>116</v>
       </c>
       <c r="B51" t="s">
-        <v>167</v>
+        <v>117</v>
       </c>
       <c r="C51" t="s">
-        <v>171</v>
+        <v>118</v>
       </c>
       <c r="D51" t="s">
-        <v>172</v>
+        <v>119</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>175</v>
-      </c>
-      <c r="B52" t="s">
-        <v>174</v>
-      </c>
-      <c r="C52" t="s">
-        <v>184</v>
-      </c>
-      <c r="D52" t="s">
-        <v>183</v>
-      </c>
+      <c r="A52" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>176</v>
+        <v>58</v>
       </c>
       <c r="B53" t="s">
-        <v>178</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>180</v>
+        <v>48</v>
+      </c>
+      <c r="C53" t="s">
+        <v>59</v>
+      </c>
+      <c r="D53" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>177</v>
-      </c>
-      <c r="B54" t="s">
-        <v>174</v>
-      </c>
-      <c r="C54" t="s">
-        <v>179</v>
-      </c>
-      <c r="D54" t="s">
-        <v>181</v>
-      </c>
+      <c r="A54" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B55" s="8"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="8"/>
+      <c r="A55" t="s">
+        <v>164</v>
+      </c>
+      <c r="B55" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" t="s">
+        <v>165</v>
+      </c>
+      <c r="D55" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>170</v>
       </c>
       <c r="B56" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
       <c r="C56" t="s">
-        <v>62</v>
+        <v>168</v>
       </c>
       <c r="D56" t="s">
-        <v>63</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>120</v>
+        <v>173</v>
       </c>
       <c r="B57" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="C57" t="s">
-        <v>121</v>
+        <v>185</v>
       </c>
       <c r="D57" t="s">
-        <v>122</v>
+        <v>186</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>64</v>
+        <v>182</v>
       </c>
       <c r="B58" t="s">
-        <v>9</v>
+        <v>167</v>
       </c>
       <c r="C58" t="s">
-        <v>65</v>
+        <v>171</v>
       </c>
       <c r="D58" t="s">
-        <v>66</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>67</v>
+        <v>175</v>
       </c>
       <c r="B59" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="C59" t="s">
-        <v>68</v>
+        <v>184</v>
       </c>
       <c r="D59" t="s">
-        <v>268</v>
+        <v>183</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>263</v>
+        <v>176</v>
       </c>
       <c r="B60" t="s">
-        <v>9</v>
-      </c>
-      <c r="C60" t="s">
-        <v>264</v>
-      </c>
-      <c r="D60" t="s">
-        <v>264</v>
+        <v>178</v>
+      </c>
+      <c r="C60" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="B61" t="s">
-        <v>9</v>
+        <v>174</v>
       </c>
       <c r="C61" t="s">
-        <v>70</v>
+        <v>179</v>
       </c>
       <c r="D61" t="s">
-        <v>71</v>
+        <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
-        <v>205</v>
-      </c>
-      <c r="B62" t="s">
-        <v>9</v>
-      </c>
-      <c r="C62" t="s">
-        <v>206</v>
-      </c>
-      <c r="D62" t="s">
-        <v>207</v>
-      </c>
+      <c r="A62" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
+      <c r="D62" s="8"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>210</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>9</v>
       </c>
       <c r="C63" t="s">
-        <v>208</v>
+        <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>209</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>191</v>
+        <v>120</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>192</v>
+        <v>121</v>
       </c>
       <c r="D64" t="s">
-        <v>193</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>202</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>203</v>
+        <v>65</v>
       </c>
       <c r="D65" t="s">
-        <v>204</v>
+        <v>66</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>217</v>
+        <v>67</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>218</v>
+        <v>68</v>
       </c>
       <c r="D66" t="s">
-        <v>219</v>
+        <v>267</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>189</v>
+        <v>262</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
       <c r="D67" t="s">
-        <v>237</v>
+        <v>263</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D68" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="D69" t="s">
-        <v>17</v>
+        <v>207</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="D70" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>75</v>
+        <v>191</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>76</v>
+        <v>192</v>
       </c>
       <c r="D71" t="s">
-        <v>77</v>
+        <v>193</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D72" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="B73" t="s">
         <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="D73" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>78</v>
+        <v>189</v>
       </c>
       <c r="B74" t="s">
         <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>79</v>
+        <v>235</v>
       </c>
       <c r="D74" t="s">
-        <v>80</v>
+        <v>236</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>197</v>
+        <v>72</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>195</v>
+        <v>73</v>
       </c>
       <c r="D75" t="s">
-        <v>196</v>
+        <v>74</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>221</v>
+        <v>194</v>
       </c>
       <c r="D76" t="s">
-        <v>222</v>
+        <v>17</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>240</v>
+        <v>211</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>238</v>
+        <v>212</v>
       </c>
       <c r="D77" t="s">
-        <v>239</v>
+        <v>213</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>241</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>242</v>
+        <v>76</v>
       </c>
       <c r="D78" t="s">
-        <v>134</v>
+        <v>77</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>243</v>
+        <v>198</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>244</v>
+        <v>200</v>
       </c>
       <c r="D79" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>84</v>
+        <v>214</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>85</v>
+        <v>215</v>
       </c>
       <c r="D80" t="s">
-        <v>86</v>
+        <v>216</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>8</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>10</v>
+        <v>79</v>
       </c>
       <c r="D81" t="s">
-        <v>11</v>
+        <v>80</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>246</v>
+        <v>197</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>246</v>
+        <v>195</v>
       </c>
       <c r="D82" t="s">
-        <v>247</v>
+        <v>196</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B83" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D83" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="D84" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B85" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="D85" t="s">
-        <v>253</v>
+        <v>134</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>275</v>
+        <v>242</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>271</v>
+        <v>243</v>
       </c>
       <c r="D86" t="s">
-        <v>273</v>
+        <v>244</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>276</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>272</v>
+        <v>85</v>
       </c>
       <c r="D87" t="s">
-        <v>274</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>257</v>
+        <v>8</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>259</v>
+        <v>10</v>
       </c>
       <c r="D88" t="s">
-        <v>261</v>
+        <v>11</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="B89" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
       <c r="D89" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>223</v>
       </c>
       <c r="B90" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="C90" t="s">
-        <v>136</v>
+        <v>223</v>
       </c>
       <c r="D90" t="s">
-        <v>137</v>
+        <v>225</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="D91" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>15</v>
+        <v>248</v>
       </c>
       <c r="B92" t="s">
+        <v>224</v>
+      </c>
+      <c r="C92" t="s">
+        <v>251</v>
+      </c>
+      <c r="D92" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>274</v>
+      </c>
+      <c r="B93" t="s">
         <v>9</v>
       </c>
-      <c r="C92" t="s">
-        <v>16</v>
-      </c>
-      <c r="D92" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A93" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B93" s="2"/>
-      <c r="C93" s="2"/>
-      <c r="D93" s="2"/>
+      <c r="C93" t="s">
+        <v>270</v>
+      </c>
+      <c r="D93" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>139</v>
+        <v>275</v>
       </c>
       <c r="B94" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
       <c r="C94" t="s">
-        <v>158</v>
+        <v>271</v>
       </c>
       <c r="D94" t="s">
-        <v>157</v>
+        <v>273</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>156</v>
+        <v>256</v>
       </c>
       <c r="B95" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>159</v>
+        <v>258</v>
       </c>
       <c r="D95" t="s">
-        <v>162</v>
+        <v>260</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>140</v>
+        <v>257</v>
       </c>
       <c r="B96" t="s">
-        <v>138</v>
+        <v>224</v>
       </c>
       <c r="C96" t="s">
-        <v>141</v>
+        <v>259</v>
       </c>
       <c r="D96" t="s">
-        <v>148</v>
+        <v>261</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B97" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="D97" t="s">
-        <v>147</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>142</v>
+        <v>253</v>
       </c>
       <c r="B98" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>143</v>
+        <v>254</v>
       </c>
       <c r="D98" t="s">
-        <v>144</v>
+        <v>255</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>149</v>
+        <v>15</v>
       </c>
       <c r="B99" t="s">
+        <v>9</v>
+      </c>
+      <c r="C99" t="s">
+        <v>16</v>
+      </c>
+      <c r="D99" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C99" t="s">
-        <v>161</v>
-      </c>
-      <c r="D99" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>151</v>
-      </c>
-      <c r="B100" t="s">
-        <v>138</v>
-      </c>
-      <c r="C100" t="s">
-        <v>160</v>
-      </c>
-      <c r="D100" t="s">
-        <v>152</v>
-      </c>
+      <c r="B100" s="2"/>
+      <c r="C100" s="2"/>
+      <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="B101" t="s">
         <v>138</v>
       </c>
       <c r="C101" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D101" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B102" s="4"/>
-      <c r="C102" s="4"/>
-      <c r="D102" s="4"/>
+      <c r="A102" t="s">
+        <v>156</v>
+      </c>
+      <c r="B102" t="s">
+        <v>138</v>
+      </c>
+      <c r="C102" t="s">
+        <v>159</v>
+      </c>
+      <c r="D102" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>87</v>
+        <v>140</v>
       </c>
       <c r="B103" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C103" t="s">
-        <v>89</v>
+        <v>141</v>
       </c>
       <c r="D103" t="s">
-        <v>90</v>
+        <v>148</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>91</v>
+        <v>145</v>
       </c>
       <c r="B104" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C104" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="D104" t="s">
-        <v>92</v>
+        <v>147</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>188</v>
+        <v>142</v>
       </c>
       <c r="B105" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C105" t="s">
-        <v>189</v>
+        <v>143</v>
       </c>
       <c r="D105" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
+        <v>149</v>
+      </c>
+      <c r="B106" t="s">
+        <v>138</v>
+      </c>
+      <c r="C106" t="s">
+        <v>161</v>
+      </c>
+      <c r="D106" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>151</v>
+      </c>
+      <c r="B107" t="s">
+        <v>138</v>
+      </c>
+      <c r="C107" t="s">
+        <v>160</v>
+      </c>
+      <c r="D107" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>153</v>
+      </c>
+      <c r="B108" t="s">
+        <v>138</v>
+      </c>
+      <c r="C108" t="s">
+        <v>154</v>
+      </c>
+      <c r="D108" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A109" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B109" s="4"/>
+      <c r="C109" s="4"/>
+      <c r="D109" s="4"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>87</v>
+      </c>
+      <c r="B110" t="s">
+        <v>88</v>
+      </c>
+      <c r="C110" t="s">
+        <v>89</v>
+      </c>
+      <c r="D110" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>91</v>
+      </c>
+      <c r="B111" t="s">
+        <v>88</v>
+      </c>
+      <c r="C111" t="s">
+        <v>69</v>
+      </c>
+      <c r="D111" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>188</v>
+      </c>
+      <c r="B112" t="s">
+        <v>88</v>
+      </c>
+      <c r="C112" t="s">
+        <v>189</v>
+      </c>
+      <c r="D112" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
         <v>93</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B113" t="s">
         <v>88</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C113" t="s">
         <v>94</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D113" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Data download works fully, just need filters working now!
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99F9CD95-1204-4DF7-B9F2-985240F37C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F7F79E-6F96-44ED-A038-DD81815483C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="342">
   <si>
     <t>id</t>
   </si>
@@ -1025,6 +1025,27 @@
   </si>
   <si>
     <t>Sélectionnez un format (.xlsx non disponible au-delà d'un million de lignes)</t>
+  </si>
+  <si>
+    <t>measurement_type</t>
+  </si>
+  <si>
+    <t>Measurement type (frequency)</t>
+  </si>
+  <si>
+    <t>Type de mesure (fréquence)</t>
+  </si>
+  <si>
+    <t>dl_prep</t>
+  </si>
+  <si>
+    <t>notification for download</t>
+  </si>
+  <si>
+    <t>Preparing download...</t>
+  </si>
+  <si>
+    <t>Préparation du téléchargement...</t>
   </si>
 </sst>
 </file>
@@ -1959,10 +1980,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2427,1060 +2448,1085 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="10" t="s">
+      <c r="A35" t="s">
+        <v>338</v>
+      </c>
+      <c r="B35" t="s">
+        <v>339</v>
+      </c>
+      <c r="C35" t="s">
+        <v>340</v>
+      </c>
+      <c r="D35" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>228</v>
-      </c>
-      <c r="B36" t="s">
-        <v>229</v>
-      </c>
-      <c r="C36" t="s">
-        <v>103</v>
-      </c>
-      <c r="D36" t="s">
-        <v>104</v>
-      </c>
+      <c r="B36" s="10"/>
+      <c r="C36" s="10"/>
+      <c r="D36" s="10"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>228</v>
       </c>
       <c r="B37" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="D37" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>226</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C38" t="s">
-        <v>233</v>
+        <v>82</v>
       </c>
       <c r="D38" t="s">
-        <v>234</v>
+        <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="B39" t="s">
-        <v>265</v>
+        <v>232</v>
       </c>
       <c r="C39" t="s">
-        <v>268</v>
+        <v>233</v>
       </c>
       <c r="D39" t="s">
-        <v>269</v>
+        <v>234</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B40" t="s">
         <v>265</v>
       </c>
       <c r="C40" t="s">
-        <v>285</v>
+        <v>268</v>
       </c>
       <c r="D40" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>279</v>
+        <v>266</v>
       </c>
       <c r="B41" t="s">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="C41" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="D41" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B42" t="s">
         <v>277</v>
       </c>
       <c r="C42" t="s">
+        <v>280</v>
+      </c>
+      <c r="D42" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>282</v>
+      </c>
+      <c r="B43" t="s">
+        <v>277</v>
+      </c>
+      <c r="C43" t="s">
         <v>283</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D43" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>54</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B45" t="s">
         <v>48</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C45" t="s">
         <v>55</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D45" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="6" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>56</v>
-      </c>
-      <c r="B46" t="s">
-        <v>48</v>
-      </c>
-      <c r="C46" t="s">
-        <v>57</v>
-      </c>
-      <c r="D46" t="s">
-        <v>57</v>
-      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>105</v>
+        <v>56</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>114</v>
+        <v>57</v>
       </c>
       <c r="D47" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B48" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C48" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="D48" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B49" t="s">
         <v>108</v>
       </c>
       <c r="C49" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D49" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>109</v>
       </c>
       <c r="B50" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="C50" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="D50" t="s">
-        <v>313</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>132</v>
+      </c>
+      <c r="B51" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" t="s">
+        <v>133</v>
+      </c>
+      <c r="D51" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
         <v>116</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>117</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>118</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" s="7" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" t="s">
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7"/>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
         <v>58</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B54" t="s">
         <v>48</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C54" t="s">
         <v>59</v>
       </c>
-      <c r="D53" t="s">
+      <c r="D54" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>164</v>
-      </c>
-      <c r="B55" t="s">
-        <v>48</v>
-      </c>
-      <c r="C55" t="s">
-        <v>165</v>
-      </c>
-      <c r="D55" t="s">
-        <v>166</v>
-      </c>
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="B56" t="s">
-        <v>167</v>
+        <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D56" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B57" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C57" t="s">
-        <v>185</v>
+        <v>168</v>
       </c>
       <c r="D57" t="s">
-        <v>186</v>
+        <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B58" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="C58" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="D58" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C59" t="s">
-        <v>184</v>
+        <v>171</v>
       </c>
       <c r="D59" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B60" t="s">
-        <v>178</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D60" s="9" t="s">
-        <v>180</v>
+        <v>174</v>
+      </c>
+      <c r="C60" t="s">
+        <v>184</v>
+      </c>
+      <c r="D60" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>176</v>
+      </c>
+      <c r="B61" t="s">
+        <v>178</v>
+      </c>
+      <c r="C61" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="D61" s="9" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
         <v>177</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B62" t="s">
         <v>174</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C62" t="s">
         <v>179</v>
       </c>
-      <c r="D61" t="s">
+      <c r="D62" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="8" t="s">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B62" s="8"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="8"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" t="s">
-        <v>61</v>
-      </c>
-      <c r="B63" t="s">
-        <v>9</v>
-      </c>
-      <c r="C63" t="s">
-        <v>62</v>
-      </c>
-      <c r="D63" t="s">
-        <v>63</v>
-      </c>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>120</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
         <v>9</v>
       </c>
       <c r="C64" t="s">
-        <v>121</v>
+        <v>62</v>
       </c>
       <c r="D64" t="s">
-        <v>122</v>
+        <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="B65" t="s">
         <v>9</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>121</v>
       </c>
       <c r="D65" t="s">
-        <v>66</v>
+        <v>122</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>9</v>
       </c>
       <c r="C66" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>267</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>262</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
         <v>9</v>
       </c>
       <c r="C67" t="s">
-        <v>263</v>
+        <v>68</v>
       </c>
       <c r="D67" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>262</v>
       </c>
       <c r="B68" t="s">
         <v>9</v>
       </c>
       <c r="C68" t="s">
-        <v>70</v>
+        <v>263</v>
       </c>
       <c r="D68" t="s">
-        <v>71</v>
+        <v>263</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>205</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
         <v>9</v>
       </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>70</v>
       </c>
       <c r="D69" t="s">
-        <v>207</v>
+        <v>71</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B70" t="s">
         <v>9</v>
       </c>
       <c r="C70" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D70" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="B71" t="s">
         <v>9</v>
       </c>
       <c r="C71" t="s">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="D71" t="s">
-        <v>193</v>
+        <v>209</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="B72" t="s">
         <v>9</v>
       </c>
       <c r="C72" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="D72" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>217</v>
+        <v>202</v>
       </c>
       <c r="B73" t="s">
         <v>9</v>
       </c>
       <c r="C73" t="s">
-        <v>218</v>
+        <v>203</v>
       </c>
       <c r="D73" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>189</v>
+        <v>217</v>
       </c>
       <c r="B74" t="s">
         <v>9</v>
       </c>
       <c r="C74" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="D74" t="s">
-        <v>236</v>
+        <v>219</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>189</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>73</v>
+        <v>235</v>
       </c>
       <c r="D75" t="s">
-        <v>74</v>
+        <v>236</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>199</v>
+        <v>72</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>194</v>
+        <v>73</v>
       </c>
       <c r="D76" t="s">
-        <v>17</v>
+        <v>74</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>212</v>
+        <v>194</v>
       </c>
       <c r="D77" t="s">
-        <v>213</v>
+        <v>17</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>211</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>76</v>
+        <v>212</v>
       </c>
       <c r="D78" t="s">
-        <v>77</v>
+        <v>213</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>198</v>
+        <v>75</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>200</v>
+        <v>76</v>
       </c>
       <c r="D79" t="s">
-        <v>201</v>
+        <v>77</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>215</v>
+        <v>200</v>
       </c>
       <c r="D80" t="s">
-        <v>216</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>78</v>
+        <v>214</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>79</v>
+        <v>215</v>
       </c>
       <c r="D81" t="s">
-        <v>80</v>
+        <v>216</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>197</v>
+        <v>78</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>195</v>
+        <v>79</v>
       </c>
       <c r="D82" t="s">
-        <v>196</v>
+        <v>80</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>221</v>
+        <v>195</v>
       </c>
       <c r="D83" t="s">
-        <v>222</v>
+        <v>196</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="D84" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="D85" t="s">
-        <v>134</v>
+        <v>238</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D86" t="s">
-        <v>244</v>
+        <v>134</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>84</v>
+        <v>242</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>85</v>
+        <v>243</v>
       </c>
       <c r="D87" t="s">
-        <v>86</v>
+        <v>244</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>8</v>
-      </c>
-      <c r="B88" t="s">
-        <v>9</v>
+        <v>335</v>
       </c>
       <c r="C88" t="s">
-        <v>10</v>
+        <v>336</v>
       </c>
       <c r="D88" t="s">
-        <v>11</v>
+        <v>337</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>245</v>
+        <v>84</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>245</v>
+        <v>85</v>
       </c>
       <c r="D89" t="s">
-        <v>246</v>
+        <v>86</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>223</v>
+        <v>8</v>
       </c>
       <c r="B90" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>223</v>
+        <v>10</v>
       </c>
       <c r="D90" t="s">
-        <v>225</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D91" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>248</v>
+        <v>223</v>
       </c>
       <c r="B92" t="s">
         <v>224</v>
       </c>
       <c r="C92" t="s">
-        <v>251</v>
+        <v>223</v>
       </c>
       <c r="D92" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>274</v>
+        <v>247</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>270</v>
+        <v>249</v>
       </c>
       <c r="D93" t="s">
-        <v>272</v>
+        <v>250</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>275</v>
+        <v>248</v>
       </c>
       <c r="B94" t="s">
         <v>224</v>
       </c>
       <c r="C94" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="D94" t="s">
-        <v>273</v>
+        <v>252</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="D95" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>257</v>
+        <v>275</v>
       </c>
       <c r="B96" t="s">
         <v>224</v>
       </c>
       <c r="C96" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="D96" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>135</v>
+        <v>256</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>136</v>
+        <v>258</v>
       </c>
       <c r="D97" t="s">
-        <v>137</v>
+        <v>260</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>253</v>
+        <v>257</v>
       </c>
       <c r="B98" t="s">
-        <v>9</v>
+        <v>224</v>
       </c>
       <c r="C98" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="D98" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>15</v>
+        <v>135</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>16</v>
+        <v>136</v>
       </c>
       <c r="D99" t="s">
-        <v>17</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A100" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B100" s="2"/>
-      <c r="C100" s="2"/>
-      <c r="D100" s="2"/>
+      <c r="A100" t="s">
+        <v>253</v>
+      </c>
+      <c r="B100" t="s">
+        <v>9</v>
+      </c>
+      <c r="C100" t="s">
+        <v>254</v>
+      </c>
+      <c r="D100" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>139</v>
+        <v>15</v>
       </c>
       <c r="B101" t="s">
+        <v>9</v>
+      </c>
+      <c r="C101" t="s">
+        <v>16</v>
+      </c>
+      <c r="D101" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="C101" t="s">
-        <v>158</v>
-      </c>
-      <c r="D101" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>156</v>
-      </c>
-      <c r="B102" t="s">
-        <v>138</v>
-      </c>
-      <c r="C102" t="s">
-        <v>159</v>
-      </c>
-      <c r="D102" t="s">
-        <v>162</v>
-      </c>
+      <c r="B102" s="2"/>
+      <c r="C102" s="2"/>
+      <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B103" t="s">
         <v>138</v>
       </c>
       <c r="C103" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="D103" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B104" t="s">
         <v>138</v>
       </c>
       <c r="C104" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="D104" t="s">
-        <v>147</v>
+        <v>162</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B105" t="s">
         <v>138</v>
       </c>
       <c r="C105" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D105" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="B106" t="s">
         <v>138</v>
       </c>
       <c r="C106" t="s">
-        <v>161</v>
+        <v>146</v>
       </c>
       <c r="D106" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="B107" t="s">
         <v>138</v>
       </c>
       <c r="C107" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="D107" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="B108" t="s">
         <v>138</v>
       </c>
       <c r="C108" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="D108" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B109" s="4"/>
-      <c r="C109" s="4"/>
-      <c r="D109" s="4"/>
+      <c r="A109" t="s">
+        <v>151</v>
+      </c>
+      <c r="B109" t="s">
+        <v>138</v>
+      </c>
+      <c r="C109" t="s">
+        <v>160</v>
+      </c>
+      <c r="D109" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="B110" t="s">
-        <v>88</v>
+        <v>138</v>
       </c>
       <c r="C110" t="s">
-        <v>89</v>
+        <v>154</v>
       </c>
       <c r="D110" t="s">
-        <v>90</v>
+        <v>155</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" t="s">
-        <v>91</v>
-      </c>
-      <c r="B111" t="s">
-        <v>88</v>
-      </c>
-      <c r="C111" t="s">
-        <v>69</v>
-      </c>
-      <c r="D111" t="s">
-        <v>92</v>
-      </c>
+      <c r="A111" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B111" s="4"/>
+      <c r="C111" s="4"/>
+      <c r="D111" s="4"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>188</v>
+        <v>87</v>
       </c>
       <c r="B112" t="s">
         <v>88</v>
       </c>
       <c r="C112" t="s">
-        <v>189</v>
+        <v>89</v>
       </c>
       <c r="D112" t="s">
-        <v>190</v>
+        <v>90</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B113" t="s">
         <v>88</v>
       </c>
       <c r="C113" t="s">
+        <v>69</v>
+      </c>
+      <c r="D113" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>188</v>
+      </c>
+      <c r="B114" t="s">
+        <v>88</v>
+      </c>
+      <c r="C114" t="s">
+        <v>189</v>
+      </c>
+      <c r="D114" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>93</v>
+      </c>
+      <c r="B115" t="s">
+        <v>88</v>
+      </c>
+      <c r="C115" t="s">
         <v>94</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D115" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
make login button and modal multi-lingual
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F7F79E-6F96-44ED-A038-DD81815483C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F12CAD-2348-46A3-8D9F-88F33A7170E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="379">
   <si>
     <t>id</t>
   </si>
@@ -1046,6 +1046,117 @@
   </si>
   <si>
     <t>Préparation du téléchargement...</t>
+  </si>
+  <si>
+    <t>login_txt</t>
+  </si>
+  <si>
+    <t>Login pop-up</t>
+  </si>
+  <si>
+    <t>Body text for pop-up</t>
+  </si>
+  <si>
+    <t>Reserved for partner organizations/individuals. Contact us if you think you should have access.</t>
+  </si>
+  <si>
+    <t>Réservé pour les partenaires. Contactez-nous si vous pensez avoir besoin d'accès.</t>
+  </si>
+  <si>
+    <t>un</t>
+  </si>
+  <si>
+    <t>pwd</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Nom d'utilisateur</t>
+  </si>
+  <si>
+    <t>Mot de passe</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>login_success</t>
+  </si>
+  <si>
+    <t>You are now logged in as</t>
+  </si>
+  <si>
+    <t>login_fail</t>
+  </si>
+  <si>
+    <t>Username or password failed.</t>
+  </si>
+  <si>
+    <t>login_success_msg</t>
+  </si>
+  <si>
+    <t>login_fail_msg</t>
+  </si>
+  <si>
+    <t>modal title</t>
+  </si>
+  <si>
+    <t>modal text</t>
+  </si>
+  <si>
+    <t>Nom d'utilisateur ou du mot de passe non reconnu.</t>
+  </si>
+  <si>
+    <t>Login successful</t>
+  </si>
+  <si>
+    <t>Connecté</t>
+  </si>
+  <si>
+    <t>Vous êtes maintenant connecté sous le nom d'utilisateur</t>
+  </si>
+  <si>
+    <t>Échec</t>
+  </si>
+  <si>
+    <t>Login failed</t>
+  </si>
+  <si>
+    <t>login_close</t>
+  </si>
+  <si>
+    <t>modal actionButton text</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Fermer</t>
+  </si>
+  <si>
+    <t>login_fail_attempts</t>
+  </si>
+  <si>
+    <t>Too many login attempts. Please try again later.</t>
+  </si>
+  <si>
+    <t>Trop d'essais, essayez plus tard.</t>
+  </si>
+  <si>
+    <t>login_confirm</t>
+  </si>
+  <si>
+    <t>Log in</t>
+  </si>
+  <si>
+    <t>Connection</t>
   </si>
 </sst>
 </file>
@@ -1980,22 +2091,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D115"/>
+  <dimension ref="A1:D126"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.109375" customWidth="1"/>
+    <col min="1" max="1" width="29.140625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="43.5546875" customWidth="1"/>
-    <col min="4" max="4" width="49.88671875" customWidth="1"/>
-    <col min="5" max="5" width="54.44140625" customWidth="1"/>
+    <col min="3" max="3" width="43.5703125" customWidth="1"/>
+    <col min="4" max="4" width="49.85546875" customWidth="1"/>
+    <col min="5" max="5" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2009,7 +2120,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -2023,7 +2134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -2037,7 +2148,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>131</v>
       </c>
@@ -2045,7 +2156,7 @@
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -2059,7 +2170,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>18</v>
       </c>
@@ -2073,7 +2184,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2087,7 +2198,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2101,7 +2212,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -2115,7 +2226,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>33</v>
       </c>
@@ -2129,7 +2240,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>37</v>
       </c>
@@ -2143,1390 +2254,1538 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>342</v>
+      </c>
+      <c r="B13" t="s">
+        <v>344</v>
+      </c>
+      <c r="C13" t="s">
+        <v>345</v>
+      </c>
+      <c r="D13" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>347</v>
+      </c>
+      <c r="B14" t="s">
+        <v>349</v>
+      </c>
+      <c r="C14" t="s">
+        <v>350</v>
+      </c>
+      <c r="D14" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" t="s">
+        <v>354</v>
+      </c>
+      <c r="C15" t="s">
+        <v>353</v>
+      </c>
+      <c r="D15" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" t="s">
+        <v>361</v>
+      </c>
+      <c r="C16" t="s">
+        <v>364</v>
+      </c>
+      <c r="D16" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>359</v>
+      </c>
+      <c r="B17" t="s">
+        <v>362</v>
+      </c>
+      <c r="C17" t="s">
+        <v>356</v>
+      </c>
+      <c r="D17" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>357</v>
+      </c>
+      <c r="B18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C18" t="s">
+        <v>368</v>
+      </c>
+      <c r="D18" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B19" t="s">
+        <v>362</v>
+      </c>
+      <c r="C19" t="s">
+        <v>358</v>
+      </c>
+      <c r="D19" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>373</v>
+      </c>
+      <c r="B20" t="s">
+        <v>362</v>
+      </c>
+      <c r="C20" t="s">
+        <v>374</v>
+      </c>
+      <c r="D20" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>376</v>
+      </c>
+      <c r="B21" t="s">
+        <v>370</v>
+      </c>
+      <c r="C21" t="s">
+        <v>377</v>
+      </c>
+      <c r="D21" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>369</v>
+      </c>
+      <c r="B22" t="s">
+        <v>370</v>
+      </c>
+      <c r="C22" t="s">
+        <v>371</v>
+      </c>
+      <c r="D22" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B24" t="s">
         <v>41</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C24" t="s">
         <v>187</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D24" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>43</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B25" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C25" t="s">
         <v>45</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D25" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B27" t="s">
         <v>48</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C27" t="s">
         <v>49</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="B28" s="4"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>51</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C29" t="s">
         <v>52</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D29" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>278</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B30" t="s">
         <v>276</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C30" t="s">
         <v>286</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D30" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>96</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B31" t="s">
         <v>230</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C31" t="s">
         <v>97</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D31" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>288</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B32" t="s">
         <v>291</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C32" t="s">
         <v>289</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D32" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>295</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B33" t="s">
         <v>297</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C33" t="s">
         <v>296</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D33" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>292</v>
-      </c>
-      <c r="B23" t="s">
-        <v>298</v>
-      </c>
-      <c r="C23" t="s">
-        <v>303</v>
-      </c>
-      <c r="D23" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>293</v>
-      </c>
-      <c r="B24" t="s">
-        <v>298</v>
-      </c>
-      <c r="C24" t="s">
-        <v>327</v>
-      </c>
-      <c r="D24" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>294</v>
-      </c>
-      <c r="B25" t="s">
-        <v>298</v>
-      </c>
-      <c r="C25" t="s">
-        <v>328</v>
-      </c>
-      <c r="D25" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>299</v>
-      </c>
-      <c r="B26" t="s">
-        <v>300</v>
-      </c>
-      <c r="C26" t="s">
-        <v>301</v>
-      </c>
-      <c r="D26" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>326</v>
-      </c>
-      <c r="B27" t="s">
-        <v>300</v>
-      </c>
-      <c r="C27" t="s">
-        <v>305</v>
-      </c>
-      <c r="D27" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>307</v>
-      </c>
-      <c r="B28" t="s">
-        <v>300</v>
-      </c>
-      <c r="C28" t="s">
-        <v>308</v>
-      </c>
-      <c r="D28" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>310</v>
-      </c>
-      <c r="B29" t="s">
-        <v>297</v>
-      </c>
-      <c r="C29" t="s">
-        <v>311</v>
-      </c>
-      <c r="D29" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>314</v>
-      </c>
-      <c r="B30" t="s">
-        <v>297</v>
-      </c>
-      <c r="C30" t="s">
-        <v>315</v>
-      </c>
-      <c r="D30" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>332</v>
-      </c>
-      <c r="B31" t="s">
-        <v>297</v>
-      </c>
-      <c r="C31" t="s">
-        <v>333</v>
-      </c>
-      <c r="D31" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>317</v>
-      </c>
-      <c r="B32" t="s">
-        <v>298</v>
-      </c>
-      <c r="C32" t="s">
-        <v>319</v>
-      </c>
-      <c r="D32" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>318</v>
-      </c>
-      <c r="B33" t="s">
-        <v>298</v>
-      </c>
-      <c r="C33" t="s">
-        <v>321</v>
-      </c>
-      <c r="D33" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>323</v>
       </c>
       <c r="B34" t="s">
         <v>298</v>
       </c>
       <c r="C34" t="s">
+        <v>303</v>
+      </c>
+      <c r="D34" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>293</v>
+      </c>
+      <c r="B35" t="s">
+        <v>298</v>
+      </c>
+      <c r="C35" t="s">
+        <v>327</v>
+      </c>
+      <c r="D35" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>294</v>
+      </c>
+      <c r="B36" t="s">
+        <v>298</v>
+      </c>
+      <c r="C36" t="s">
+        <v>328</v>
+      </c>
+      <c r="D36" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>299</v>
+      </c>
+      <c r="B37" t="s">
+        <v>300</v>
+      </c>
+      <c r="C37" t="s">
+        <v>301</v>
+      </c>
+      <c r="D37" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>326</v>
+      </c>
+      <c r="B38" t="s">
+        <v>300</v>
+      </c>
+      <c r="C38" t="s">
+        <v>305</v>
+      </c>
+      <c r="D38" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>307</v>
+      </c>
+      <c r="B39" t="s">
+        <v>300</v>
+      </c>
+      <c r="C39" t="s">
+        <v>308</v>
+      </c>
+      <c r="D39" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>310</v>
+      </c>
+      <c r="B40" t="s">
+        <v>297</v>
+      </c>
+      <c r="C40" t="s">
+        <v>311</v>
+      </c>
+      <c r="D40" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>314</v>
+      </c>
+      <c r="B41" t="s">
+        <v>297</v>
+      </c>
+      <c r="C41" t="s">
+        <v>315</v>
+      </c>
+      <c r="D41" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>332</v>
+      </c>
+      <c r="B42" t="s">
+        <v>297</v>
+      </c>
+      <c r="C42" t="s">
+        <v>333</v>
+      </c>
+      <c r="D42" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>317</v>
+      </c>
+      <c r="B43" t="s">
+        <v>298</v>
+      </c>
+      <c r="C43" t="s">
+        <v>319</v>
+      </c>
+      <c r="D43" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>318</v>
+      </c>
+      <c r="B44" t="s">
+        <v>298</v>
+      </c>
+      <c r="C44" t="s">
+        <v>321</v>
+      </c>
+      <c r="D44" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>323</v>
+      </c>
+      <c r="B45" t="s">
+        <v>298</v>
+      </c>
+      <c r="C45" t="s">
         <v>324</v>
       </c>
-      <c r="D34" t="s">
+      <c r="D45" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>338</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B46" t="s">
         <v>339</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C46" t="s">
         <v>340</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D46" t="s">
         <v>341</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="10" t="s">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="10"/>
-      <c r="D36" s="10"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
+      <c r="B47" s="10"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>228</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B48" t="s">
         <v>229</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C48" t="s">
         <v>103</v>
       </c>
-      <c r="D37" t="s">
+      <c r="D48" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>81</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B49" t="s">
         <v>231</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C49" t="s">
         <v>82</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D49" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>226</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B50" t="s">
         <v>232</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C50" t="s">
         <v>233</v>
       </c>
-      <c r="D39" t="s">
+      <c r="D50" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>264</v>
       </c>
-      <c r="B40" t="s">
+      <c r="B51" t="s">
         <v>265</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C51" t="s">
         <v>268</v>
       </c>
-      <c r="D40" t="s">
+      <c r="D51" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>266</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B52" t="s">
         <v>265</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C52" t="s">
         <v>285</v>
       </c>
-      <c r="D41" t="s">
+      <c r="D52" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>279</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B53" t="s">
         <v>277</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C53" t="s">
         <v>280</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D53" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>282</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B54" t="s">
         <v>277</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C54" t="s">
         <v>283</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D54" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>54</v>
-      </c>
-      <c r="B45" t="s">
-        <v>48</v>
-      </c>
-      <c r="C45" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>56</v>
-      </c>
-      <c r="B47" t="s">
-        <v>48</v>
-      </c>
-      <c r="C47" t="s">
-        <v>57</v>
-      </c>
-      <c r="D47" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>105</v>
-      </c>
-      <c r="B48" t="s">
-        <v>106</v>
-      </c>
-      <c r="C48" t="s">
-        <v>114</v>
-      </c>
-      <c r="D48" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>107</v>
-      </c>
-      <c r="B49" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49" t="s">
-        <v>110</v>
-      </c>
-      <c r="D49" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>109</v>
-      </c>
-      <c r="B50" t="s">
-        <v>108</v>
-      </c>
-      <c r="C50" t="s">
-        <v>111</v>
-      </c>
-      <c r="D50" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>132</v>
-      </c>
-      <c r="B51" t="s">
-        <v>106</v>
-      </c>
-      <c r="C51" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>116</v>
-      </c>
-      <c r="B52" t="s">
-        <v>117</v>
-      </c>
-      <c r="C52" t="s">
-        <v>118</v>
-      </c>
-      <c r="D52" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" t="s">
-        <v>48</v>
-      </c>
-      <c r="C54" t="s">
-        <v>59</v>
-      </c>
-      <c r="D54" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" t="s">
-        <v>164</v>
       </c>
       <c r="B56" t="s">
         <v>48</v>
       </c>
       <c r="C56" t="s">
+        <v>55</v>
+      </c>
+      <c r="D56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C58" t="s">
+        <v>57</v>
+      </c>
+      <c r="D58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>105</v>
+      </c>
+      <c r="B59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C59" t="s">
+        <v>114</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" t="s">
+        <v>108</v>
+      </c>
+      <c r="C60" t="s">
+        <v>110</v>
+      </c>
+      <c r="D60" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" t="s">
+        <v>108</v>
+      </c>
+      <c r="C61" t="s">
+        <v>111</v>
+      </c>
+      <c r="D61" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>132</v>
+      </c>
+      <c r="B62" t="s">
+        <v>106</v>
+      </c>
+      <c r="C62" t="s">
+        <v>133</v>
+      </c>
+      <c r="D62" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>116</v>
+      </c>
+      <c r="B63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C63" t="s">
+        <v>118</v>
+      </c>
+      <c r="D63" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="7"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" t="s">
+        <v>48</v>
+      </c>
+      <c r="C65" t="s">
+        <v>59</v>
+      </c>
+      <c r="D65" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B66" s="4"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>164</v>
+      </c>
+      <c r="B67" t="s">
+        <v>48</v>
+      </c>
+      <c r="C67" t="s">
         <v>165</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D67" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
         <v>170</v>
       </c>
-      <c r="B57" t="s">
+      <c r="B68" t="s">
         <v>167</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C68" t="s">
         <v>168</v>
       </c>
-      <c r="D57" t="s">
+      <c r="D68" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
         <v>173</v>
       </c>
-      <c r="B58" t="s">
+      <c r="B69" t="s">
         <v>174</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C69" t="s">
         <v>185</v>
       </c>
-      <c r="D58" t="s">
+      <c r="D69" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
         <v>182</v>
       </c>
-      <c r="B59" t="s">
+      <c r="B70" t="s">
         <v>167</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C70" t="s">
         <v>171</v>
       </c>
-      <c r="D59" t="s">
+      <c r="D70" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
         <v>175</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B71" t="s">
         <v>174</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C71" t="s">
         <v>184</v>
       </c>
-      <c r="D60" t="s">
+      <c r="D71" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
         <v>176</v>
       </c>
-      <c r="B61" t="s">
+      <c r="B72" t="s">
         <v>178</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C72" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D72" s="9" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
         <v>177</v>
       </c>
-      <c r="B62" t="s">
+      <c r="B73" t="s">
         <v>174</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C73" t="s">
         <v>179</v>
       </c>
-      <c r="D62" t="s">
+      <c r="D73" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="8" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="B63" s="8"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="8"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" t="s">
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
+      <c r="D74" s="8"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>61</v>
-      </c>
-      <c r="B64" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" t="s">
-        <v>62</v>
-      </c>
-      <c r="D64" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>120</v>
-      </c>
-      <c r="B65" t="s">
-        <v>9</v>
-      </c>
-      <c r="C65" t="s">
-        <v>121</v>
-      </c>
-      <c r="D65" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" t="s">
-        <v>64</v>
-      </c>
-      <c r="B66" t="s">
-        <v>9</v>
-      </c>
-      <c r="C66" t="s">
-        <v>65</v>
-      </c>
-      <c r="D66" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>67</v>
-      </c>
-      <c r="B67" t="s">
-        <v>9</v>
-      </c>
-      <c r="C67" t="s">
-        <v>68</v>
-      </c>
-      <c r="D67" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" t="s">
-        <v>262</v>
-      </c>
-      <c r="B68" t="s">
-        <v>9</v>
-      </c>
-      <c r="C68" t="s">
-        <v>263</v>
-      </c>
-      <c r="D68" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" t="s">
-        <v>69</v>
-      </c>
-      <c r="B69" t="s">
-        <v>9</v>
-      </c>
-      <c r="C69" t="s">
-        <v>70</v>
-      </c>
-      <c r="D69" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" t="s">
-        <v>205</v>
-      </c>
-      <c r="B70" t="s">
-        <v>9</v>
-      </c>
-      <c r="C70" t="s">
-        <v>206</v>
-      </c>
-      <c r="D70" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>210</v>
-      </c>
-      <c r="B71" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" t="s">
-        <v>208</v>
-      </c>
-      <c r="D71" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" t="s">
-        <v>191</v>
-      </c>
-      <c r="B72" t="s">
-        <v>9</v>
-      </c>
-      <c r="C72" t="s">
-        <v>192</v>
-      </c>
-      <c r="D72" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>202</v>
-      </c>
-      <c r="B73" t="s">
-        <v>9</v>
-      </c>
-      <c r="C73" t="s">
-        <v>203</v>
-      </c>
-      <c r="D73" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>217</v>
-      </c>
-      <c r="B74" t="s">
-        <v>9</v>
-      </c>
-      <c r="C74" t="s">
-        <v>218</v>
-      </c>
-      <c r="D74" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>189</v>
       </c>
       <c r="B75" t="s">
         <v>9</v>
       </c>
       <c r="C75" t="s">
-        <v>235</v>
+        <v>62</v>
       </c>
       <c r="D75" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>72</v>
+        <v>120</v>
       </c>
       <c r="B76" t="s">
         <v>9</v>
       </c>
       <c r="C76" t="s">
-        <v>73</v>
+        <v>121</v>
       </c>
       <c r="D76" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>199</v>
+        <v>64</v>
       </c>
       <c r="B77" t="s">
         <v>9</v>
       </c>
       <c r="C77" t="s">
-        <v>194</v>
+        <v>65</v>
       </c>
       <c r="D77" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>211</v>
+        <v>67</v>
       </c>
       <c r="B78" t="s">
         <v>9</v>
       </c>
       <c r="C78" t="s">
-        <v>212</v>
+        <v>68</v>
       </c>
       <c r="D78" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>75</v>
+        <v>262</v>
       </c>
       <c r="B79" t="s">
         <v>9</v>
       </c>
       <c r="C79" t="s">
-        <v>76</v>
+        <v>263</v>
       </c>
       <c r="D79" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>198</v>
+        <v>69</v>
       </c>
       <c r="B80" t="s">
         <v>9</v>
       </c>
       <c r="C80" t="s">
-        <v>200</v>
+        <v>70</v>
       </c>
       <c r="D80" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B81" t="s">
         <v>9</v>
       </c>
       <c r="C81" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="D81" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>78</v>
+        <v>210</v>
       </c>
       <c r="B82" t="s">
         <v>9</v>
       </c>
       <c r="C82" t="s">
-        <v>79</v>
+        <v>208</v>
       </c>
       <c r="D82" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="B83" t="s">
         <v>9</v>
       </c>
       <c r="C83" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D83" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>220</v>
+        <v>202</v>
       </c>
       <c r="B84" t="s">
         <v>9</v>
       </c>
       <c r="C84" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="D84" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>239</v>
+        <v>217</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="D85" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>240</v>
+        <v>189</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="D86" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>242</v>
+        <v>72</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>243</v>
+        <v>73</v>
       </c>
       <c r="D87" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>335</v>
+        <v>199</v>
+      </c>
+      <c r="B88" t="s">
+        <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>336</v>
+        <v>194</v>
       </c>
       <c r="D88" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>84</v>
+        <v>211</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>85</v>
+        <v>212</v>
       </c>
       <c r="D89" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>8</v>
+        <v>75</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>10</v>
+        <v>76</v>
       </c>
       <c r="D90" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>245</v>
+        <v>198</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>245</v>
+        <v>200</v>
       </c>
       <c r="D91" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="B92" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
       <c r="D92" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>247</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>249</v>
+        <v>79</v>
       </c>
       <c r="D93" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
       <c r="B94" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>251</v>
+        <v>195</v>
       </c>
       <c r="D94" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>274</v>
+        <v>220</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>270</v>
+        <v>221</v>
       </c>
       <c r="D95" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="B96" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>271</v>
+        <v>237</v>
       </c>
       <c r="D96" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>258</v>
+        <v>241</v>
       </c>
       <c r="D97" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="B98" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="D98" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>135</v>
-      </c>
-      <c r="B99" t="s">
-        <v>9</v>
+        <v>335</v>
       </c>
       <c r="C99" t="s">
-        <v>136</v>
+        <v>336</v>
       </c>
       <c r="D99" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>253</v>
+        <v>84</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>254</v>
+        <v>85</v>
       </c>
       <c r="D100" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="C101" t="s">
+        <v>10</v>
+      </c>
+      <c r="D101" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>245</v>
+      </c>
+      <c r="B102" t="s">
+        <v>9</v>
+      </c>
+      <c r="C102" t="s">
+        <v>245</v>
+      </c>
+      <c r="D102" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>223</v>
+      </c>
+      <c r="B103" t="s">
+        <v>224</v>
+      </c>
+      <c r="C103" t="s">
+        <v>223</v>
+      </c>
+      <c r="D103" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>247</v>
+      </c>
+      <c r="B104" t="s">
+        <v>9</v>
+      </c>
+      <c r="C104" t="s">
+        <v>249</v>
+      </c>
+      <c r="D104" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>248</v>
+      </c>
+      <c r="B105" t="s">
+        <v>224</v>
+      </c>
+      <c r="C105" t="s">
+        <v>251</v>
+      </c>
+      <c r="D105" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>274</v>
+      </c>
+      <c r="B106" t="s">
+        <v>9</v>
+      </c>
+      <c r="C106" t="s">
+        <v>270</v>
+      </c>
+      <c r="D106" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>275</v>
+      </c>
+      <c r="B107" t="s">
+        <v>224</v>
+      </c>
+      <c r="C107" t="s">
+        <v>271</v>
+      </c>
+      <c r="D107" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>256</v>
+      </c>
+      <c r="B108" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108" t="s">
+        <v>258</v>
+      </c>
+      <c r="D108" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>257</v>
+      </c>
+      <c r="B109" t="s">
+        <v>224</v>
+      </c>
+      <c r="C109" t="s">
+        <v>259</v>
+      </c>
+      <c r="D109" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>135</v>
+      </c>
+      <c r="B110" t="s">
+        <v>9</v>
+      </c>
+      <c r="C110" t="s">
+        <v>136</v>
+      </c>
+      <c r="D110" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>253</v>
+      </c>
+      <c r="B111" t="s">
+        <v>9</v>
+      </c>
+      <c r="C111" t="s">
+        <v>254</v>
+      </c>
+      <c r="D111" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" t="s">
+        <v>15</v>
+      </c>
+      <c r="B112" t="s">
+        <v>9</v>
+      </c>
+      <c r="C112" t="s">
         <v>16</v>
       </c>
-      <c r="D101" t="s">
+      <c r="D112" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A102" s="2" t="s">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="B102" s="2"/>
-      <c r="C102" s="2"/>
-      <c r="D102" s="2"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
+      <c r="B113" s="2"/>
+      <c r="C113" s="2"/>
+      <c r="D113" s="2"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
         <v>139</v>
       </c>
-      <c r="B103" t="s">
+      <c r="B114" t="s">
         <v>138</v>
       </c>
-      <c r="C103" t="s">
+      <c r="C114" t="s">
         <v>158</v>
       </c>
-      <c r="D103" t="s">
+      <c r="D114" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115" t="s">
         <v>156</v>
       </c>
-      <c r="B104" t="s">
+      <c r="B115" t="s">
         <v>138</v>
       </c>
-      <c r="C104" t="s">
+      <c r="C115" t="s">
         <v>159</v>
       </c>
-      <c r="D104" t="s">
+      <c r="D115" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116" t="s">
         <v>140</v>
       </c>
-      <c r="B105" t="s">
+      <c r="B116" t="s">
         <v>138</v>
       </c>
-      <c r="C105" t="s">
+      <c r="C116" t="s">
         <v>141</v>
       </c>
-      <c r="D105" t="s">
+      <c r="D116" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117" t="s">
         <v>145</v>
       </c>
-      <c r="B106" t="s">
+      <c r="B117" t="s">
         <v>138</v>
       </c>
-      <c r="C106" t="s">
+      <c r="C117" t="s">
         <v>146</v>
       </c>
-      <c r="D106" t="s">
+      <c r="D117" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A118" t="s">
         <v>142</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B118" t="s">
         <v>138</v>
       </c>
-      <c r="C107" t="s">
+      <c r="C118" t="s">
         <v>143</v>
       </c>
-      <c r="D107" t="s">
+      <c r="D118" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" t="s">
         <v>149</v>
       </c>
-      <c r="B108" t="s">
+      <c r="B119" t="s">
         <v>138</v>
       </c>
-      <c r="C108" t="s">
+      <c r="C119" t="s">
         <v>161</v>
       </c>
-      <c r="D108" t="s">
+      <c r="D119" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
         <v>151</v>
       </c>
-      <c r="B109" t="s">
+      <c r="B120" t="s">
         <v>138</v>
       </c>
-      <c r="C109" t="s">
+      <c r="C120" t="s">
         <v>160</v>
       </c>
-      <c r="D109" t="s">
+      <c r="D120" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
         <v>153</v>
       </c>
-      <c r="B110" t="s">
+      <c r="B121" t="s">
         <v>138</v>
       </c>
-      <c r="C110" t="s">
+      <c r="C121" t="s">
         <v>154</v>
       </c>
-      <c r="D110" t="s">
+      <c r="D121" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A111" s="4" t="s">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="B111" s="4"/>
-      <c r="C111" s="4"/>
-      <c r="D111" s="4"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A112" t="s">
+      <c r="B122" s="4"/>
+      <c r="C122" s="4"/>
+      <c r="D122" s="4"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>87</v>
       </c>
-      <c r="B112" t="s">
+      <c r="B123" t="s">
         <v>88</v>
       </c>
-      <c r="C112" t="s">
+      <c r="C123" t="s">
         <v>89</v>
       </c>
-      <c r="D112" t="s">
+      <c r="D123" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" t="s">
         <v>91</v>
       </c>
-      <c r="B113" t="s">
+      <c r="B124" t="s">
         <v>88</v>
       </c>
-      <c r="C113" t="s">
+      <c r="C124" t="s">
         <v>69</v>
       </c>
-      <c r="D113" t="s">
+      <c r="D124" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
         <v>188</v>
       </c>
-      <c r="B114" t="s">
+      <c r="B125" t="s">
         <v>88</v>
       </c>
-      <c r="C114" t="s">
+      <c r="C125" t="s">
         <v>189</v>
       </c>
-      <c r="D114" t="s">
+      <c r="D125" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" t="s">
         <v>93</v>
       </c>
-      <c r="B115" t="s">
+      <c r="B126" t="s">
         <v>88</v>
       </c>
-      <c r="C115" t="s">
+      <c r="C126" t="s">
         <v>94</v>
       </c>
-      <c r="D115" t="s">
+      <c r="D126" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Improve filters across modules, make headway on plotView module
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09F12CAD-2348-46A3-8D9F-88F33A7170E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE21314-6046-417C-AA2B-34D17AE9CA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="379">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="406">
   <si>
     <t>id</t>
   </si>
@@ -406,9 +406,6 @@
     <t>Image view module</t>
   </si>
   <si>
-    <t>Plot view module</t>
-  </si>
-  <si>
     <t>Generic labels</t>
   </si>
   <si>
@@ -1157,6 +1154,90 @@
   </si>
   <si>
     <t>Connection</t>
+  </si>
+  <si>
+    <t>tooltip text to explain to user what to do</t>
+  </si>
+  <si>
+    <t>tooltip_visualize_map</t>
+  </si>
+  <si>
+    <t>tooltip_visualize_plot</t>
+  </si>
+  <si>
+    <t>placeholder text</t>
+  </si>
+  <si>
+    <t>Optional…</t>
+  </si>
+  <si>
+    <t>Optionnel…</t>
+  </si>
+  <si>
+    <t>Only the parameter and date options are mandatory; other fields are there to help you narrow your options.</t>
+  </si>
+  <si>
+    <t>Placeholder…</t>
+  </si>
+  <si>
+    <t>Visualize/plot module</t>
+  </si>
+  <si>
+    <t>optional_placeholder</t>
+  </si>
+  <si>
+    <t>mandatory_placeholder</t>
+  </si>
+  <si>
+    <t>Select a parameter</t>
+  </si>
+  <si>
+    <t>Sélectionnez un paramètre</t>
+  </si>
+  <si>
+    <t>map_date_select</t>
+  </si>
+  <si>
+    <t>Sélectionnez une date</t>
+  </si>
+  <si>
+    <t>Select a date</t>
+  </si>
+  <si>
+    <t>map_date_within_select</t>
+  </si>
+  <si>
+    <t>With data within ... day(s) at most</t>
+  </si>
+  <si>
+    <t>Avec données dans un délai de … jour(s) au plus</t>
+  </si>
+  <si>
+    <t>render_map</t>
+  </si>
+  <si>
+    <t>Créer la carte</t>
+  </si>
+  <si>
+    <t>Create map</t>
+  </si>
+  <si>
+    <t>map_absolute</t>
+  </si>
+  <si>
+    <t>Absolute values</t>
+  </si>
+  <si>
+    <t>Valeures absolues</t>
+  </si>
+  <si>
+    <t>map_relative</t>
+  </si>
+  <si>
+    <t>% historical range</t>
+  </si>
+  <si>
+    <t>% plage historique</t>
   </si>
 </sst>
 </file>
@@ -2091,10 +2172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D126"/>
+  <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="E92" sqref="E92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2150,7 +2231,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2256,7 +2337,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2264,142 +2345,142 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B13" t="s">
+        <v>343</v>
+      </c>
+      <c r="C13" t="s">
         <v>344</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>345</v>
-      </c>
-      <c r="D13" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B14" t="s">
+        <v>348</v>
+      </c>
+      <c r="C14" t="s">
         <v>349</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>350</v>
-      </c>
-      <c r="D14" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B15" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C15" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D15" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B16" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C16" t="s">
+        <v>363</v>
+      </c>
+      <c r="D16" t="s">
         <v>364</v>
-      </c>
-      <c r="D16" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B17" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B18" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C18" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D18" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B19" t="s">
+        <v>361</v>
+      </c>
+      <c r="C19" t="s">
+        <v>357</v>
+      </c>
+      <c r="D19" t="s">
         <v>362</v>
-      </c>
-      <c r="C19" t="s">
-        <v>358</v>
-      </c>
-      <c r="D19" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>372</v>
+      </c>
+      <c r="B20" t="s">
+        <v>361</v>
+      </c>
+      <c r="C20" t="s">
         <v>373</v>
       </c>
-      <c r="B20" t="s">
-        <v>362</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>374</v>
-      </c>
-      <c r="D20" t="s">
-        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>375</v>
+      </c>
+      <c r="B21" t="s">
+        <v>369</v>
+      </c>
+      <c r="C21" t="s">
         <v>376</v>
       </c>
-      <c r="B21" t="s">
-        <v>370</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>377</v>
-      </c>
-      <c r="D21" t="s">
-        <v>378</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>368</v>
+      </c>
+      <c r="B22" t="s">
         <v>369</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>370</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>371</v>
-      </c>
-      <c r="D22" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2418,7 +2499,7 @@
         <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -2484,16 +2565,16 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B30" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C30" t="s">
+        <v>285</v>
+      </c>
+      <c r="D30" t="s">
         <v>286</v>
-      </c>
-      <c r="D30" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2501,7 +2582,7 @@
         <v>96</v>
       </c>
       <c r="B31" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C31" t="s">
         <v>97</v>
@@ -2512,217 +2593,217 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>287</v>
+      </c>
+      <c r="B32" t="s">
+        <v>290</v>
+      </c>
+      <c r="C32" t="s">
         <v>288</v>
       </c>
-      <c r="B32" t="s">
-        <v>291</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>289</v>
-      </c>
-      <c r="D32" t="s">
-        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>294</v>
+      </c>
+      <c r="B33" t="s">
+        <v>296</v>
+      </c>
+      <c r="C33" t="s">
         <v>295</v>
       </c>
-      <c r="B33" t="s">
-        <v>297</v>
-      </c>
-      <c r="C33" t="s">
-        <v>296</v>
-      </c>
       <c r="D33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B34" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C34" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D34" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B35" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C35" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D35" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B36" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C36" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D36" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>298</v>
+      </c>
+      <c r="B37" t="s">
         <v>299</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>300</v>
       </c>
-      <c r="C37" t="s">
-        <v>301</v>
-      </c>
       <c r="D37" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B38" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C38" t="s">
+        <v>304</v>
+      </c>
+      <c r="D38" t="s">
         <v>305</v>
-      </c>
-      <c r="D38" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>306</v>
+      </c>
+      <c r="B39" t="s">
+        <v>299</v>
+      </c>
+      <c r="C39" t="s">
         <v>307</v>
       </c>
-      <c r="B39" t="s">
-        <v>300</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>308</v>
-      </c>
-      <c r="D39" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>309</v>
+      </c>
+      <c r="B40" t="s">
+        <v>296</v>
+      </c>
+      <c r="C40" t="s">
         <v>310</v>
       </c>
-      <c r="B40" t="s">
-        <v>297</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>311</v>
-      </c>
-      <c r="D40" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>313</v>
+      </c>
+      <c r="B41" t="s">
+        <v>296</v>
+      </c>
+      <c r="C41" t="s">
         <v>314</v>
       </c>
-      <c r="B41" t="s">
-        <v>297</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>315</v>
-      </c>
-      <c r="D41" t="s">
-        <v>316</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>331</v>
+      </c>
+      <c r="B42" t="s">
+        <v>296</v>
+      </c>
+      <c r="C42" t="s">
         <v>332</v>
       </c>
-      <c r="B42" t="s">
-        <v>297</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>333</v>
-      </c>
-      <c r="D42" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B43" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C43" t="s">
+        <v>318</v>
+      </c>
+      <c r="D43" t="s">
         <v>319</v>
-      </c>
-      <c r="D43" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B44" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C44" t="s">
+        <v>320</v>
+      </c>
+      <c r="D44" t="s">
         <v>321</v>
-      </c>
-      <c r="D44" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>322</v>
+      </c>
+      <c r="B45" t="s">
+        <v>297</v>
+      </c>
+      <c r="C45" t="s">
         <v>323</v>
       </c>
-      <c r="B45" t="s">
-        <v>298</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>324</v>
-      </c>
-      <c r="D45" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>337</v>
+      </c>
+      <c r="B46" t="s">
         <v>338</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>339</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>340</v>
-      </c>
-      <c r="D46" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2730,10 +2811,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>227</v>
+      </c>
+      <c r="B48" t="s">
         <v>228</v>
-      </c>
-      <c r="B48" t="s">
-        <v>229</v>
       </c>
       <c r="C48" t="s">
         <v>103</v>
@@ -2747,7 +2828,7 @@
         <v>81</v>
       </c>
       <c r="B49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C49" t="s">
         <v>82</v>
@@ -2758,72 +2839,72 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B50" t="s">
+        <v>231</v>
+      </c>
+      <c r="C50" t="s">
         <v>232</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>233</v>
-      </c>
-      <c r="D50" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>263</v>
+      </c>
+      <c r="B51" t="s">
         <v>264</v>
       </c>
-      <c r="B51" t="s">
-        <v>265</v>
-      </c>
       <c r="C51" t="s">
+        <v>267</v>
+      </c>
+      <c r="D51" t="s">
         <v>268</v>
-      </c>
-      <c r="D51" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B52" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D52" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>278</v>
+      </c>
+      <c r="B53" t="s">
+        <v>276</v>
+      </c>
+      <c r="C53" t="s">
         <v>279</v>
       </c>
-      <c r="B53" t="s">
-        <v>277</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>280</v>
-      </c>
-      <c r="D53" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>281</v>
+      </c>
+      <c r="B54" t="s">
+        <v>276</v>
+      </c>
+      <c r="C54" t="s">
         <v>282</v>
       </c>
-      <c r="B54" t="s">
-        <v>277</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>283</v>
-      </c>
-      <c r="D54" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -2914,16 +2995,16 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B62" t="s">
         <v>106</v>
       </c>
       <c r="C62" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D62" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -2942,7 +3023,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>128</v>
+        <v>386</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -2963,829 +3044,940 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
+      <c r="A66" t="s">
+        <v>379</v>
+      </c>
+      <c r="B66" t="s">
+        <v>378</v>
+      </c>
+      <c r="C66" t="s">
+        <v>384</v>
+      </c>
+      <c r="D66" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>164</v>
+        <v>380</v>
       </c>
       <c r="B67" t="s">
-        <v>48</v>
+        <v>378</v>
       </c>
       <c r="C67" t="s">
-        <v>165</v>
+        <v>385</v>
       </c>
       <c r="D67" t="s">
-        <v>166</v>
+        <v>385</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>170</v>
+        <v>387</v>
       </c>
       <c r="B68" t="s">
-        <v>167</v>
+        <v>381</v>
       </c>
       <c r="C68" t="s">
-        <v>168</v>
+        <v>382</v>
       </c>
       <c r="D68" t="s">
-        <v>169</v>
+        <v>383</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>173</v>
+        <v>388</v>
       </c>
       <c r="B69" t="s">
-        <v>174</v>
+        <v>381</v>
       </c>
       <c r="C69" t="s">
-        <v>185</v>
+        <v>389</v>
       </c>
       <c r="D69" t="s">
-        <v>186</v>
+        <v>390</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>182</v>
-      </c>
-      <c r="B70" t="s">
-        <v>167</v>
+        <v>391</v>
       </c>
       <c r="C70" t="s">
-        <v>171</v>
+        <v>393</v>
       </c>
       <c r="D70" t="s">
-        <v>172</v>
+        <v>392</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>175</v>
-      </c>
-      <c r="B71" t="s">
-        <v>174</v>
+        <v>394</v>
       </c>
       <c r="C71" t="s">
-        <v>184</v>
+        <v>395</v>
       </c>
       <c r="D71" t="s">
-        <v>183</v>
+        <v>396</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>176</v>
-      </c>
-      <c r="B72" t="s">
-        <v>178</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>177</v>
-      </c>
-      <c r="B73" t="s">
-        <v>174</v>
-      </c>
-      <c r="C73" t="s">
-        <v>179</v>
-      </c>
-      <c r="D73" t="s">
-        <v>181</v>
+        <v>397</v>
+      </c>
+      <c r="C72" t="s">
+        <v>399</v>
+      </c>
+      <c r="D72" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B74" s="8"/>
-      <c r="C74" s="8"/>
-      <c r="D74" s="8"/>
+      <c r="A74" t="s">
+        <v>400</v>
+      </c>
+      <c r="C74" t="s">
+        <v>401</v>
+      </c>
+      <c r="D74" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>61</v>
-      </c>
-      <c r="B75" t="s">
-        <v>9</v>
+        <v>403</v>
       </c>
       <c r="C75" t="s">
-        <v>62</v>
+        <v>404</v>
       </c>
       <c r="D75" t="s">
-        <v>63</v>
+        <v>405</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>120</v>
-      </c>
-      <c r="B76" t="s">
-        <v>9</v>
-      </c>
-      <c r="C76" t="s">
-        <v>121</v>
-      </c>
-      <c r="D76" t="s">
-        <v>122</v>
-      </c>
+      <c r="A76" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B76" s="4"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>64</v>
+        <v>163</v>
       </c>
       <c r="B77" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="C77" t="s">
-        <v>65</v>
+        <v>164</v>
       </c>
       <c r="D77" t="s">
-        <v>66</v>
+        <v>165</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="B78" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="C78" t="s">
-        <v>68</v>
+        <v>167</v>
       </c>
       <c r="D78" t="s">
-        <v>267</v>
+        <v>168</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>262</v>
+        <v>172</v>
       </c>
       <c r="B79" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="C79" t="s">
-        <v>263</v>
+        <v>184</v>
       </c>
       <c r="D79" t="s">
-        <v>263</v>
+        <v>185</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>69</v>
+        <v>181</v>
       </c>
       <c r="B80" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="C80" t="s">
-        <v>70</v>
+        <v>170</v>
       </c>
       <c r="D80" t="s">
-        <v>71</v>
+        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>205</v>
+        <v>174</v>
       </c>
       <c r="B81" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="C81" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="D81" t="s">
-        <v>207</v>
+        <v>182</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>210</v>
+        <v>175</v>
       </c>
       <c r="B82" t="s">
-        <v>9</v>
-      </c>
-      <c r="C82" t="s">
-        <v>208</v>
-      </c>
-      <c r="D82" t="s">
-        <v>209</v>
+        <v>177</v>
+      </c>
+      <c r="C82" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>191</v>
+        <v>176</v>
       </c>
       <c r="B83" t="s">
-        <v>9</v>
+        <v>173</v>
       </c>
       <c r="C83" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="D83" t="s">
-        <v>193</v>
+        <v>180</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>202</v>
-      </c>
-      <c r="B84" t="s">
-        <v>9</v>
-      </c>
-      <c r="C84" t="s">
-        <v>203</v>
-      </c>
-      <c r="D84" t="s">
-        <v>204</v>
-      </c>
+      <c r="A84" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
+      <c r="D84" s="8"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>217</v>
+        <v>61</v>
       </c>
       <c r="B85" t="s">
         <v>9</v>
       </c>
       <c r="C85" t="s">
-        <v>218</v>
+        <v>62</v>
       </c>
       <c r="D85" t="s">
-        <v>219</v>
+        <v>63</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>189</v>
+        <v>120</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>235</v>
+        <v>121</v>
       </c>
       <c r="D86" t="s">
-        <v>236</v>
+        <v>122</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="B87" t="s">
         <v>9</v>
       </c>
       <c r="C87" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="D87" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>199</v>
+        <v>67</v>
       </c>
       <c r="B88" t="s">
         <v>9</v>
       </c>
       <c r="C88" t="s">
-        <v>194</v>
+        <v>68</v>
       </c>
       <c r="D88" t="s">
-        <v>17</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>211</v>
+        <v>261</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>212</v>
+        <v>262</v>
       </c>
       <c r="D89" t="s">
-        <v>213</v>
+        <v>262</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="D90" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="D91" t="s">
-        <v>201</v>
+        <v>206</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="D92" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>78</v>
+        <v>190</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>79</v>
+        <v>191</v>
       </c>
       <c r="D93" t="s">
-        <v>80</v>
+        <v>192</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="D94" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="D95" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>239</v>
+        <v>188</v>
       </c>
       <c r="B96" t="s">
         <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="D96" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>240</v>
+        <v>72</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>241</v>
+        <v>73</v>
       </c>
       <c r="D97" t="s">
-        <v>134</v>
+        <v>74</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>242</v>
+        <v>198</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>243</v>
+        <v>193</v>
       </c>
       <c r="D98" t="s">
-        <v>244</v>
+        <v>17</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>335</v>
+        <v>210</v>
+      </c>
+      <c r="B99" t="s">
+        <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>336</v>
+        <v>211</v>
       </c>
       <c r="D99" t="s">
-        <v>337</v>
+        <v>212</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="D100" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>8</v>
+        <v>197</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>10</v>
+        <v>199</v>
       </c>
       <c r="D101" t="s">
-        <v>11</v>
+        <v>200</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>245</v>
+        <v>214</v>
       </c>
       <c r="D102" t="s">
-        <v>246</v>
+        <v>215</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>223</v>
+        <v>78</v>
       </c>
       <c r="B103" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>223</v>
+        <v>79</v>
       </c>
       <c r="D103" t="s">
-        <v>225</v>
+        <v>80</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>247</v>
+        <v>196</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>249</v>
+        <v>194</v>
       </c>
       <c r="D104" t="s">
-        <v>250</v>
+        <v>195</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>248</v>
+        <v>219</v>
       </c>
       <c r="B105" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>251</v>
+        <v>220</v>
       </c>
       <c r="D105" t="s">
-        <v>252</v>
+        <v>221</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>274</v>
+        <v>238</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>270</v>
+        <v>236</v>
       </c>
       <c r="D106" t="s">
-        <v>272</v>
+        <v>237</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>275</v>
+        <v>239</v>
       </c>
       <c r="B107" t="s">
-        <v>224</v>
+        <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>271</v>
+        <v>240</v>
       </c>
       <c r="D107" t="s">
-        <v>273</v>
+        <v>133</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="D108" t="s">
-        <v>260</v>
+        <v>243</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>257</v>
-      </c>
-      <c r="B109" t="s">
-        <v>224</v>
+        <v>334</v>
       </c>
       <c r="C109" t="s">
-        <v>259</v>
+        <v>335</v>
       </c>
       <c r="D109" t="s">
-        <v>261</v>
+        <v>336</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>135</v>
+        <v>84</v>
       </c>
       <c r="B110" t="s">
         <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>136</v>
+        <v>85</v>
       </c>
       <c r="D110" t="s">
-        <v>137</v>
+        <v>86</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>253</v>
+        <v>8</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
       </c>
       <c r="C111" t="s">
-        <v>254</v>
+        <v>10</v>
       </c>
       <c r="D111" t="s">
-        <v>255</v>
+        <v>11</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>15</v>
+        <v>244</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>16</v>
+        <v>244</v>
       </c>
       <c r="D112" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="B113" s="2"/>
-      <c r="C113" s="2"/>
-      <c r="D113" s="2"/>
+      <c r="A113" t="s">
+        <v>222</v>
+      </c>
+      <c r="B113" t="s">
+        <v>223</v>
+      </c>
+      <c r="C113" t="s">
+        <v>222</v>
+      </c>
+      <c r="D113" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>139</v>
+        <v>246</v>
       </c>
       <c r="B114" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>158</v>
+        <v>248</v>
       </c>
       <c r="D114" t="s">
-        <v>157</v>
+        <v>249</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="B115" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="C115" t="s">
-        <v>159</v>
+        <v>250</v>
       </c>
       <c r="D115" t="s">
-        <v>162</v>
+        <v>251</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>140</v>
+        <v>273</v>
       </c>
       <c r="B116" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>141</v>
+        <v>269</v>
       </c>
       <c r="D116" t="s">
-        <v>148</v>
+        <v>271</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>145</v>
+        <v>274</v>
       </c>
       <c r="B117" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="C117" t="s">
-        <v>146</v>
+        <v>270</v>
       </c>
       <c r="D117" t="s">
-        <v>147</v>
+        <v>272</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>142</v>
+        <v>255</v>
       </c>
       <c r="B118" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>143</v>
+        <v>257</v>
       </c>
       <c r="D118" t="s">
-        <v>144</v>
+        <v>259</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>149</v>
+        <v>256</v>
       </c>
       <c r="B119" t="s">
-        <v>138</v>
+        <v>223</v>
       </c>
       <c r="C119" t="s">
-        <v>161</v>
+        <v>258</v>
       </c>
       <c r="D119" t="s">
-        <v>150</v>
+        <v>260</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="B120" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>160</v>
+        <v>135</v>
       </c>
       <c r="D120" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>153</v>
+        <v>252</v>
       </c>
       <c r="B121" t="s">
-        <v>138</v>
+        <v>9</v>
       </c>
       <c r="C121" t="s">
-        <v>154</v>
+        <v>253</v>
       </c>
       <c r="D121" t="s">
-        <v>155</v>
+        <v>254</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
+      <c r="A122" t="s">
+        <v>15</v>
+      </c>
+      <c r="B122" t="s">
+        <v>9</v>
+      </c>
+      <c r="C122" t="s">
+        <v>16</v>
+      </c>
+      <c r="D122" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>87</v>
-      </c>
-      <c r="B123" t="s">
-        <v>88</v>
-      </c>
-      <c r="C123" t="s">
-        <v>89</v>
-      </c>
-      <c r="D123" t="s">
-        <v>90</v>
-      </c>
+      <c r="A123" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B123" s="2"/>
+      <c r="C123" s="2"/>
+      <c r="D123" s="2"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>91</v>
+        <v>138</v>
       </c>
       <c r="B124" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="C124" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
       <c r="D124" t="s">
-        <v>92</v>
+        <v>156</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="B125" t="s">
-        <v>88</v>
+        <v>137</v>
       </c>
       <c r="C125" t="s">
-        <v>189</v>
+        <v>158</v>
       </c>
       <c r="D125" t="s">
-        <v>190</v>
+        <v>161</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
+        <v>139</v>
+      </c>
+      <c r="B126" t="s">
+        <v>137</v>
+      </c>
+      <c r="C126" t="s">
+        <v>140</v>
+      </c>
+      <c r="D126" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" t="s">
+        <v>144</v>
+      </c>
+      <c r="B127" t="s">
+        <v>137</v>
+      </c>
+      <c r="C127" t="s">
+        <v>145</v>
+      </c>
+      <c r="D127" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" t="s">
+        <v>141</v>
+      </c>
+      <c r="B128" t="s">
+        <v>137</v>
+      </c>
+      <c r="C128" t="s">
+        <v>142</v>
+      </c>
+      <c r="D128" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>148</v>
+      </c>
+      <c r="B129" t="s">
+        <v>137</v>
+      </c>
+      <c r="C129" t="s">
+        <v>160</v>
+      </c>
+      <c r="D129" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A130" t="s">
+        <v>150</v>
+      </c>
+      <c r="B130" t="s">
+        <v>137</v>
+      </c>
+      <c r="C130" t="s">
+        <v>159</v>
+      </c>
+      <c r="D130" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>152</v>
+      </c>
+      <c r="B131" t="s">
+        <v>137</v>
+      </c>
+      <c r="C131" t="s">
+        <v>153</v>
+      </c>
+      <c r="D131" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A132" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B132" s="4"/>
+      <c r="C132" s="4"/>
+      <c r="D132" s="4"/>
+    </row>
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>87</v>
+      </c>
+      <c r="B133" t="s">
+        <v>88</v>
+      </c>
+      <c r="C133" t="s">
+        <v>89</v>
+      </c>
+      <c r="D133" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>91</v>
+      </c>
+      <c r="B134" t="s">
+        <v>88</v>
+      </c>
+      <c r="C134" t="s">
+        <v>69</v>
+      </c>
+      <c r="D134" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>187</v>
+      </c>
+      <c r="B135" t="s">
+        <v>88</v>
+      </c>
+      <c r="C135" t="s">
+        <v>188</v>
+      </c>
+      <c r="D135" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A136" t="s">
         <v>93</v>
       </c>
-      <c r="B126" t="s">
+      <c r="B136" t="s">
         <v>88</v>
       </c>
-      <c r="C126" t="s">
+      <c r="C136" t="s">
         <v>94</v>
       </c>
-      <c r="D126" t="s">
+      <c r="D136" t="s">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update hydroApp for new DB schema, start on streamLine update
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -5,17 +5,30 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yukongovernment-my.sharepoint.com/personal/gtdelapl_ynet_gov_yk_ca/Documents/Documents/YGwater/inst/apps/streamLine/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADE21314-6046-417C-AA2B-34D17AE9CA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{ADE21314-6046-417C-AA2B-34D17AE9CA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3CAABAC-C859-416B-ACE0-B6662D9E4CD7}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -229,15 +242,6 @@
     <t>Discrete</t>
   </si>
   <si>
-    <t>param_type</t>
-  </si>
-  <si>
-    <t>Parameter Type</t>
-  </si>
-  <si>
-    <t>Type de paramètre</t>
-  </si>
-  <si>
     <t>parameter</t>
   </si>
   <si>
@@ -295,12 +299,6 @@
     <t>param_name_fr</t>
   </si>
   <si>
-    <t>param_type_col</t>
-  </si>
-  <si>
-    <t>param_type_fr</t>
-  </si>
-  <si>
     <t>generic_name_col</t>
   </si>
   <si>
@@ -634,24 +632,6 @@
     <t>Groupes de paramètres</t>
   </si>
   <si>
-    <t>param_types</t>
-  </si>
-  <si>
-    <t>Parameter Types</t>
-  </si>
-  <si>
-    <t>Types de paramètres</t>
-  </si>
-  <si>
-    <t>Parameter Type(s)</t>
-  </si>
-  <si>
-    <t>Type(s) de paramètre(s)</t>
-  </si>
-  <si>
-    <t>param_type(s)</t>
-  </si>
-  <si>
     <t>parameter(s)</t>
   </si>
   <si>
@@ -1238,6 +1218,39 @@
   </si>
   <si>
     <t>% plage historique</t>
+  </si>
+  <si>
+    <t>media_type</t>
+  </si>
+  <si>
+    <t>media_types</t>
+  </si>
+  <si>
+    <t>media_type(s)</t>
+  </si>
+  <si>
+    <t>Sample Media Type</t>
+  </si>
+  <si>
+    <t>Sample Media Types</t>
+  </si>
+  <si>
+    <t>Type de média d'échantillonage</t>
+  </si>
+  <si>
+    <t>Types de médias d'échantillonage</t>
+  </si>
+  <si>
+    <t>Sample Media Type(s)</t>
+  </si>
+  <si>
+    <t>Type(s) de médias(s) d'échantillonage</t>
+  </si>
+  <si>
+    <t>media_type_col</t>
+  </si>
+  <si>
+    <t>media_type_fr</t>
   </si>
 </sst>
 </file>
@@ -2174,8 +2187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="E92" sqref="E92"/>
+    <sheetView tabSelected="1" topLeftCell="A114" workbookViewId="0">
+      <selection activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2217,21 +2230,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2337,7 +2350,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>342</v>
+        <v>331</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2345,147 +2358,147 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>341</v>
+        <v>330</v>
       </c>
       <c r="B13" t="s">
-        <v>343</v>
+        <v>332</v>
       </c>
       <c r="C13" t="s">
-        <v>344</v>
+        <v>333</v>
       </c>
       <c r="D13" t="s">
-        <v>345</v>
+        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>346</v>
+        <v>335</v>
       </c>
       <c r="B14" t="s">
-        <v>348</v>
+        <v>337</v>
       </c>
       <c r="C14" t="s">
-        <v>349</v>
+        <v>338</v>
       </c>
       <c r="D14" t="s">
-        <v>350</v>
+        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>347</v>
+        <v>336</v>
       </c>
       <c r="B15" t="s">
-        <v>353</v>
+        <v>342</v>
       </c>
       <c r="C15" t="s">
-        <v>352</v>
+        <v>341</v>
       </c>
       <c r="D15" t="s">
-        <v>351</v>
+        <v>340</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>354</v>
+        <v>343</v>
       </c>
       <c r="B16" t="s">
-        <v>360</v>
+        <v>349</v>
       </c>
       <c r="C16" t="s">
-        <v>363</v>
+        <v>352</v>
       </c>
       <c r="D16" t="s">
-        <v>364</v>
+        <v>353</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>358</v>
+        <v>347</v>
       </c>
       <c r="B17" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="C17" t="s">
-        <v>355</v>
+        <v>344</v>
       </c>
       <c r="D17" t="s">
-        <v>365</v>
+        <v>354</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>345</v>
+      </c>
+      <c r="B18" t="s">
+        <v>349</v>
+      </c>
+      <c r="C18" t="s">
         <v>356</v>
       </c>
-      <c r="B18" t="s">
-        <v>360</v>
-      </c>
-      <c r="C18" t="s">
-        <v>367</v>
-      </c>
       <c r="D18" t="s">
-        <v>366</v>
+        <v>355</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>359</v>
+        <v>348</v>
       </c>
       <c r="B19" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="C19" t="s">
-        <v>357</v>
+        <v>346</v>
       </c>
       <c r="D19" t="s">
-        <v>362</v>
+        <v>351</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="B20" t="s">
-        <v>361</v>
+        <v>350</v>
       </c>
       <c r="C20" t="s">
-        <v>373</v>
+        <v>362</v>
       </c>
       <c r="D20" t="s">
-        <v>374</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>375</v>
+        <v>364</v>
       </c>
       <c r="B21" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="C21" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="D21" t="s">
-        <v>377</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>368</v>
+        <v>357</v>
       </c>
       <c r="B22" t="s">
-        <v>369</v>
+        <v>358</v>
       </c>
       <c r="C22" t="s">
-        <v>370</v>
+        <v>359</v>
       </c>
       <c r="D22" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2499,7 +2512,7 @@
         <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -2521,7 +2534,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2543,7 +2556,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2565,245 +2578,245 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>277</v>
+        <v>266</v>
       </c>
       <c r="B30" t="s">
+        <v>264</v>
+      </c>
+      <c r="C30" t="s">
+        <v>274</v>
+      </c>
+      <c r="D30" t="s">
         <v>275</v>
-      </c>
-      <c r="C30" t="s">
-        <v>285</v>
-      </c>
-      <c r="D30" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B31" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="C31" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D31" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>287</v>
+        <v>276</v>
       </c>
       <c r="B32" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="C32" t="s">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="D32" t="s">
-        <v>289</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B33" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C33" t="s">
-        <v>295</v>
+        <v>284</v>
       </c>
       <c r="D33" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>280</v>
+      </c>
+      <c r="B34" t="s">
+        <v>286</v>
+      </c>
+      <c r="C34" t="s">
         <v>291</v>
       </c>
-      <c r="B34" t="s">
-        <v>297</v>
-      </c>
-      <c r="C34" t="s">
-        <v>302</v>
-      </c>
       <c r="D34" t="s">
-        <v>301</v>
+        <v>290</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B35" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C35" t="s">
-        <v>326</v>
+        <v>315</v>
       </c>
       <c r="D35" t="s">
-        <v>328</v>
+        <v>317</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="B36" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C36" t="s">
-        <v>327</v>
+        <v>316</v>
       </c>
       <c r="D36" t="s">
-        <v>329</v>
+        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>298</v>
+        <v>287</v>
       </c>
       <c r="B37" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="C37" t="s">
-        <v>300</v>
+        <v>289</v>
       </c>
       <c r="D37" t="s">
-        <v>303</v>
+        <v>292</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>325</v>
+        <v>314</v>
       </c>
       <c r="B38" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="C38" t="s">
-        <v>304</v>
+        <v>293</v>
       </c>
       <c r="D38" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>306</v>
+        <v>295</v>
       </c>
       <c r="B39" t="s">
-        <v>299</v>
+        <v>288</v>
       </c>
       <c r="C39" t="s">
-        <v>307</v>
+        <v>296</v>
       </c>
       <c r="D39" t="s">
-        <v>308</v>
+        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>309</v>
+        <v>298</v>
       </c>
       <c r="B40" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C40" t="s">
-        <v>310</v>
+        <v>299</v>
       </c>
       <c r="D40" t="s">
-        <v>311</v>
+        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
       <c r="B41" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C41" t="s">
-        <v>314</v>
+        <v>303</v>
       </c>
       <c r="D41" t="s">
-        <v>315</v>
+        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>331</v>
+        <v>320</v>
       </c>
       <c r="B42" t="s">
-        <v>296</v>
+        <v>285</v>
       </c>
       <c r="C42" t="s">
-        <v>332</v>
+        <v>321</v>
       </c>
       <c r="D42" t="s">
-        <v>333</v>
+        <v>322</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="B43" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C43" t="s">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="D43" t="s">
-        <v>319</v>
+        <v>308</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>317</v>
+        <v>306</v>
       </c>
       <c r="B44" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C44" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="D44" t="s">
-        <v>321</v>
+        <v>310</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>322</v>
+        <v>311</v>
       </c>
       <c r="B45" t="s">
-        <v>297</v>
+        <v>286</v>
       </c>
       <c r="C45" t="s">
-        <v>323</v>
+        <v>312</v>
       </c>
       <c r="D45" t="s">
-        <v>324</v>
+        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>337</v>
+        <v>326</v>
       </c>
       <c r="B46" t="s">
-        <v>338</v>
+        <v>327</v>
       </c>
       <c r="C46" t="s">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="D46" t="s">
-        <v>340</v>
+        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>226</v>
+        <v>215</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2811,105 +2824,105 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B48" t="s">
-        <v>228</v>
+        <v>217</v>
       </c>
       <c r="C48" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D48" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>230</v>
+        <v>219</v>
       </c>
       <c r="C49" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D49" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>225</v>
+        <v>214</v>
       </c>
       <c r="B50" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="C50" t="s">
-        <v>232</v>
+        <v>221</v>
       </c>
       <c r="D50" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>263</v>
+        <v>252</v>
       </c>
       <c r="B51" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C51" t="s">
-        <v>267</v>
+        <v>256</v>
       </c>
       <c r="D51" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>265</v>
+        <v>254</v>
       </c>
       <c r="B52" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="C52" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
       <c r="D52" t="s">
-        <v>284</v>
+        <v>273</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>278</v>
+        <v>267</v>
       </c>
       <c r="B53" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C53" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="D53" t="s">
-        <v>280</v>
+        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>281</v>
+        <v>270</v>
       </c>
       <c r="B54" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C54" t="s">
-        <v>282</v>
+        <v>271</v>
       </c>
       <c r="D54" t="s">
-        <v>283</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2931,7 +2944,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -2953,77 +2966,77 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B59" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C59" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D59" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" t="s">
+        <v>103</v>
+      </c>
+      <c r="C60" t="s">
+        <v>105</v>
+      </c>
+      <c r="D60" t="s">
         <v>107</v>
-      </c>
-      <c r="B60" t="s">
-        <v>108</v>
-      </c>
-      <c r="C60" t="s">
-        <v>110</v>
-      </c>
-      <c r="D60" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="B61" t="s">
+        <v>103</v>
+      </c>
+      <c r="C61" t="s">
+        <v>106</v>
+      </c>
+      <c r="D61" t="s">
         <v>108</v>
-      </c>
-      <c r="C61" t="s">
-        <v>111</v>
-      </c>
-      <c r="D61" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="D62" t="s">
-        <v>312</v>
+        <v>301</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B63" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C63" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D63" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>386</v>
+        <v>375</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -3045,118 +3058,118 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>379</v>
+        <v>368</v>
       </c>
       <c r="B66" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="C66" t="s">
-        <v>384</v>
+        <v>373</v>
       </c>
       <c r="D66" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>380</v>
+        <v>369</v>
       </c>
       <c r="B67" t="s">
-        <v>378</v>
+        <v>367</v>
       </c>
       <c r="C67" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
       <c r="D67" t="s">
-        <v>385</v>
+        <v>374</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>387</v>
+        <v>376</v>
       </c>
       <c r="B68" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="C68" t="s">
-        <v>382</v>
+        <v>371</v>
       </c>
       <c r="D68" t="s">
-        <v>383</v>
+        <v>372</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>388</v>
+        <v>377</v>
       </c>
       <c r="B69" t="s">
-        <v>381</v>
+        <v>370</v>
       </c>
       <c r="C69" t="s">
-        <v>389</v>
+        <v>378</v>
       </c>
       <c r="D69" t="s">
-        <v>390</v>
+        <v>379</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>391</v>
+        <v>380</v>
       </c>
       <c r="C70" t="s">
-        <v>393</v>
+        <v>382</v>
       </c>
       <c r="D70" t="s">
-        <v>392</v>
+        <v>381</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>394</v>
+        <v>383</v>
       </c>
       <c r="C71" t="s">
-        <v>395</v>
+        <v>384</v>
       </c>
       <c r="D71" t="s">
-        <v>396</v>
+        <v>385</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>397</v>
+        <v>386</v>
       </c>
       <c r="C72" t="s">
-        <v>399</v>
+        <v>388</v>
       </c>
       <c r="D72" t="s">
-        <v>398</v>
+        <v>387</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>400</v>
+        <v>389</v>
       </c>
       <c r="C74" t="s">
-        <v>401</v>
+        <v>390</v>
       </c>
       <c r="D74" t="s">
-        <v>402</v>
+        <v>391</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>403</v>
+        <v>392</v>
       </c>
       <c r="C75" t="s">
-        <v>404</v>
+        <v>393</v>
       </c>
       <c r="D75" t="s">
-        <v>405</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -3164,105 +3177,105 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B77" t="s">
         <v>48</v>
       </c>
       <c r="C77" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D77" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B78" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C78" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D78" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="B79" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C79" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="D79" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B80" t="s">
+        <v>161</v>
+      </c>
+      <c r="C80" t="s">
+        <v>165</v>
+      </c>
+      <c r="D80" t="s">
         <v>166</v>
-      </c>
-      <c r="C80" t="s">
-        <v>170</v>
-      </c>
-      <c r="D80" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="B81" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C81" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="D81" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B82" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D82" s="9" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="B83" t="s">
+        <v>168</v>
+      </c>
+      <c r="C83" t="s">
         <v>173</v>
       </c>
-      <c r="C83" t="s">
-        <v>178</v>
-      </c>
       <c r="D83" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
@@ -3284,16 +3297,16 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D86" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3321,144 +3334,144 @@
         <v>68</v>
       </c>
       <c r="D88" t="s">
-        <v>266</v>
+        <v>255</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>261</v>
+        <v>250</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
       <c r="D89" t="s">
-        <v>262</v>
+        <v>251</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>69</v>
+        <v>395</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>70</v>
+        <v>398</v>
       </c>
       <c r="D90" t="s">
-        <v>71</v>
+        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>204</v>
+        <v>396</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>205</v>
+        <v>399</v>
       </c>
       <c r="D91" t="s">
-        <v>206</v>
+        <v>401</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>209</v>
+        <v>397</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>207</v>
+        <v>402</v>
       </c>
       <c r="D92" t="s">
-        <v>208</v>
+        <v>403</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="D93" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="D94" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="D95" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B96" t="s">
         <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>234</v>
+        <v>223</v>
       </c>
       <c r="D96" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D97" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="D98" t="s">
         <v>17</v>
@@ -3466,167 +3479,167 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D99" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="D100" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D101" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="D102" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="D103" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="D104" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="D105" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>238</v>
+        <v>227</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>236</v>
+        <v>225</v>
       </c>
       <c r="D106" t="s">
-        <v>237</v>
+        <v>226</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>239</v>
+        <v>228</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="D107" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>241</v>
+        <v>230</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>242</v>
+        <v>231</v>
       </c>
       <c r="D108" t="s">
-        <v>243</v>
+        <v>232</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>334</v>
+        <v>323</v>
       </c>
       <c r="C109" t="s">
-        <v>335</v>
+        <v>324</v>
       </c>
       <c r="D109" t="s">
-        <v>336</v>
+        <v>325</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B110" t="s">
         <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D110" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
@@ -3645,142 +3658,142 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>244</v>
+        <v>233</v>
       </c>
       <c r="D112" t="s">
-        <v>245</v>
+        <v>234</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="B113" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C113" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="D113" t="s">
-        <v>224</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B114" t="s">
         <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>248</v>
+        <v>237</v>
       </c>
       <c r="D114" t="s">
-        <v>249</v>
+        <v>238</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>247</v>
+        <v>236</v>
       </c>
       <c r="B115" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C115" t="s">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="D115" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>273</v>
+        <v>262</v>
       </c>
       <c r="B116" t="s">
         <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="D116" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>274</v>
+        <v>263</v>
       </c>
       <c r="B117" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C117" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="D117" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>255</v>
+        <v>244</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="D118" t="s">
-        <v>259</v>
+        <v>248</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
       <c r="B119" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
       <c r="C119" t="s">
-        <v>258</v>
+        <v>247</v>
       </c>
       <c r="D119" t="s">
-        <v>260</v>
+        <v>249</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B120" t="s">
         <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D120" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="B121" t="s">
         <v>9</v>
       </c>
       <c r="C121" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="D121" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3799,7 +3812,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3807,119 +3820,119 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B124" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C124" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="D124" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B125" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C125" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D125" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B126" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C126" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="D126" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B127" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C127" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D127" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B128" t="s">
+        <v>132</v>
+      </c>
+      <c r="C128" t="s">
         <v>137</v>
       </c>
-      <c r="C128" t="s">
-        <v>142</v>
-      </c>
       <c r="D128" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B129" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C129" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D129" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B130" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C130" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D130" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B131" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="C131" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D131" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -3927,58 +3940,58 @@
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
+        <v>84</v>
+      </c>
+      <c r="B133" t="s">
+        <v>85</v>
+      </c>
+      <c r="C133" t="s">
+        <v>86</v>
+      </c>
+      <c r="D133" t="s">
         <v>87</v>
-      </c>
-      <c r="B133" t="s">
-        <v>88</v>
-      </c>
-      <c r="C133" t="s">
-        <v>89</v>
-      </c>
-      <c r="D133" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>91</v>
+        <v>404</v>
       </c>
       <c r="B134" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C134" t="s">
-        <v>69</v>
+        <v>395</v>
       </c>
       <c r="D134" t="s">
-        <v>92</v>
+        <v>405</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="B135" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C135" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D135" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B136" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C136" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D136" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start to add maps to application
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://yukongovernment-my.sharepoint.com/personal/gtdelapl_ynet_gov_yk_ca/Documents/Documents/YGwater/inst/apps/streamLine/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\OneDrive - Government of Yukon\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="13_ncr:1_{ADE21314-6046-417C-AA2B-34D17AE9CA50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3CAABAC-C859-416B-ACE0-B6662D9E4CD7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66655630-4FB9-4F76-B7F2-634940C19632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="translations" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="404">
   <si>
     <t>id</t>
   </si>
@@ -291,12 +291,6 @@
   </si>
   <si>
     <t xml:space="preserve">DB column selection </t>
-  </si>
-  <si>
-    <t>param_name</t>
-  </si>
-  <si>
-    <t>param_name_fr</t>
   </si>
   <si>
     <t>generic_name_col</t>
@@ -2187,8 +2181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D136"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="A134" sqref="A134"/>
+    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2230,21 +2224,21 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" t="s">
         <v>94</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D3" t="s">
         <v>95</v>
-      </c>
-      <c r="C3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -2350,7 +2344,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2358,147 +2352,147 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>328</v>
+      </c>
+      <c r="B13" t="s">
         <v>330</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>331</v>
+      </c>
+      <c r="D13" t="s">
         <v>332</v>
-      </c>
-      <c r="C13" t="s">
-        <v>333</v>
-      </c>
-      <c r="D13" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>333</v>
+      </c>
+      <c r="B14" t="s">
         <v>335</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>336</v>
+      </c>
+      <c r="D14" t="s">
         <v>337</v>
-      </c>
-      <c r="C14" t="s">
-        <v>338</v>
-      </c>
-      <c r="D14" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="B15" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C15" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D15" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B16" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C16" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D16" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="C17" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D17" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B18" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="C18" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D18" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>346</v>
+      </c>
+      <c r="B19" t="s">
         <v>348</v>
       </c>
-      <c r="B19" t="s">
-        <v>350</v>
-      </c>
       <c r="C19" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D19" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>359</v>
+      </c>
+      <c r="B20" t="s">
+        <v>348</v>
+      </c>
+      <c r="C20" t="s">
+        <v>360</v>
+      </c>
+      <c r="D20" t="s">
         <v>361</v>
-      </c>
-      <c r="B20" t="s">
-        <v>350</v>
-      </c>
-      <c r="C20" t="s">
-        <v>362</v>
-      </c>
-      <c r="D20" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>362</v>
+      </c>
+      <c r="B21" t="s">
+        <v>356</v>
+      </c>
+      <c r="C21" t="s">
+        <v>363</v>
+      </c>
+      <c r="D21" t="s">
         <v>364</v>
-      </c>
-      <c r="B21" t="s">
-        <v>358</v>
-      </c>
-      <c r="C21" t="s">
-        <v>365</v>
-      </c>
-      <c r="D21" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>355</v>
+      </c>
+      <c r="B22" t="s">
+        <v>356</v>
+      </c>
+      <c r="C22" t="s">
         <v>357</v>
       </c>
-      <c r="B22" t="s">
+      <c r="D22" t="s">
         <v>358</v>
-      </c>
-      <c r="C22" t="s">
-        <v>359</v>
-      </c>
-      <c r="D22" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -2512,7 +2506,7 @@
         <v>41</v>
       </c>
       <c r="C24" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -2534,7 +2528,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -2556,7 +2550,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2578,245 +2572,245 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="B30" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C30" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D30" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>89</v>
+      </c>
+      <c r="B31" t="s">
+        <v>216</v>
+      </c>
+      <c r="C31" t="s">
+        <v>90</v>
+      </c>
+      <c r="D31" t="s">
         <v>91</v>
-      </c>
-      <c r="B31" t="s">
-        <v>218</v>
-      </c>
-      <c r="C31" t="s">
-        <v>92</v>
-      </c>
-      <c r="D31" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>274</v>
+      </c>
+      <c r="B32" t="s">
+        <v>277</v>
+      </c>
+      <c r="C32" t="s">
+        <v>275</v>
+      </c>
+      <c r="D32" t="s">
         <v>276</v>
-      </c>
-      <c r="B32" t="s">
-        <v>279</v>
-      </c>
-      <c r="C32" t="s">
-        <v>277</v>
-      </c>
-      <c r="D32" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>281</v>
+      </c>
+      <c r="B33" t="s">
         <v>283</v>
       </c>
-      <c r="B33" t="s">
-        <v>285</v>
-      </c>
       <c r="C33" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D33" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="B34" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C34" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D34" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B35" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C35" t="s">
+        <v>313</v>
+      </c>
+      <c r="D35" t="s">
         <v>315</v>
-      </c>
-      <c r="D35" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="B36" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C36" t="s">
+        <v>314</v>
+      </c>
+      <c r="D36" t="s">
         <v>316</v>
-      </c>
-      <c r="D36" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>285</v>
+      </c>
+      <c r="B37" t="s">
+        <v>286</v>
+      </c>
+      <c r="C37" t="s">
         <v>287</v>
       </c>
-      <c r="B37" t="s">
-        <v>288</v>
-      </c>
-      <c r="C37" t="s">
-        <v>289</v>
-      </c>
       <c r="D37" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C38" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D38" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>293</v>
+      </c>
+      <c r="B39" t="s">
+        <v>286</v>
+      </c>
+      <c r="C39" t="s">
+        <v>294</v>
+      </c>
+      <c r="D39" t="s">
         <v>295</v>
-      </c>
-      <c r="B39" t="s">
-        <v>288</v>
-      </c>
-      <c r="C39" t="s">
-        <v>296</v>
-      </c>
-      <c r="D39" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>296</v>
+      </c>
+      <c r="B40" t="s">
+        <v>283</v>
+      </c>
+      <c r="C40" t="s">
+        <v>297</v>
+      </c>
+      <c r="D40" t="s">
         <v>298</v>
-      </c>
-      <c r="B40" t="s">
-        <v>285</v>
-      </c>
-      <c r="C40" t="s">
-        <v>299</v>
-      </c>
-      <c r="D40" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>300</v>
+      </c>
+      <c r="B41" t="s">
+        <v>283</v>
+      </c>
+      <c r="C41" t="s">
+        <v>301</v>
+      </c>
+      <c r="D41" t="s">
         <v>302</v>
-      </c>
-      <c r="B41" t="s">
-        <v>285</v>
-      </c>
-      <c r="C41" t="s">
-        <v>303</v>
-      </c>
-      <c r="D41" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>318</v>
+      </c>
+      <c r="B42" t="s">
+        <v>283</v>
+      </c>
+      <c r="C42" t="s">
+        <v>319</v>
+      </c>
+      <c r="D42" t="s">
         <v>320</v>
-      </c>
-      <c r="B42" t="s">
-        <v>285</v>
-      </c>
-      <c r="C42" t="s">
-        <v>321</v>
-      </c>
-      <c r="D42" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>303</v>
+      </c>
+      <c r="B43" t="s">
+        <v>284</v>
+      </c>
+      <c r="C43" t="s">
         <v>305</v>
       </c>
-      <c r="B43" t="s">
-        <v>286</v>
-      </c>
-      <c r="C43" t="s">
-        <v>307</v>
-      </c>
       <c r="D43" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="B44" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C44" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D44" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>309</v>
+      </c>
+      <c r="B45" t="s">
+        <v>284</v>
+      </c>
+      <c r="C45" t="s">
+        <v>310</v>
+      </c>
+      <c r="D45" t="s">
         <v>311</v>
-      </c>
-      <c r="B45" t="s">
-        <v>286</v>
-      </c>
-      <c r="C45" t="s">
-        <v>312</v>
-      </c>
-      <c r="D45" t="s">
-        <v>313</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>324</v>
+      </c>
+      <c r="B46" t="s">
+        <v>325</v>
+      </c>
+      <c r="C46" t="s">
         <v>326</v>
       </c>
-      <c r="B46" t="s">
+      <c r="D46" t="s">
         <v>327</v>
-      </c>
-      <c r="C46" t="s">
-        <v>328</v>
-      </c>
-      <c r="D46" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2824,16 +2818,16 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B48" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C48" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D48" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2841,7 +2835,7 @@
         <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C49" t="s">
         <v>79</v>
@@ -2852,77 +2846,77 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B50" t="s">
+        <v>218</v>
+      </c>
+      <c r="C50" t="s">
+        <v>219</v>
+      </c>
+      <c r="D50" t="s">
         <v>220</v>
-      </c>
-      <c r="C50" t="s">
-        <v>221</v>
-      </c>
-      <c r="D50" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="B51" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C51" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D51" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="B52" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C52" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D52" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>265</v>
+      </c>
+      <c r="B53" t="s">
+        <v>263</v>
+      </c>
+      <c r="C53" t="s">
+        <v>266</v>
+      </c>
+      <c r="D53" t="s">
         <v>267</v>
-      </c>
-      <c r="B53" t="s">
-        <v>265</v>
-      </c>
-      <c r="C53" t="s">
-        <v>268</v>
-      </c>
-      <c r="D53" t="s">
-        <v>269</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>268</v>
+      </c>
+      <c r="B54" t="s">
+        <v>263</v>
+      </c>
+      <c r="C54" t="s">
+        <v>269</v>
+      </c>
+      <c r="D54" t="s">
         <v>270</v>
-      </c>
-      <c r="B54" t="s">
-        <v>265</v>
-      </c>
-      <c r="C54" t="s">
-        <v>271</v>
-      </c>
-      <c r="D54" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
@@ -2944,7 +2938,7 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
@@ -2966,77 +2960,77 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B59" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C59" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D59" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B60" t="s">
+        <v>101</v>
+      </c>
+      <c r="C60" t="s">
         <v>103</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>105</v>
-      </c>
-      <c r="D60" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>102</v>
+      </c>
+      <c r="B61" t="s">
+        <v>101</v>
+      </c>
+      <c r="C61" t="s">
         <v>104</v>
       </c>
-      <c r="B61" t="s">
-        <v>103</v>
-      </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
         <v>106</v>
-      </c>
-      <c r="D61" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C62" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D62" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
+        <v>109</v>
+      </c>
+      <c r="B63" t="s">
+        <v>110</v>
+      </c>
+      <c r="C63" t="s">
         <v>111</v>
       </c>
-      <c r="B63" t="s">
+      <c r="D63" t="s">
         <v>112</v>
-      </c>
-      <c r="C63" t="s">
-        <v>113</v>
-      </c>
-      <c r="D63" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -3058,118 +3052,118 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="B66" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C66" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="D66" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B67" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C67" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D67" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B68" t="s">
+        <v>368</v>
+      </c>
+      <c r="C68" t="s">
+        <v>369</v>
+      </c>
+      <c r="D68" t="s">
         <v>370</v>
-      </c>
-      <c r="C68" t="s">
-        <v>371</v>
-      </c>
-      <c r="D68" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>375</v>
+      </c>
+      <c r="B69" t="s">
+        <v>368</v>
+      </c>
+      <c r="C69" t="s">
+        <v>376</v>
+      </c>
+      <c r="D69" t="s">
         <v>377</v>
-      </c>
-      <c r="B69" t="s">
-        <v>370</v>
-      </c>
-      <c r="C69" t="s">
-        <v>378</v>
-      </c>
-      <c r="D69" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>378</v>
+      </c>
+      <c r="C70" t="s">
         <v>380</v>
       </c>
-      <c r="C70" t="s">
-        <v>382</v>
-      </c>
       <c r="D70" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>381</v>
+      </c>
+      <c r="C71" t="s">
+        <v>382</v>
+      </c>
+      <c r="D71" t="s">
         <v>383</v>
-      </c>
-      <c r="C71" t="s">
-        <v>384</v>
-      </c>
-      <c r="D71" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>384</v>
+      </c>
+      <c r="C72" t="s">
         <v>386</v>
       </c>
-      <c r="C72" t="s">
-        <v>388</v>
-      </c>
       <c r="D72" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>387</v>
+      </c>
+      <c r="C74" t="s">
+        <v>388</v>
+      </c>
+      <c r="D74" t="s">
         <v>389</v>
-      </c>
-      <c r="C74" t="s">
-        <v>390</v>
-      </c>
-      <c r="D74" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>390</v>
+      </c>
+      <c r="C75" t="s">
+        <v>391</v>
+      </c>
+      <c r="D75" t="s">
         <v>392</v>
-      </c>
-      <c r="C75" t="s">
-        <v>393</v>
-      </c>
-      <c r="D75" t="s">
-        <v>394</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -3177,105 +3171,105 @@
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B77" t="s">
         <v>48</v>
       </c>
       <c r="C77" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D77" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B78" t="s">
+        <v>159</v>
+      </c>
+      <c r="C78" t="s">
+        <v>160</v>
+      </c>
+      <c r="D78" t="s">
         <v>161</v>
-      </c>
-      <c r="C78" t="s">
-        <v>162</v>
-      </c>
-      <c r="D78" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B79" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C79" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D79" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B80" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C80" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D80" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B81" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C81" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D81" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
+        <v>168</v>
+      </c>
+      <c r="B82" t="s">
         <v>170</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="9" t="s">
         <v>172</v>
       </c>
-      <c r="C82" s="9" t="s">
-        <v>174</v>
-      </c>
       <c r="D82" s="9" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
+        <v>169</v>
+      </c>
+      <c r="B83" t="s">
+        <v>166</v>
+      </c>
+      <c r="C83" t="s">
         <v>171</v>
       </c>
-      <c r="B83" t="s">
-        <v>168</v>
-      </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>173</v>
-      </c>
-      <c r="D83" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="8" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B84" s="8"/>
       <c r="C84" s="8"/>
@@ -3297,16 +3291,16 @@
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B86" t="s">
         <v>9</v>
       </c>
       <c r="C86" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D86" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -3334,119 +3328,119 @@
         <v>68</v>
       </c>
       <c r="D88" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="D89" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
       </c>
       <c r="C90" t="s">
+        <v>396</v>
+      </c>
+      <c r="D90" t="s">
         <v>398</v>
-      </c>
-      <c r="D90" t="s">
-        <v>400</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
       </c>
       <c r="C91" t="s">
+        <v>397</v>
+      </c>
+      <c r="D91" t="s">
         <v>399</v>
-      </c>
-      <c r="D91" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="D92" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D93" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D94" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D95" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B96" t="s">
         <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D96" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3465,13 +3459,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D98" t="s">
         <v>17</v>
@@ -3479,16 +3473,16 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D99" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3507,30 +3501,30 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D101" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D102" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3549,83 +3543,83 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D104" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D105" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D106" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D107" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D108" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>321</v>
+      </c>
+      <c r="C109" t="s">
+        <v>322</v>
+      </c>
+      <c r="D109" t="s">
         <v>323</v>
-      </c>
-      <c r="C109" t="s">
-        <v>324</v>
-      </c>
-      <c r="D109" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,142 +3652,142 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D112" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>209</v>
+      </c>
+      <c r="B113" t="s">
+        <v>210</v>
+      </c>
+      <c r="C113" t="s">
+        <v>209</v>
+      </c>
+      <c r="D113" t="s">
         <v>211</v>
-      </c>
-      <c r="B113" t="s">
-        <v>212</v>
-      </c>
-      <c r="C113" t="s">
-        <v>211</v>
-      </c>
-      <c r="D113" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B114" t="s">
         <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D114" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B115" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C115" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D115" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B116" t="s">
         <v>9</v>
       </c>
       <c r="C116" t="s">
+        <v>256</v>
+      </c>
+      <c r="D116" t="s">
         <v>258</v>
-      </c>
-      <c r="D116" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B117" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C117" t="s">
+        <v>257</v>
+      </c>
+      <c r="D117" t="s">
         <v>259</v>
-      </c>
-      <c r="D117" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
+        <v>244</v>
+      </c>
+      <c r="D118" t="s">
         <v>246</v>
-      </c>
-      <c r="D118" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
+        <v>243</v>
+      </c>
+      <c r="B119" t="s">
+        <v>210</v>
+      </c>
+      <c r="C119" t="s">
         <v>245</v>
       </c>
-      <c r="B119" t="s">
-        <v>212</v>
-      </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
         <v>247</v>
-      </c>
-      <c r="D119" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B120" t="s">
         <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D120" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B121" t="s">
         <v>9</v>
       </c>
       <c r="C121" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D121" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3812,7 +3806,7 @@
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B123" s="2"/>
       <c r="C123" s="2"/>
@@ -3820,119 +3814,119 @@
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B124" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C124" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D124" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B125" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C125" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D125" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B126" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C126" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D126" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
+        <v>137</v>
+      </c>
+      <c r="B127" t="s">
+        <v>130</v>
+      </c>
+      <c r="C127" t="s">
+        <v>138</v>
+      </c>
+      <c r="D127" t="s">
         <v>139</v>
-      </c>
-      <c r="B127" t="s">
-        <v>132</v>
-      </c>
-      <c r="C127" t="s">
-        <v>140</v>
-      </c>
-      <c r="D127" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
+        <v>134</v>
+      </c>
+      <c r="B128" t="s">
+        <v>130</v>
+      </c>
+      <c r="C128" t="s">
+        <v>135</v>
+      </c>
+      <c r="D128" t="s">
         <v>136</v>
-      </c>
-      <c r="B128" t="s">
-        <v>132</v>
-      </c>
-      <c r="C128" t="s">
-        <v>137</v>
-      </c>
-      <c r="D128" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B129" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C129" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D129" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B130" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C130" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D130" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
+        <v>145</v>
+      </c>
+      <c r="B131" t="s">
+        <v>130</v>
+      </c>
+      <c r="C131" t="s">
+        <v>146</v>
+      </c>
+      <c r="D131" t="s">
         <v>147</v>
-      </c>
-      <c r="B131" t="s">
-        <v>132</v>
-      </c>
-      <c r="C131" t="s">
-        <v>148</v>
-      </c>
-      <c r="D131" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -3946,52 +3940,52 @@
         <v>85</v>
       </c>
       <c r="C133" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D133" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="B134" t="s">
         <v>85</v>
       </c>
       <c r="C134" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D134" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B135" t="s">
         <v>85</v>
       </c>
       <c r="C135" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D135" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B136" t="s">
         <v>85</v>
       </c>
       <c r="C136" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D136" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
A bit closer to a functional map
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\OneDrive - Government of Yukon\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66655630-4FB9-4F76-B7F2-634940C19632}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2982CF-575C-4D14-B13E-AF7D009AD014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="406">
   <si>
     <t>id</t>
   </si>
@@ -1245,6 +1245,12 @@
   </si>
   <si>
     <t>media_type_fr</t>
+  </si>
+  <si>
+    <t>param_name</t>
+  </si>
+  <si>
+    <t>param_name_fr</t>
   </si>
 </sst>
 </file>
@@ -3940,10 +3946,10 @@
         <v>85</v>
       </c>
       <c r="C133" t="s">
-        <v>87</v>
+        <v>404</v>
       </c>
       <c r="D133" t="s">
-        <v>88</v>
+        <v>405</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
tweaks to map view
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\OneDrive - Government of Yukon\Documents\YGwater\inst\apps\streamLine\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2982CF-575C-4D14-B13E-AF7D009AD014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25A1940-1F43-45DD-9D2E-02C50B7162E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="410">
   <si>
     <t>id</t>
   </si>
@@ -581,9 +581,6 @@
     <t>group</t>
   </si>
   <si>
-    <t>group_fr</t>
-  </si>
-  <si>
     <t>param_group</t>
   </si>
   <si>
@@ -1251,6 +1248,21 @@
   </si>
   <si>
     <t>param_name_fr</t>
+  </si>
+  <si>
+    <t>group_name</t>
+  </si>
+  <si>
+    <t>group_name_fr</t>
+  </si>
+  <si>
+    <t>param_sub_group_col</t>
+  </si>
+  <si>
+    <t>sub_group_name</t>
+  </si>
+  <si>
+    <t>sub_group_name_fr</t>
   </si>
 </sst>
 </file>
@@ -2185,10 +2197,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D136"/>
+  <dimension ref="A1:D137"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="D133" sqref="D133"/>
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2350,7 +2362,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2358,142 +2370,142 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B13" t="s">
+        <v>329</v>
+      </c>
+      <c r="C13" t="s">
         <v>330</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>331</v>
-      </c>
-      <c r="D13" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B14" t="s">
+        <v>334</v>
+      </c>
+      <c r="C14" t="s">
         <v>335</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>336</v>
-      </c>
-      <c r="D14" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B15" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C15" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D15" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B16" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C16" t="s">
+        <v>349</v>
+      </c>
+      <c r="D16" t="s">
         <v>350</v>
-      </c>
-      <c r="D16" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B17" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C17" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D17" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B18" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C18" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D18" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B19" t="s">
+        <v>347</v>
+      </c>
+      <c r="C19" t="s">
+        <v>343</v>
+      </c>
+      <c r="D19" t="s">
         <v>348</v>
-      </c>
-      <c r="C19" t="s">
-        <v>344</v>
-      </c>
-      <c r="D19" t="s">
-        <v>349</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>358</v>
+      </c>
+      <c r="B20" t="s">
+        <v>347</v>
+      </c>
+      <c r="C20" t="s">
         <v>359</v>
       </c>
-      <c r="B20" t="s">
-        <v>348</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>360</v>
-      </c>
-      <c r="D20" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>361</v>
+      </c>
+      <c r="B21" t="s">
+        <v>355</v>
+      </c>
+      <c r="C21" t="s">
         <v>362</v>
       </c>
-      <c r="B21" t="s">
-        <v>356</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>363</v>
-      </c>
-      <c r="D21" t="s">
-        <v>364</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>354</v>
+      </c>
+      <c r="B22" t="s">
         <v>355</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>356</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>357</v>
-      </c>
-      <c r="D22" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -2578,16 +2590,16 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B30" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C30" t="s">
+        <v>271</v>
+      </c>
+      <c r="D30" t="s">
         <v>272</v>
-      </c>
-      <c r="D30" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -2595,7 +2607,7 @@
         <v>89</v>
       </c>
       <c r="B31" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C31" t="s">
         <v>90</v>
@@ -2606,217 +2618,217 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>273</v>
+      </c>
+      <c r="B32" t="s">
+        <v>276</v>
+      </c>
+      <c r="C32" t="s">
         <v>274</v>
       </c>
-      <c r="B32" t="s">
-        <v>277</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>275</v>
-      </c>
-      <c r="D32" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>280</v>
+      </c>
+      <c r="B33" t="s">
+        <v>282</v>
+      </c>
+      <c r="C33" t="s">
         <v>281</v>
       </c>
-      <c r="B33" t="s">
-        <v>283</v>
-      </c>
-      <c r="C33" t="s">
-        <v>282</v>
-      </c>
       <c r="D33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B34" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C34" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D34" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B35" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C35" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D35" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B36" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C36" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D36" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>284</v>
+      </c>
+      <c r="B37" t="s">
         <v>285</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>286</v>
       </c>
-      <c r="C37" t="s">
-        <v>287</v>
-      </c>
       <c r="D37" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B38" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C38" t="s">
+        <v>290</v>
+      </c>
+      <c r="D38" t="s">
         <v>291</v>
-      </c>
-      <c r="D38" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>292</v>
+      </c>
+      <c r="B39" t="s">
+        <v>285</v>
+      </c>
+      <c r="C39" t="s">
         <v>293</v>
       </c>
-      <c r="B39" t="s">
-        <v>286</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>294</v>
-      </c>
-      <c r="D39" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>295</v>
+      </c>
+      <c r="B40" t="s">
+        <v>282</v>
+      </c>
+      <c r="C40" t="s">
         <v>296</v>
       </c>
-      <c r="B40" t="s">
-        <v>283</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="D40" t="s">
         <v>297</v>
-      </c>
-      <c r="D40" t="s">
-        <v>298</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>299</v>
+      </c>
+      <c r="B41" t="s">
+        <v>282</v>
+      </c>
+      <c r="C41" t="s">
         <v>300</v>
       </c>
-      <c r="B41" t="s">
-        <v>283</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="D41" t="s">
         <v>301</v>
-      </c>
-      <c r="D41" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>317</v>
+      </c>
+      <c r="B42" t="s">
+        <v>282</v>
+      </c>
+      <c r="C42" t="s">
         <v>318</v>
       </c>
-      <c r="B42" t="s">
-        <v>283</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D42" t="s">
         <v>319</v>
-      </c>
-      <c r="D42" t="s">
-        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B43" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C43" t="s">
+        <v>304</v>
+      </c>
+      <c r="D43" t="s">
         <v>305</v>
-      </c>
-      <c r="D43" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B44" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C44" t="s">
+        <v>306</v>
+      </c>
+      <c r="D44" t="s">
         <v>307</v>
-      </c>
-      <c r="D44" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>308</v>
+      </c>
+      <c r="B45" t="s">
+        <v>283</v>
+      </c>
+      <c r="C45" t="s">
         <v>309</v>
       </c>
-      <c r="B45" t="s">
-        <v>284</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>310</v>
-      </c>
-      <c r="D45" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>323</v>
+      </c>
+      <c r="B46" t="s">
         <v>324</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>325</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>326</v>
-      </c>
-      <c r="D46" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="10" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2824,10 +2836,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>213</v>
+      </c>
+      <c r="B48" t="s">
         <v>214</v>
-      </c>
-      <c r="B48" t="s">
-        <v>215</v>
       </c>
       <c r="C48" t="s">
         <v>96</v>
@@ -2841,7 +2853,7 @@
         <v>78</v>
       </c>
       <c r="B49" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C49" t="s">
         <v>79</v>
@@ -2852,72 +2864,72 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B50" t="s">
+        <v>217</v>
+      </c>
+      <c r="C50" t="s">
         <v>218</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>219</v>
-      </c>
-      <c r="D50" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>249</v>
+      </c>
+      <c r="B51" t="s">
         <v>250</v>
       </c>
-      <c r="B51" t="s">
-        <v>251</v>
-      </c>
       <c r="C51" t="s">
+        <v>253</v>
+      </c>
+      <c r="D51" t="s">
         <v>254</v>
-      </c>
-      <c r="D51" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B52" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D52" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>264</v>
+      </c>
+      <c r="B53" t="s">
+        <v>262</v>
+      </c>
+      <c r="C53" t="s">
         <v>265</v>
       </c>
-      <c r="B53" t="s">
-        <v>263</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="D53" t="s">
         <v>266</v>
-      </c>
-      <c r="D53" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>267</v>
+      </c>
+      <c r="B54" t="s">
+        <v>262</v>
+      </c>
+      <c r="C54" t="s">
         <v>268</v>
       </c>
-      <c r="B54" t="s">
-        <v>263</v>
-      </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>269</v>
-      </c>
-      <c r="D54" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -3017,7 +3029,7 @@
         <v>125</v>
       </c>
       <c r="D62" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -3036,7 +3048,7 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B64" s="7"/>
       <c r="C64" s="7"/>
@@ -3058,113 +3070,113 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B66" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C66" t="s">
+        <v>370</v>
+      </c>
+      <c r="D66" t="s">
         <v>371</v>
-      </c>
-      <c r="D66" t="s">
-        <v>372</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B67" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C67" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D67" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B68" t="s">
+        <v>367</v>
+      </c>
+      <c r="C68" t="s">
         <v>368</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>369</v>
-      </c>
-      <c r="D68" t="s">
-        <v>370</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
+        <v>374</v>
+      </c>
+      <c r="B69" t="s">
+        <v>367</v>
+      </c>
+      <c r="C69" t="s">
         <v>375</v>
       </c>
-      <c r="B69" t="s">
-        <v>368</v>
-      </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
         <v>376</v>
-      </c>
-      <c r="D69" t="s">
-        <v>377</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
+        <v>377</v>
+      </c>
+      <c r="C70" t="s">
+        <v>379</v>
+      </c>
+      <c r="D70" t="s">
         <v>378</v>
-      </c>
-      <c r="C70" t="s">
-        <v>380</v>
-      </c>
-      <c r="D70" t="s">
-        <v>379</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
+        <v>380</v>
+      </c>
+      <c r="C71" t="s">
         <v>381</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
         <v>382</v>
-      </c>
-      <c r="D71" t="s">
-        <v>383</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
+        <v>383</v>
+      </c>
+      <c r="C72" t="s">
+        <v>385</v>
+      </c>
+      <c r="D72" t="s">
         <v>384</v>
-      </c>
-      <c r="C72" t="s">
-        <v>386</v>
-      </c>
-      <c r="D72" t="s">
-        <v>385</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
+        <v>386</v>
+      </c>
+      <c r="C74" t="s">
         <v>387</v>
       </c>
-      <c r="C74" t="s">
+      <c r="D74" t="s">
         <v>388</v>
-      </c>
-      <c r="D74" t="s">
-        <v>389</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
+        <v>389</v>
+      </c>
+      <c r="C75" t="s">
         <v>390</v>
       </c>
-      <c r="C75" t="s">
+      <c r="D75" t="s">
         <v>391</v>
-      </c>
-      <c r="D75" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -3334,105 +3346,105 @@
         <v>68</v>
       </c>
       <c r="D88" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D89" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D90" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D91" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
       </c>
       <c r="C92" t="s">
+        <v>399</v>
+      </c>
+      <c r="D92" t="s">
         <v>400</v>
-      </c>
-      <c r="D92" t="s">
-        <v>401</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
       <c r="C93" t="s">
+        <v>183</v>
+      </c>
+      <c r="D93" t="s">
         <v>184</v>
-      </c>
-      <c r="D93" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
       </c>
       <c r="C94" t="s">
+        <v>194</v>
+      </c>
+      <c r="D94" t="s">
         <v>195</v>
-      </c>
-      <c r="D94" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
       <c r="C95" t="s">
+        <v>203</v>
+      </c>
+      <c r="D95" t="s">
         <v>204</v>
-      </c>
-      <c r="D95" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -3443,10 +3455,10 @@
         <v>9</v>
       </c>
       <c r="C96" t="s">
+        <v>220</v>
+      </c>
+      <c r="D96" t="s">
         <v>221</v>
-      </c>
-      <c r="D96" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -3465,13 +3477,13 @@
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D98" t="s">
         <v>17</v>
@@ -3479,16 +3491,16 @@
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
       </c>
       <c r="C99" t="s">
+        <v>197</v>
+      </c>
+      <c r="D99" t="s">
         <v>198</v>
-      </c>
-      <c r="D99" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -3507,30 +3519,30 @@
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="C101" t="s">
+        <v>191</v>
+      </c>
+      <c r="D101" t="s">
         <v>192</v>
-      </c>
-      <c r="D101" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
       </c>
       <c r="C102" t="s">
+        <v>200</v>
+      </c>
+      <c r="D102" t="s">
         <v>201</v>
-      </c>
-      <c r="D102" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -3549,55 +3561,55 @@
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
       </c>
       <c r="C104" t="s">
+        <v>186</v>
+      </c>
+      <c r="D104" t="s">
         <v>187</v>
-      </c>
-      <c r="D104" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
       <c r="C105" t="s">
+        <v>206</v>
+      </c>
+      <c r="D105" t="s">
         <v>207</v>
-      </c>
-      <c r="D105" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
       </c>
       <c r="C106" t="s">
+        <v>222</v>
+      </c>
+      <c r="D106" t="s">
         <v>223</v>
-      </c>
-      <c r="D106" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D107" t="s">
         <v>126</v>
@@ -3605,27 +3617,27 @@
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
       <c r="C108" t="s">
+        <v>228</v>
+      </c>
+      <c r="D108" t="s">
         <v>229</v>
-      </c>
-      <c r="D108" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
+        <v>320</v>
+      </c>
+      <c r="C109" t="s">
         <v>321</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>322</v>
-      </c>
-      <c r="D109" t="s">
-        <v>323</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
@@ -3658,114 +3670,114 @@
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
       </c>
       <c r="C112" t="s">
+        <v>230</v>
+      </c>
+      <c r="D112" t="s">
         <v>231</v>
-      </c>
-      <c r="D112" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
+        <v>208</v>
+      </c>
+      <c r="B113" t="s">
         <v>209</v>
       </c>
-      <c r="B113" t="s">
+      <c r="C113" t="s">
+        <v>208</v>
+      </c>
+      <c r="D113" t="s">
         <v>210</v>
-      </c>
-      <c r="C113" t="s">
-        <v>209</v>
-      </c>
-      <c r="D113" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B114" t="s">
         <v>9</v>
       </c>
       <c r="C114" t="s">
+        <v>234</v>
+      </c>
+      <c r="D114" t="s">
         <v>235</v>
-      </c>
-      <c r="D114" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B115" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C115" t="s">
+        <v>236</v>
+      </c>
+      <c r="D115" t="s">
         <v>237</v>
-      </c>
-      <c r="D115" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B116" t="s">
         <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D116" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B117" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C117" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D117" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D118" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B119" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C119" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D119" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
@@ -3784,16 +3796,16 @@
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B121" t="s">
         <v>9</v>
       </c>
       <c r="C121" t="s">
+        <v>239</v>
+      </c>
+      <c r="D121" t="s">
         <v>240</v>
-      </c>
-      <c r="D121" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
@@ -3946,24 +3958,24 @@
         <v>85</v>
       </c>
       <c r="C133" t="s">
+        <v>403</v>
+      </c>
+      <c r="D133" t="s">
         <v>404</v>
-      </c>
-      <c r="D133" t="s">
-        <v>405</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B134" t="s">
         <v>85</v>
       </c>
       <c r="C134" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D134" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
@@ -3974,23 +3986,37 @@
         <v>85</v>
       </c>
       <c r="C135" t="s">
-        <v>181</v>
+        <v>405</v>
       </c>
       <c r="D135" t="s">
-        <v>182</v>
+        <v>406</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>86</v>
+        <v>407</v>
       </c>
       <c r="B136" t="s">
         <v>85</v>
       </c>
       <c r="C136" t="s">
+        <v>408</v>
+      </c>
+      <c r="D136" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>86</v>
+      </c>
+      <c r="B137" t="s">
+        <v>85</v>
+      </c>
+      <c r="C137" t="s">
         <v>87</v>
       </c>
-      <c r="D136" t="s">
+      <c r="D137" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add new map for parameter visualization
</commit_message>
<xml_diff>
--- a/inst/apps/streamLine/translations.xlsx
+++ b/inst/apps/streamLine/translations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtdelapl\Documents\YGwater\inst\apps\streamLine\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25A1940-1F43-45DD-9D2E-02C50B7162E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4EF92C5-AD99-4F86-9106-B083ACFB5DFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="426">
   <si>
     <t>id</t>
   </si>
@@ -1196,18 +1196,9 @@
     <t>map_absolute</t>
   </si>
   <si>
-    <t>Absolute values</t>
-  </si>
-  <si>
-    <t>Valeures absolues</t>
-  </si>
-  <si>
     <t>map_relative</t>
   </si>
   <si>
-    <t>% historical range</t>
-  </si>
-  <si>
     <t>% plage historique</t>
   </si>
   <si>
@@ -1263,6 +1254,63 @@
   </si>
   <si>
     <t>sub_group_name_fr</t>
+  </si>
+  <si>
+    <t>map_min_yrs</t>
+  </si>
+  <si>
+    <t>minimum number of years to use historic range stats</t>
+  </si>
+  <si>
+    <t>With at least … years of record</t>
+  </si>
+  <si>
+    <t>Avec au moins … années de mesures</t>
+  </si>
+  <si>
+    <t>map_target_date</t>
+  </si>
+  <si>
+    <t>target date for historical range map</t>
+  </si>
+  <si>
+    <t>Target date</t>
+  </si>
+  <si>
+    <t>Date ciblée</t>
+  </si>
+  <si>
+    <t>Absolute value</t>
+  </si>
+  <si>
+    <t>Valeure absolue</t>
+  </si>
+  <si>
+    <t>map_actual_date</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>map_actual_yrs</t>
+  </si>
+  <si>
+    <t>Years of record</t>
+  </si>
+  <si>
+    <t>Années de mesures</t>
+  </si>
+  <si>
+    <t>map_actual_hist_range</t>
+  </si>
+  <si>
+    <t>Historic range</t>
+  </si>
+  <si>
+    <t>Plage historique</t>
+  </si>
+  <si>
+    <t>% historic range</t>
   </si>
 </sst>
 </file>
@@ -2197,10 +2245,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D137"/>
+  <dimension ref="A1:D141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A118" workbookViewId="0">
-      <selection activeCell="A135" sqref="A135"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3157,866 +3205,927 @@
         <v>384</v>
       </c>
     </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>407</v>
+      </c>
+      <c r="B73" t="s">
+        <v>408</v>
+      </c>
+      <c r="C73" t="s">
+        <v>409</v>
+      </c>
+      <c r="D73" t="s">
+        <v>410</v>
+      </c>
+    </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>386</v>
+        <v>411</v>
+      </c>
+      <c r="B74" t="s">
+        <v>412</v>
       </c>
       <c r="C74" t="s">
-        <v>387</v>
+        <v>413</v>
       </c>
       <c r="D74" t="s">
-        <v>388</v>
+        <v>414</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C75" t="s">
-        <v>390</v>
+        <v>415</v>
       </c>
       <c r="D75" t="s">
-        <v>391</v>
+        <v>416</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
+      <c r="A76" t="s">
+        <v>387</v>
+      </c>
+      <c r="C76" t="s">
+        <v>425</v>
+      </c>
+      <c r="D76" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>156</v>
-      </c>
-      <c r="B77" t="s">
-        <v>48</v>
+        <v>417</v>
       </c>
       <c r="C77" t="s">
-        <v>157</v>
+        <v>418</v>
       </c>
       <c r="D77" t="s">
-        <v>158</v>
+        <v>418</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>162</v>
-      </c>
-      <c r="B78" t="s">
-        <v>159</v>
+        <v>419</v>
       </c>
       <c r="C78" t="s">
-        <v>160</v>
+        <v>420</v>
       </c>
       <c r="D78" t="s">
-        <v>161</v>
+        <v>421</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>165</v>
-      </c>
-      <c r="B79" t="s">
-        <v>166</v>
+        <v>422</v>
       </c>
       <c r="C79" t="s">
-        <v>177</v>
+        <v>423</v>
       </c>
       <c r="D79" t="s">
-        <v>178</v>
+        <v>424</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>174</v>
-      </c>
-      <c r="B80" t="s">
-        <v>159</v>
-      </c>
-      <c r="C80" t="s">
-        <v>163</v>
-      </c>
-      <c r="D80" t="s">
-        <v>164</v>
-      </c>
+      <c r="A80" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="B80" s="4"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="B81" t="s">
-        <v>166</v>
+        <v>48</v>
       </c>
       <c r="C81" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="D81" t="s">
-        <v>175</v>
+        <v>158</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="B82" t="s">
-        <v>170</v>
-      </c>
-      <c r="C82" s="9" t="s">
-        <v>172</v>
-      </c>
-      <c r="D82" s="9" t="s">
-        <v>172</v>
+        <v>159</v>
+      </c>
+      <c r="C82" t="s">
+        <v>160</v>
+      </c>
+      <c r="D82" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="B83" t="s">
         <v>166</v>
       </c>
       <c r="C83" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D83" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B84" s="8"/>
-      <c r="C84" s="8"/>
-      <c r="D84" s="8"/>
+      <c r="A84" t="s">
+        <v>174</v>
+      </c>
+      <c r="B84" t="s">
+        <v>159</v>
+      </c>
+      <c r="C84" t="s">
+        <v>163</v>
+      </c>
+      <c r="D84" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>61</v>
+        <v>167</v>
       </c>
       <c r="B85" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="C85" t="s">
-        <v>62</v>
+        <v>176</v>
       </c>
       <c r="D85" t="s">
-        <v>63</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>113</v>
+        <v>168</v>
       </c>
       <c r="B86" t="s">
-        <v>9</v>
-      </c>
-      <c r="C86" t="s">
-        <v>114</v>
-      </c>
-      <c r="D86" t="s">
-        <v>115</v>
+        <v>170</v>
+      </c>
+      <c r="C86" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="D86" s="9" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>64</v>
+        <v>169</v>
       </c>
       <c r="B87" t="s">
-        <v>9</v>
+        <v>166</v>
       </c>
       <c r="C87" t="s">
-        <v>65</v>
+        <v>171</v>
       </c>
       <c r="D87" t="s">
-        <v>66</v>
+        <v>173</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>67</v>
-      </c>
-      <c r="B88" t="s">
-        <v>9</v>
-      </c>
-      <c r="C88" t="s">
-        <v>68</v>
-      </c>
-      <c r="D88" t="s">
-        <v>252</v>
-      </c>
+      <c r="A88" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="8"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>247</v>
+        <v>61</v>
       </c>
       <c r="B89" t="s">
         <v>9</v>
       </c>
       <c r="C89" t="s">
-        <v>248</v>
+        <v>62</v>
       </c>
       <c r="D89" t="s">
-        <v>248</v>
+        <v>63</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>392</v>
+        <v>113</v>
       </c>
       <c r="B90" t="s">
         <v>9</v>
       </c>
       <c r="C90" t="s">
-        <v>395</v>
+        <v>114</v>
       </c>
       <c r="D90" t="s">
-        <v>397</v>
+        <v>115</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>393</v>
+        <v>64</v>
       </c>
       <c r="B91" t="s">
         <v>9</v>
       </c>
       <c r="C91" t="s">
-        <v>396</v>
+        <v>65</v>
       </c>
       <c r="D91" t="s">
-        <v>398</v>
+        <v>66</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>394</v>
+        <v>67</v>
       </c>
       <c r="B92" t="s">
         <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>399</v>
+        <v>68</v>
       </c>
       <c r="D92" t="s">
-        <v>400</v>
+        <v>252</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>182</v>
+        <v>247</v>
       </c>
       <c r="B93" t="s">
         <v>9</v>
       </c>
       <c r="C93" t="s">
-        <v>183</v>
+        <v>248</v>
       </c>
       <c r="D93" t="s">
-        <v>184</v>
+        <v>248</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>193</v>
+        <v>389</v>
       </c>
       <c r="B94" t="s">
         <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>194</v>
+        <v>392</v>
       </c>
       <c r="D94" t="s">
-        <v>195</v>
+        <v>394</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>202</v>
+        <v>390</v>
       </c>
       <c r="B95" t="s">
         <v>9</v>
       </c>
       <c r="C95" t="s">
-        <v>203</v>
+        <v>393</v>
       </c>
       <c r="D95" t="s">
-        <v>204</v>
+        <v>395</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>181</v>
+        <v>391</v>
       </c>
       <c r="B96" t="s">
         <v>9</v>
       </c>
       <c r="C96" t="s">
-        <v>220</v>
+        <v>396</v>
       </c>
       <c r="D96" t="s">
-        <v>221</v>
+        <v>397</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>69</v>
+        <v>182</v>
       </c>
       <c r="B97" t="s">
         <v>9</v>
       </c>
       <c r="C97" t="s">
-        <v>70</v>
+        <v>183</v>
       </c>
       <c r="D97" t="s">
-        <v>71</v>
+        <v>184</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="B98" t="s">
         <v>9</v>
       </c>
       <c r="C98" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D98" t="s">
-        <v>17</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="B99" t="s">
         <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D99" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>72</v>
+        <v>181</v>
       </c>
       <c r="B100" t="s">
         <v>9</v>
       </c>
       <c r="C100" t="s">
-        <v>73</v>
+        <v>220</v>
       </c>
       <c r="D100" t="s">
-        <v>74</v>
+        <v>221</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>189</v>
+        <v>69</v>
       </c>
       <c r="B101" t="s">
         <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>191</v>
+        <v>70</v>
       </c>
       <c r="D101" t="s">
-        <v>192</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B102" t="s">
         <v>9</v>
       </c>
       <c r="C102" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="D102" t="s">
-        <v>201</v>
+        <v>17</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>75</v>
+        <v>196</v>
       </c>
       <c r="B103" t="s">
         <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>76</v>
+        <v>197</v>
       </c>
       <c r="D103" t="s">
-        <v>77</v>
+        <v>198</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>188</v>
+        <v>72</v>
       </c>
       <c r="B104" t="s">
         <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>186</v>
+        <v>73</v>
       </c>
       <c r="D104" t="s">
-        <v>187</v>
+        <v>74</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="B105" t="s">
         <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="D105" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>224</v>
+        <v>199</v>
       </c>
       <c r="B106" t="s">
         <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>222</v>
+        <v>200</v>
       </c>
       <c r="D106" t="s">
-        <v>223</v>
+        <v>201</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>225</v>
+        <v>75</v>
       </c>
       <c r="B107" t="s">
         <v>9</v>
       </c>
       <c r="C107" t="s">
-        <v>226</v>
+        <v>76</v>
       </c>
       <c r="D107" t="s">
-        <v>126</v>
+        <v>77</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>227</v>
+        <v>188</v>
       </c>
       <c r="B108" t="s">
         <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>228</v>
+        <v>186</v>
       </c>
       <c r="D108" t="s">
-        <v>229</v>
+        <v>187</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>320</v>
+        <v>205</v>
+      </c>
+      <c r="B109" t="s">
+        <v>9</v>
       </c>
       <c r="C109" t="s">
-        <v>321</v>
+        <v>206</v>
       </c>
       <c r="D109" t="s">
-        <v>322</v>
+        <v>207</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>81</v>
+        <v>224</v>
       </c>
       <c r="B110" t="s">
         <v>9</v>
       </c>
       <c r="C110" t="s">
-        <v>82</v>
+        <v>222</v>
       </c>
       <c r="D110" t="s">
-        <v>83</v>
+        <v>223</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>8</v>
+        <v>225</v>
       </c>
       <c r="B111" t="s">
         <v>9</v>
       </c>
       <c r="C111" t="s">
-        <v>10</v>
+        <v>226</v>
       </c>
       <c r="D111" t="s">
-        <v>11</v>
+        <v>126</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B112" t="s">
         <v>9</v>
       </c>
       <c r="C112" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D112" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>208</v>
-      </c>
-      <c r="B113" t="s">
-        <v>209</v>
+        <v>320</v>
       </c>
       <c r="C113" t="s">
-        <v>208</v>
+        <v>321</v>
       </c>
       <c r="D113" t="s">
-        <v>210</v>
+        <v>322</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>232</v>
+        <v>81</v>
       </c>
       <c r="B114" t="s">
         <v>9</v>
       </c>
       <c r="C114" t="s">
-        <v>234</v>
+        <v>82</v>
       </c>
       <c r="D114" t="s">
-        <v>235</v>
+        <v>83</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>233</v>
+        <v>8</v>
       </c>
       <c r="B115" t="s">
-        <v>209</v>
+        <v>9</v>
       </c>
       <c r="C115" t="s">
-        <v>236</v>
+        <v>10</v>
       </c>
       <c r="D115" t="s">
-        <v>237</v>
+        <v>11</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="B116" t="s">
         <v>9</v>
       </c>
       <c r="C116" t="s">
-        <v>255</v>
+        <v>230</v>
       </c>
       <c r="D116" t="s">
-        <v>257</v>
+        <v>231</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>260</v>
+        <v>208</v>
       </c>
       <c r="B117" t="s">
         <v>209</v>
       </c>
       <c r="C117" t="s">
-        <v>256</v>
+        <v>208</v>
       </c>
       <c r="D117" t="s">
-        <v>258</v>
+        <v>210</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="B118" t="s">
         <v>9</v>
       </c>
       <c r="C118" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="D118" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="B119" t="s">
         <v>209</v>
       </c>
       <c r="C119" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D119" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>127</v>
+        <v>259</v>
       </c>
       <c r="B120" t="s">
         <v>9</v>
       </c>
       <c r="C120" t="s">
-        <v>128</v>
+        <v>255</v>
       </c>
       <c r="D120" t="s">
-        <v>129</v>
+        <v>257</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>238</v>
+        <v>260</v>
       </c>
       <c r="B121" t="s">
-        <v>9</v>
+        <v>209</v>
       </c>
       <c r="C121" t="s">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="D121" t="s">
-        <v>240</v>
+        <v>258</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>15</v>
+        <v>241</v>
       </c>
       <c r="B122" t="s">
         <v>9</v>
       </c>
       <c r="C122" t="s">
-        <v>16</v>
+        <v>243</v>
       </c>
       <c r="D122" t="s">
-        <v>17</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-      <c r="D123" s="2"/>
+      <c r="A123" t="s">
+        <v>242</v>
+      </c>
+      <c r="B123" t="s">
+        <v>209</v>
+      </c>
+      <c r="C123" t="s">
+        <v>244</v>
+      </c>
+      <c r="D123" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B124" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="C124" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D124" t="s">
-        <v>149</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>148</v>
+        <v>238</v>
       </c>
       <c r="B125" t="s">
-        <v>130</v>
+        <v>9</v>
       </c>
       <c r="C125" t="s">
-        <v>151</v>
+        <v>239</v>
       </c>
       <c r="D125" t="s">
-        <v>154</v>
+        <v>240</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>132</v>
+        <v>15</v>
       </c>
       <c r="B126" t="s">
+        <v>9</v>
+      </c>
+      <c r="C126" t="s">
+        <v>16</v>
+      </c>
+      <c r="D126" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C126" t="s">
-        <v>133</v>
-      </c>
-      <c r="D126" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>137</v>
-      </c>
-      <c r="B127" t="s">
-        <v>130</v>
-      </c>
-      <c r="C127" t="s">
-        <v>138</v>
-      </c>
-      <c r="D127" t="s">
-        <v>139</v>
-      </c>
+      <c r="B127" s="2"/>
+      <c r="C127" s="2"/>
+      <c r="D127" s="2"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B128" t="s">
         <v>130</v>
       </c>
       <c r="C128" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="D128" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B129" t="s">
         <v>130</v>
       </c>
       <c r="C129" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="D129" t="s">
-        <v>142</v>
+        <v>154</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
       <c r="B130" t="s">
         <v>130</v>
       </c>
       <c r="C130" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="D130" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B131" t="s">
         <v>130</v>
       </c>
       <c r="C131" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D131" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B132" s="4"/>
-      <c r="C132" s="4"/>
-      <c r="D132" s="4"/>
+      <c r="A132" t="s">
+        <v>134</v>
+      </c>
+      <c r="B132" t="s">
+        <v>130</v>
+      </c>
+      <c r="C132" t="s">
+        <v>135</v>
+      </c>
+      <c r="D132" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>84</v>
+        <v>141</v>
       </c>
       <c r="B133" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="C133" t="s">
-        <v>403</v>
+        <v>153</v>
       </c>
       <c r="D133" t="s">
-        <v>404</v>
+        <v>142</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>401</v>
+        <v>143</v>
       </c>
       <c r="B134" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="C134" t="s">
-        <v>392</v>
+        <v>152</v>
       </c>
       <c r="D134" t="s">
-        <v>402</v>
+        <v>144</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="B135" t="s">
-        <v>85</v>
+        <v>130</v>
       </c>
       <c r="C135" t="s">
-        <v>405</v>
+        <v>146</v>
       </c>
       <c r="D135" t="s">
-        <v>406</v>
+        <v>147</v>
       </c>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>407</v>
-      </c>
-      <c r="B136" t="s">
-        <v>85</v>
-      </c>
-      <c r="C136" t="s">
-        <v>408</v>
-      </c>
-      <c r="D136" t="s">
-        <v>409</v>
-      </c>
+      <c r="A136" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B136" s="4"/>
+      <c r="C136" s="4"/>
+      <c r="D136" s="4"/>
     </row>
     <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B137" t="s">
         <v>85</v>
       </c>
       <c r="C137" t="s">
+        <v>400</v>
+      </c>
+      <c r="D137" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A138" t="s">
+        <v>398</v>
+      </c>
+      <c r="B138" t="s">
+        <v>85</v>
+      </c>
+      <c r="C138" t="s">
+        <v>389</v>
+      </c>
+      <c r="D138" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>180</v>
+      </c>
+      <c r="B139" t="s">
+        <v>85</v>
+      </c>
+      <c r="C139" t="s">
+        <v>402</v>
+      </c>
+      <c r="D139" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A140" t="s">
+        <v>404</v>
+      </c>
+      <c r="B140" t="s">
+        <v>85</v>
+      </c>
+      <c r="C140" t="s">
+        <v>405</v>
+      </c>
+      <c r="D140" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>86</v>
+      </c>
+      <c r="B141" t="s">
+        <v>85</v>
+      </c>
+      <c r="C141" t="s">
         <v>87</v>
       </c>
-      <c r="D137" t="s">
+      <c r="D141" t="s">
         <v>88</v>
       </c>
     </row>

</xml_diff>